<commit_message>
Add location filter for job scrapping
</commit_message>
<xml_diff>
--- a/clients.example.xlsx
+++ b/clients.example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\projects\shiva\dbot-11\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{730D0C36-0DA6-45E3-BE9B-5466FA75D5FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A842A013-AAD4-4CB5-B779-58C1D90765B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3948,7 +3948,7 @@
   </sheetPr>
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add new about 20 urls
</commit_message>
<xml_diff>
--- a/clients.example.xlsx
+++ b/clients.example.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1647" uniqueCount="1096">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1698" uniqueCount="1128">
   <si>
     <t>ID</t>
   </si>
@@ -3286,6 +3286,102 @@
   </si>
   <si>
     <t>https://www.vitabiotics.com/pages/careers</t>
+  </si>
+  <si>
+    <t>acai outdoor</t>
+  </si>
+  <si>
+    <t>https://acaioutdoorwear.com/pages/careers?srsltid=AfmBOoqnOobmUDr6S8GiBsDp-PDhvxfbWJgkukM8PWSnqPoEmQJihHcF</t>
+  </si>
+  <si>
+    <t>acorn intelligence</t>
+  </si>
+  <si>
+    <t>https://acorn-i.com/join-our-team/</t>
+  </si>
+  <si>
+    <t>baxi partnership</t>
+  </si>
+  <si>
+    <t>https://bdrthermea.wd103.myworkdayjobs.com/External?locationCountry=29247e57dbaf46fb855b224e03170bc7</t>
+  </si>
+  <si>
+    <t>bitrise</t>
+  </si>
+  <si>
+    <t>https://bitrise.io/careers</t>
+  </si>
+  <si>
+    <t>blacklane</t>
+  </si>
+  <si>
+    <t>https://boards.greenhouse.io/blacklane</t>
+  </si>
+  <si>
+    <t>bgf</t>
+  </si>
+  <si>
+    <t>https://careers.bgf.co.uk/#jobs</t>
+  </si>
+  <si>
+    <t>care fertility</t>
+  </si>
+  <si>
+    <t>https://careers.carefertility.com/CareFertility/Home</t>
+  </si>
+  <si>
+    <t>chambers &amp; partners</t>
+  </si>
+  <si>
+    <t>ci&amp;t</t>
+  </si>
+  <si>
+    <t>https://ciandt.com/us/en-us/careers/open-positions</t>
+  </si>
+  <si>
+    <t>countingup</t>
+  </si>
+  <si>
+    <t>https://countingup.com/careers/</t>
+  </si>
+  <si>
+    <t>bevan brittan llp</t>
+  </si>
+  <si>
+    <t>https://fsr.cvmailuk.com/bevanbrittan/main.cfm?srxksl=1</t>
+  </si>
+  <si>
+    <t>arthur j gallagher</t>
+  </si>
+  <si>
+    <t>https://jobs.ajg.com/ajg-uk/jobs</t>
+  </si>
+  <si>
+    <t>klowt</t>
+  </si>
+  <si>
+    <t>https://klowt.com/join-klowt/#vacancies</t>
+  </si>
+  <si>
+    <t>alpha pet ventures</t>
+  </si>
+  <si>
+    <t>https://www.alpha.pet/en/career/jobs-and-application</t>
+  </si>
+  <si>
+    <t>blueprint partners</t>
+  </si>
+  <si>
+    <t>https://www.blueprintpartners.com/job-opportunities</t>
+  </si>
+  <si>
+    <t>capital economics</t>
+  </si>
+  <si>
+    <t>https://www.capitaleconomics.com/careers</t>
+  </si>
+  <si>
+    <t>carnall farrar</t>
   </si>
   <si>
     <t>Big Bus Tours</t>
@@ -3328,7 +3424,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="35">
+  <fonts count="37">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3430,6 +3526,17 @@
       <sz val="11"/>
       <name val="Aptos"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
     </font>
     <font>
       <u/>
@@ -4056,134 +4163,134 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="7" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="7" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="8" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -4341,14 +4448,29 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4703,8 +4825,8 @@
   </sheetPr>
   <dimension ref="A1:D840"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A539" workbookViewId="0">
+      <selection activeCell="D543" sqref="D543:D560"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="3"/>
@@ -12317,1730 +12439,1917 @@
         <v>3</v>
       </c>
     </row>
-    <row r="544" spans="4:4">
-      <c r="D544" s="55"/>
-    </row>
-    <row r="545" spans="4:4">
-      <c r="D545" s="55"/>
-    </row>
-    <row r="546" spans="4:4">
-      <c r="D546" s="55"/>
-    </row>
-    <row r="547" spans="4:4">
-      <c r="D547" s="55"/>
-    </row>
-    <row r="548" spans="4:4">
-      <c r="D548" s="55"/>
-    </row>
-    <row r="549" spans="4:4">
-      <c r="D549" s="55"/>
-    </row>
-    <row r="550" spans="4:4">
-      <c r="D550" s="55"/>
-    </row>
-    <row r="551" spans="4:4">
-      <c r="D551" s="55"/>
-    </row>
-    <row r="552" spans="4:4">
-      <c r="D552" s="55"/>
-    </row>
-    <row r="553" spans="4:4">
-      <c r="D553" s="55"/>
-    </row>
-    <row r="554" spans="4:4">
-      <c r="D554" s="55"/>
-    </row>
-    <row r="555" spans="4:4">
-      <c r="D555" s="55"/>
-    </row>
-    <row r="556" spans="4:4">
-      <c r="D556" s="55"/>
-    </row>
-    <row r="557" spans="4:4">
-      <c r="D557" s="55"/>
-    </row>
-    <row r="558" spans="4:4">
-      <c r="D558" s="55"/>
-    </row>
-    <row r="559" spans="4:4">
-      <c r="D559" s="55"/>
-    </row>
-    <row r="560" spans="4:4">
-      <c r="D560" s="55"/>
+    <row r="544" ht="28.8" spans="1:4">
+      <c r="A544" s="55">
+        <v>601</v>
+      </c>
+      <c r="B544" s="56" t="s">
+        <v>1086</v>
+      </c>
+      <c r="C544" s="57" t="s">
+        <v>1087</v>
+      </c>
+      <c r="D544" s="54" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="545" spans="1:4">
+      <c r="A545" s="55">
+        <v>602</v>
+      </c>
+      <c r="B545" s="56" t="s">
+        <v>1088</v>
+      </c>
+      <c r="C545" s="57" t="s">
+        <v>1089</v>
+      </c>
+      <c r="D545" s="54" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="546" ht="28.8" spans="1:4">
+      <c r="A546" s="55">
+        <v>603</v>
+      </c>
+      <c r="B546" s="58" t="s">
+        <v>1090</v>
+      </c>
+      <c r="C546" s="57" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D546" s="54" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="547" spans="1:4">
+      <c r="A547" s="55">
+        <v>605</v>
+      </c>
+      <c r="B547" s="56" t="s">
+        <v>1092</v>
+      </c>
+      <c r="C547" s="57" t="s">
+        <v>1093</v>
+      </c>
+      <c r="D547" s="54" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="548" spans="1:4">
+      <c r="A548" s="55">
+        <v>606</v>
+      </c>
+      <c r="B548" s="58" t="s">
+        <v>1094</v>
+      </c>
+      <c r="C548" s="57" t="s">
+        <v>1095</v>
+      </c>
+      <c r="D548" s="54" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="549" spans="1:4">
+      <c r="A549" s="55">
+        <v>607</v>
+      </c>
+      <c r="B549" s="56" t="s">
+        <v>1096</v>
+      </c>
+      <c r="C549" s="57" t="s">
+        <v>1097</v>
+      </c>
+      <c r="D549" s="54" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="550" spans="1:4">
+      <c r="A550" s="55">
+        <v>608</v>
+      </c>
+      <c r="B550" s="59" t="s">
+        <v>1098</v>
+      </c>
+      <c r="C550" s="57" t="s">
+        <v>1099</v>
+      </c>
+      <c r="D550" s="54" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="551" spans="1:4">
+      <c r="A551" s="55">
+        <v>609</v>
+      </c>
+      <c r="B551" s="59" t="s">
+        <v>1100</v>
+      </c>
+      <c r="C551" s="57" t="s">
+        <v>147</v>
+      </c>
+      <c r="D551" s="54" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="552" spans="1:4">
+      <c r="A552" s="55">
+        <v>610</v>
+      </c>
+      <c r="B552" s="56" t="s">
+        <v>1101</v>
+      </c>
+      <c r="C552" s="57" t="s">
+        <v>1102</v>
+      </c>
+      <c r="D552" s="54" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="553" spans="1:4">
+      <c r="A553" s="55">
+        <v>611</v>
+      </c>
+      <c r="B553" s="59" t="s">
+        <v>1103</v>
+      </c>
+      <c r="C553" s="57" t="s">
+        <v>1104</v>
+      </c>
+      <c r="D553" s="54" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="554" spans="1:4">
+      <c r="A554" s="55">
+        <v>612</v>
+      </c>
+      <c r="B554" s="56" t="s">
+        <v>1105</v>
+      </c>
+      <c r="C554" s="57" t="s">
+        <v>1106</v>
+      </c>
+      <c r="D554" s="54" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="555" spans="1:4">
+      <c r="A555" s="55">
+        <v>613</v>
+      </c>
+      <c r="B555" s="58" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C555" s="57" t="s">
+        <v>1108</v>
+      </c>
+      <c r="D555" s="54" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="556" spans="1:4">
+      <c r="A556" s="55">
+        <v>614</v>
+      </c>
+      <c r="B556" s="56" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C556" s="57" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D556" s="54" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="557" spans="1:4">
+      <c r="A557" s="55">
+        <v>615</v>
+      </c>
+      <c r="B557" s="56" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C557" s="57" t="s">
+        <v>1112</v>
+      </c>
+      <c r="D557" s="54" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="558" spans="1:4">
+      <c r="A558" s="55">
+        <v>616</v>
+      </c>
+      <c r="B558" s="59" t="s">
+        <v>1113</v>
+      </c>
+      <c r="C558" s="57" t="s">
+        <v>1114</v>
+      </c>
+      <c r="D558" s="54" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="559" spans="1:4">
+      <c r="A559" s="55">
+        <v>617</v>
+      </c>
+      <c r="B559" s="58" t="s">
+        <v>1115</v>
+      </c>
+      <c r="C559" s="57" t="s">
+        <v>1116</v>
+      </c>
+      <c r="D559" s="54" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="560" spans="1:4">
+      <c r="A560" s="55">
+        <v>618</v>
+      </c>
+      <c r="B560" s="56" t="s">
+        <v>1117</v>
+      </c>
+      <c r="C560" s="57" t="s">
+        <v>667</v>
+      </c>
+      <c r="D560" s="54" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="561" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A561" s="56"/>
-      <c r="B561" s="57"/>
-      <c r="C561" s="57"/>
-      <c r="D561" s="55"/>
+      <c r="A561" s="60"/>
+      <c r="B561" s="61"/>
+      <c r="C561" s="61"/>
+      <c r="D561" s="62"/>
     </row>
     <row r="562" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A562" s="56"/>
-      <c r="B562" s="57"/>
-      <c r="C562" s="57"/>
-      <c r="D562" s="55"/>
+      <c r="A562" s="60"/>
+      <c r="B562" s="61"/>
+      <c r="C562" s="61"/>
+      <c r="D562" s="62"/>
     </row>
     <row r="563" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A563" s="56"/>
-      <c r="B563" s="57"/>
-      <c r="C563" s="57"/>
-      <c r="D563" s="55"/>
+      <c r="A563" s="60"/>
+      <c r="B563" s="61"/>
+      <c r="C563" s="61"/>
+      <c r="D563" s="62"/>
     </row>
     <row r="564" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A564" s="56"/>
-      <c r="B564" s="57"/>
-      <c r="C564" s="57"/>
-      <c r="D564" s="55"/>
+      <c r="A564" s="60"/>
+      <c r="B564" s="61"/>
+      <c r="C564" s="61"/>
+      <c r="D564" s="62"/>
     </row>
     <row r="565" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A565" s="56"/>
-      <c r="B565" s="57"/>
-      <c r="C565" s="57"/>
-      <c r="D565" s="55"/>
+      <c r="A565" s="60"/>
+      <c r="B565" s="61"/>
+      <c r="C565" s="61"/>
+      <c r="D565" s="62"/>
     </row>
     <row r="566" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A566" s="56"/>
-      <c r="B566" s="57"/>
-      <c r="C566" s="57"/>
-      <c r="D566" s="55"/>
+      <c r="A566" s="60"/>
+      <c r="B566" s="61"/>
+      <c r="C566" s="61"/>
+      <c r="D566" s="62"/>
     </row>
     <row r="567" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A567" s="56"/>
-      <c r="B567" s="57"/>
-      <c r="C567" s="57"/>
-      <c r="D567" s="55"/>
+      <c r="A567" s="60"/>
+      <c r="B567" s="61"/>
+      <c r="C567" s="61"/>
+      <c r="D567" s="62"/>
     </row>
     <row r="568" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A568" s="56"/>
-      <c r="B568" s="57"/>
-      <c r="C568" s="57"/>
-      <c r="D568" s="55"/>
+      <c r="A568" s="60"/>
+      <c r="B568" s="61"/>
+      <c r="C568" s="61"/>
+      <c r="D568" s="62"/>
     </row>
     <row r="569" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A569" s="56"/>
-      <c r="B569" s="57"/>
-      <c r="C569" s="57"/>
-      <c r="D569" s="55"/>
+      <c r="A569" s="60"/>
+      <c r="B569" s="61"/>
+      <c r="C569" s="61"/>
+      <c r="D569" s="62"/>
     </row>
     <row r="570" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A570" s="56"/>
-      <c r="B570" s="57"/>
-      <c r="C570" s="57"/>
-      <c r="D570" s="55"/>
+      <c r="A570" s="60"/>
+      <c r="B570" s="61"/>
+      <c r="C570" s="61"/>
+      <c r="D570" s="62"/>
     </row>
     <row r="571" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A571" s="56"/>
-      <c r="B571" s="57"/>
-      <c r="C571" s="57"/>
-      <c r="D571" s="55"/>
+      <c r="A571" s="60"/>
+      <c r="B571" s="61"/>
+      <c r="C571" s="61"/>
+      <c r="D571" s="62"/>
     </row>
     <row r="572" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A572" s="56"/>
-      <c r="B572" s="57"/>
-      <c r="C572" s="57"/>
-      <c r="D572" s="55"/>
+      <c r="A572" s="60"/>
+      <c r="B572" s="61"/>
+      <c r="C572" s="61"/>
+      <c r="D572" s="62"/>
     </row>
     <row r="573" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A573" s="56"/>
-      <c r="B573" s="57"/>
-      <c r="C573" s="57"/>
-      <c r="D573" s="58"/>
+      <c r="A573" s="60"/>
+      <c r="B573" s="61"/>
+      <c r="C573" s="61"/>
+      <c r="D573" s="63"/>
     </row>
     <row r="575" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A575" s="56"/>
-      <c r="B575" s="57"/>
-      <c r="C575" s="57"/>
-      <c r="D575" s="58"/>
+      <c r="A575" s="60"/>
+      <c r="B575" s="61"/>
+      <c r="C575" s="61"/>
+      <c r="D575" s="63"/>
     </row>
     <row r="576" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A576" s="56"/>
-      <c r="B576" s="57"/>
-      <c r="C576" s="57"/>
-      <c r="D576" s="58"/>
+      <c r="A576" s="60"/>
+      <c r="B576" s="61"/>
+      <c r="C576" s="61"/>
+      <c r="D576" s="63"/>
     </row>
     <row r="577" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A577" s="56"/>
-      <c r="B577" s="57"/>
-      <c r="C577" s="57"/>
-      <c r="D577" s="58"/>
+      <c r="A577" s="60"/>
+      <c r="B577" s="61"/>
+      <c r="C577" s="61"/>
+      <c r="D577" s="63"/>
     </row>
     <row r="578" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A578" s="56"/>
-      <c r="B578" s="57"/>
-      <c r="C578" s="57"/>
-      <c r="D578" s="58"/>
+      <c r="A578" s="60"/>
+      <c r="B578" s="61"/>
+      <c r="C578" s="61"/>
+      <c r="D578" s="63"/>
     </row>
     <row r="579" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A579" s="56"/>
-      <c r="B579" s="57"/>
-      <c r="C579" s="57"/>
-      <c r="D579" s="58"/>
+      <c r="A579" s="60"/>
+      <c r="B579" s="61"/>
+      <c r="C579" s="61"/>
+      <c r="D579" s="63"/>
     </row>
     <row r="580" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A580" s="56"/>
-      <c r="B580" s="57"/>
-      <c r="C580" s="57"/>
-      <c r="D580" s="58"/>
+      <c r="A580" s="60"/>
+      <c r="B580" s="61"/>
+      <c r="C580" s="61"/>
+      <c r="D580" s="63"/>
     </row>
     <row r="581" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A581" s="56"/>
-      <c r="B581" s="57"/>
-      <c r="C581" s="57"/>
-      <c r="D581" s="58"/>
+      <c r="A581" s="60"/>
+      <c r="B581" s="61"/>
+      <c r="C581" s="61"/>
+      <c r="D581" s="63"/>
     </row>
     <row r="582" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A582" s="56"/>
-      <c r="B582" s="57"/>
-      <c r="C582" s="57"/>
-      <c r="D582" s="58"/>
+      <c r="A582" s="60"/>
+      <c r="B582" s="61"/>
+      <c r="C582" s="61"/>
+      <c r="D582" s="63"/>
     </row>
     <row r="583" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A583" s="56"/>
-      <c r="B583" s="57"/>
-      <c r="C583" s="57"/>
-      <c r="D583" s="58"/>
+      <c r="A583" s="60"/>
+      <c r="B583" s="61"/>
+      <c r="C583" s="61"/>
+      <c r="D583" s="63"/>
     </row>
     <row r="584" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A584" s="56"/>
-      <c r="B584" s="57"/>
-      <c r="C584" s="57"/>
-      <c r="D584" s="58"/>
+      <c r="A584" s="60"/>
+      <c r="B584" s="61"/>
+      <c r="C584" s="61"/>
+      <c r="D584" s="63"/>
     </row>
     <row r="585" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A585" s="56"/>
-      <c r="B585" s="57"/>
-      <c r="C585" s="57"/>
-      <c r="D585" s="58"/>
+      <c r="A585" s="60"/>
+      <c r="B585" s="61"/>
+      <c r="C585" s="61"/>
+      <c r="D585" s="63"/>
     </row>
     <row r="586" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A586" s="56"/>
-      <c r="B586" s="57"/>
-      <c r="C586" s="57"/>
-      <c r="D586" s="58"/>
+      <c r="A586" s="60"/>
+      <c r="B586" s="61"/>
+      <c r="C586" s="61"/>
+      <c r="D586" s="63"/>
     </row>
     <row r="587" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A587" s="56"/>
-      <c r="B587" s="57"/>
-      <c r="C587" s="57"/>
-      <c r="D587" s="58"/>
+      <c r="A587" s="60"/>
+      <c r="B587" s="61"/>
+      <c r="C587" s="61"/>
+      <c r="D587" s="63"/>
     </row>
     <row r="588" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A588" s="56"/>
-      <c r="B588" s="57"/>
-      <c r="C588" s="57"/>
-      <c r="D588" s="58"/>
+      <c r="A588" s="60"/>
+      <c r="B588" s="61"/>
+      <c r="C588" s="61"/>
+      <c r="D588" s="63"/>
     </row>
     <row r="589" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A589" s="56"/>
-      <c r="B589" s="57"/>
-      <c r="C589" s="57"/>
-      <c r="D589" s="58"/>
+      <c r="A589" s="60"/>
+      <c r="B589" s="61"/>
+      <c r="C589" s="61"/>
+      <c r="D589" s="63"/>
     </row>
     <row r="590" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A590" s="56"/>
-      <c r="B590" s="57"/>
-      <c r="C590" s="57"/>
-      <c r="D590" s="58"/>
+      <c r="A590" s="60"/>
+      <c r="B590" s="61"/>
+      <c r="C590" s="61"/>
+      <c r="D590" s="63"/>
     </row>
     <row r="591" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A591" s="56"/>
-      <c r="B591" s="57"/>
-      <c r="C591" s="57"/>
-      <c r="D591" s="58"/>
+      <c r="A591" s="60"/>
+      <c r="B591" s="61"/>
+      <c r="C591" s="61"/>
+      <c r="D591" s="63"/>
     </row>
     <row r="592" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A592" s="56"/>
-      <c r="B592" s="57"/>
-      <c r="C592" s="57"/>
-      <c r="D592" s="58"/>
+      <c r="A592" s="60"/>
+      <c r="B592" s="61"/>
+      <c r="C592" s="61"/>
+      <c r="D592" s="63"/>
     </row>
     <row r="593" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A593" s="56"/>
-      <c r="B593" s="57"/>
-      <c r="C593" s="57"/>
-      <c r="D593" s="58"/>
+      <c r="A593" s="60"/>
+      <c r="B593" s="61"/>
+      <c r="C593" s="61"/>
+      <c r="D593" s="63"/>
     </row>
     <row r="594" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A594" s="56"/>
-      <c r="B594" s="57"/>
-      <c r="C594" s="57"/>
-      <c r="D594" s="58"/>
+      <c r="A594" s="60"/>
+      <c r="B594" s="61"/>
+      <c r="C594" s="61"/>
+      <c r="D594" s="63"/>
     </row>
     <row r="595" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A595" s="56"/>
-      <c r="B595" s="57"/>
-      <c r="C595" s="57"/>
-      <c r="D595" s="58"/>
+      <c r="A595" s="60"/>
+      <c r="B595" s="61"/>
+      <c r="C595" s="61"/>
+      <c r="D595" s="63"/>
     </row>
     <row r="596" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A596" s="56"/>
-      <c r="B596" s="57"/>
-      <c r="C596" s="57"/>
-      <c r="D596" s="58"/>
+      <c r="A596" s="60"/>
+      <c r="B596" s="61"/>
+      <c r="C596" s="61"/>
+      <c r="D596" s="63"/>
     </row>
     <row r="597" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A597" s="56"/>
-      <c r="B597" s="57"/>
-      <c r="C597" s="57"/>
-      <c r="D597" s="58"/>
+      <c r="A597" s="60"/>
+      <c r="B597" s="61"/>
+      <c r="C597" s="61"/>
+      <c r="D597" s="63"/>
     </row>
     <row r="598" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A598" s="56"/>
-      <c r="B598" s="57"/>
-      <c r="C598" s="57"/>
-      <c r="D598" s="58"/>
+      <c r="A598" s="60"/>
+      <c r="B598" s="61"/>
+      <c r="C598" s="61"/>
+      <c r="D598" s="63"/>
     </row>
     <row r="599" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A599" s="56"/>
-      <c r="B599" s="57"/>
-      <c r="C599" s="57"/>
-      <c r="D599" s="58"/>
+      <c r="A599" s="60"/>
+      <c r="B599" s="61"/>
+      <c r="C599" s="61"/>
+      <c r="D599" s="63"/>
     </row>
     <row r="600" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A600" s="56"/>
-      <c r="B600" s="57"/>
-      <c r="C600" s="57"/>
-      <c r="D600" s="58"/>
+      <c r="A600" s="60"/>
+      <c r="B600" s="61"/>
+      <c r="C600" s="61"/>
+      <c r="D600" s="63"/>
     </row>
     <row r="601" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A601" s="56"/>
-      <c r="B601" s="57"/>
-      <c r="C601" s="57"/>
-      <c r="D601" s="58"/>
+      <c r="A601" s="60"/>
+      <c r="B601" s="61"/>
+      <c r="C601" s="61"/>
+      <c r="D601" s="63"/>
     </row>
     <row r="602" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A602" s="56"/>
-      <c r="B602" s="57"/>
-      <c r="C602" s="57"/>
-      <c r="D602" s="58"/>
+      <c r="A602" s="60"/>
+      <c r="B602" s="61"/>
+      <c r="C602" s="61"/>
+      <c r="D602" s="63"/>
     </row>
     <row r="603" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A603" s="56"/>
-      <c r="B603" s="57"/>
-      <c r="C603" s="57"/>
-      <c r="D603" s="58"/>
+      <c r="A603" s="60"/>
+      <c r="B603" s="61"/>
+      <c r="C603" s="61"/>
+      <c r="D603" s="63"/>
     </row>
     <row r="604" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A604" s="56"/>
-      <c r="B604" s="57"/>
-      <c r="C604" s="57"/>
-      <c r="D604" s="58"/>
+      <c r="A604" s="60"/>
+      <c r="B604" s="61"/>
+      <c r="C604" s="61"/>
+      <c r="D604" s="63"/>
     </row>
     <row r="605" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A605" s="56"/>
-      <c r="B605" s="57"/>
-      <c r="C605" s="57"/>
-      <c r="D605" s="58"/>
+      <c r="A605" s="60"/>
+      <c r="B605" s="61"/>
+      <c r="C605" s="61"/>
+      <c r="D605" s="63"/>
     </row>
     <row r="606" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A606" s="56"/>
-      <c r="B606" s="57"/>
-      <c r="C606" s="57"/>
-      <c r="D606" s="58"/>
+      <c r="A606" s="60"/>
+      <c r="B606" s="61"/>
+      <c r="C606" s="61"/>
+      <c r="D606" s="63"/>
     </row>
     <row r="607" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A607" s="56"/>
-      <c r="B607" s="57"/>
-      <c r="C607" s="57"/>
-      <c r="D607" s="58"/>
+      <c r="A607" s="60"/>
+      <c r="B607" s="61"/>
+      <c r="C607" s="61"/>
+      <c r="D607" s="63"/>
     </row>
     <row r="608" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A608" s="56"/>
-      <c r="B608" s="57"/>
-      <c r="C608" s="57"/>
-      <c r="D608" s="58"/>
+      <c r="A608" s="60"/>
+      <c r="B608" s="61"/>
+      <c r="C608" s="61"/>
+      <c r="D608" s="63"/>
     </row>
     <row r="609" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A609" s="56"/>
-      <c r="B609" s="57"/>
-      <c r="C609" s="57"/>
-      <c r="D609" s="58"/>
+      <c r="A609" s="60"/>
+      <c r="B609" s="61"/>
+      <c r="C609" s="61"/>
+      <c r="D609" s="63"/>
     </row>
     <row r="610" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A610" s="56"/>
-      <c r="B610" s="57"/>
-      <c r="C610" s="57"/>
-      <c r="D610" s="58"/>
+      <c r="A610" s="60"/>
+      <c r="B610" s="61"/>
+      <c r="C610" s="61"/>
+      <c r="D610" s="63"/>
     </row>
     <row r="611" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A611" s="56"/>
-      <c r="B611" s="57"/>
-      <c r="C611" s="57"/>
-      <c r="D611" s="58"/>
+      <c r="A611" s="60"/>
+      <c r="B611" s="61"/>
+      <c r="C611" s="61"/>
+      <c r="D611" s="63"/>
     </row>
     <row r="612" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A612" s="56"/>
-      <c r="B612" s="57"/>
-      <c r="C612" s="57"/>
-      <c r="D612" s="58"/>
+      <c r="A612" s="60"/>
+      <c r="B612" s="61"/>
+      <c r="C612" s="61"/>
+      <c r="D612" s="63"/>
     </row>
     <row r="613" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A613" s="56"/>
-      <c r="B613" s="57"/>
-      <c r="C613" s="57"/>
-      <c r="D613" s="58"/>
+      <c r="A613" s="60"/>
+      <c r="B613" s="61"/>
+      <c r="C613" s="61"/>
+      <c r="D613" s="63"/>
     </row>
     <row r="614" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A614" s="56"/>
-      <c r="B614" s="57"/>
-      <c r="C614" s="57"/>
-      <c r="D614" s="58"/>
+      <c r="A614" s="60"/>
+      <c r="B614" s="61"/>
+      <c r="C614" s="61"/>
+      <c r="D614" s="63"/>
     </row>
     <row r="615" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A615" s="56"/>
-      <c r="B615" s="57"/>
-      <c r="C615" s="57"/>
-      <c r="D615" s="58"/>
+      <c r="A615" s="60"/>
+      <c r="B615" s="61"/>
+      <c r="C615" s="61"/>
+      <c r="D615" s="63"/>
     </row>
     <row r="616" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A616" s="56"/>
-      <c r="B616" s="57"/>
-      <c r="C616" s="57"/>
-      <c r="D616" s="58"/>
+      <c r="A616" s="60"/>
+      <c r="B616" s="61"/>
+      <c r="C616" s="61"/>
+      <c r="D616" s="63"/>
     </row>
     <row r="617" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A617" s="56"/>
-      <c r="B617" s="57"/>
-      <c r="C617" s="57"/>
-      <c r="D617" s="58"/>
+      <c r="A617" s="60"/>
+      <c r="B617" s="61"/>
+      <c r="C617" s="61"/>
+      <c r="D617" s="63"/>
     </row>
     <row r="618" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A618" s="56"/>
-      <c r="B618" s="57"/>
-      <c r="C618" s="57"/>
-      <c r="D618" s="58"/>
+      <c r="A618" s="60"/>
+      <c r="B618" s="61"/>
+      <c r="C618" s="61"/>
+      <c r="D618" s="63"/>
     </row>
     <row r="619" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A619" s="56"/>
-      <c r="B619" s="57"/>
-      <c r="C619" s="57"/>
-      <c r="D619" s="58"/>
+      <c r="A619" s="60"/>
+      <c r="B619" s="61"/>
+      <c r="C619" s="61"/>
+      <c r="D619" s="63"/>
     </row>
     <row r="620" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A620" s="56"/>
-      <c r="B620" s="57"/>
-      <c r="C620" s="57"/>
-      <c r="D620" s="58"/>
+      <c r="A620" s="60"/>
+      <c r="B620" s="61"/>
+      <c r="C620" s="61"/>
+      <c r="D620" s="63"/>
     </row>
     <row r="621" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A621" s="56"/>
-      <c r="B621" s="57"/>
-      <c r="C621" s="57"/>
-      <c r="D621" s="58"/>
+      <c r="A621" s="60"/>
+      <c r="B621" s="61"/>
+      <c r="C621" s="61"/>
+      <c r="D621" s="63"/>
     </row>
     <row r="622" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A622" s="56"/>
-      <c r="B622" s="57"/>
-      <c r="C622" s="57"/>
-      <c r="D622" s="58"/>
+      <c r="A622" s="60"/>
+      <c r="B622" s="61"/>
+      <c r="C622" s="61"/>
+      <c r="D622" s="63"/>
     </row>
     <row r="623" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A623" s="56"/>
-      <c r="B623" s="57"/>
-      <c r="C623" s="57"/>
-      <c r="D623" s="58"/>
+      <c r="A623" s="60"/>
+      <c r="B623" s="61"/>
+      <c r="C623" s="61"/>
+      <c r="D623" s="63"/>
     </row>
     <row r="624" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A624" s="56"/>
-      <c r="B624" s="57"/>
-      <c r="C624" s="57"/>
-      <c r="D624" s="58"/>
+      <c r="A624" s="60"/>
+      <c r="B624" s="61"/>
+      <c r="C624" s="61"/>
+      <c r="D624" s="63"/>
     </row>
     <row r="625" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A625" s="56"/>
-      <c r="B625" s="57"/>
-      <c r="C625" s="57"/>
-      <c r="D625" s="58"/>
+      <c r="A625" s="60"/>
+      <c r="B625" s="61"/>
+      <c r="C625" s="61"/>
+      <c r="D625" s="63"/>
     </row>
     <row r="626" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A626" s="56"/>
-      <c r="B626" s="57"/>
-      <c r="C626" s="57"/>
-      <c r="D626" s="58"/>
+      <c r="A626" s="60"/>
+      <c r="B626" s="61"/>
+      <c r="C626" s="61"/>
+      <c r="D626" s="63"/>
     </row>
     <row r="627" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A627" s="56"/>
-      <c r="B627" s="57"/>
-      <c r="C627" s="57"/>
-      <c r="D627" s="58"/>
+      <c r="A627" s="60"/>
+      <c r="B627" s="61"/>
+      <c r="C627" s="61"/>
+      <c r="D627" s="63"/>
     </row>
     <row r="628" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A628" s="56"/>
-      <c r="B628" s="57"/>
-      <c r="C628" s="57"/>
-      <c r="D628" s="58"/>
+      <c r="A628" s="60"/>
+      <c r="B628" s="61"/>
+      <c r="C628" s="61"/>
+      <c r="D628" s="63"/>
     </row>
     <row r="629" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A629" s="56"/>
-      <c r="B629" s="57"/>
-      <c r="C629" s="57"/>
-      <c r="D629" s="58"/>
+      <c r="A629" s="60"/>
+      <c r="B629" s="61"/>
+      <c r="C629" s="61"/>
+      <c r="D629" s="63"/>
     </row>
     <row r="630" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A630" s="56"/>
-      <c r="B630" s="57"/>
-      <c r="C630" s="57"/>
-      <c r="D630" s="58"/>
+      <c r="A630" s="60"/>
+      <c r="B630" s="61"/>
+      <c r="C630" s="61"/>
+      <c r="D630" s="63"/>
     </row>
     <row r="631" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A631" s="56"/>
-      <c r="B631" s="57"/>
-      <c r="C631" s="57"/>
-      <c r="D631" s="58"/>
+      <c r="A631" s="60"/>
+      <c r="B631" s="61"/>
+      <c r="C631" s="61"/>
+      <c r="D631" s="63"/>
     </row>
     <row r="632" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A632" s="56"/>
-      <c r="B632" s="57"/>
-      <c r="C632" s="57"/>
-      <c r="D632" s="58"/>
+      <c r="A632" s="60"/>
+      <c r="B632" s="61"/>
+      <c r="C632" s="61"/>
+      <c r="D632" s="63"/>
     </row>
     <row r="633" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A633" s="56"/>
-      <c r="B633" s="57"/>
-      <c r="C633" s="57"/>
-      <c r="D633" s="58"/>
+      <c r="A633" s="60"/>
+      <c r="B633" s="61"/>
+      <c r="C633" s="61"/>
+      <c r="D633" s="63"/>
     </row>
     <row r="634" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A634" s="56"/>
-      <c r="B634" s="57"/>
-      <c r="C634" s="57"/>
-      <c r="D634" s="58"/>
+      <c r="A634" s="60"/>
+      <c r="B634" s="61"/>
+      <c r="C634" s="61"/>
+      <c r="D634" s="63"/>
     </row>
     <row r="635" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A635" s="56"/>
-      <c r="B635" s="57"/>
-      <c r="C635" s="57"/>
-      <c r="D635" s="58"/>
+      <c r="A635" s="60"/>
+      <c r="B635" s="61"/>
+      <c r="C635" s="61"/>
+      <c r="D635" s="63"/>
     </row>
     <row r="636" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A636" s="56"/>
-      <c r="B636" s="57"/>
-      <c r="C636" s="57"/>
-      <c r="D636" s="58"/>
+      <c r="A636" s="60"/>
+      <c r="B636" s="61"/>
+      <c r="C636" s="61"/>
+      <c r="D636" s="63"/>
     </row>
     <row r="637" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A637" s="56"/>
-      <c r="B637" s="57"/>
-      <c r="C637" s="57"/>
-      <c r="D637" s="58"/>
+      <c r="A637" s="60"/>
+      <c r="B637" s="61"/>
+      <c r="C637" s="61"/>
+      <c r="D637" s="63"/>
     </row>
     <row r="638" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A638" s="56"/>
-      <c r="B638" s="57"/>
-      <c r="C638" s="57"/>
-      <c r="D638" s="58"/>
+      <c r="A638" s="60"/>
+      <c r="B638" s="61"/>
+      <c r="C638" s="61"/>
+      <c r="D638" s="63"/>
     </row>
     <row r="639" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A639" s="56"/>
-      <c r="B639" s="57"/>
-      <c r="C639" s="57"/>
-      <c r="D639" s="58"/>
+      <c r="A639" s="60"/>
+      <c r="B639" s="61"/>
+      <c r="C639" s="61"/>
+      <c r="D639" s="63"/>
     </row>
     <row r="640" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A640" s="56"/>
-      <c r="B640" s="57"/>
-      <c r="C640" s="57"/>
-      <c r="D640" s="58"/>
+      <c r="A640" s="60"/>
+      <c r="B640" s="61"/>
+      <c r="C640" s="61"/>
+      <c r="D640" s="63"/>
     </row>
     <row r="641" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A641" s="56"/>
-      <c r="B641" s="57"/>
-      <c r="C641" s="57"/>
-      <c r="D641" s="58"/>
+      <c r="A641" s="60"/>
+      <c r="B641" s="61"/>
+      <c r="C641" s="61"/>
+      <c r="D641" s="63"/>
     </row>
     <row r="642" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A642" s="56"/>
-      <c r="B642" s="57"/>
-      <c r="C642" s="57"/>
-      <c r="D642" s="58"/>
+      <c r="A642" s="60"/>
+      <c r="B642" s="61"/>
+      <c r="C642" s="61"/>
+      <c r="D642" s="63"/>
     </row>
     <row r="643" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A643" s="56"/>
-      <c r="B643" s="57"/>
-      <c r="C643" s="57"/>
-      <c r="D643" s="58"/>
+      <c r="A643" s="60"/>
+      <c r="B643" s="61"/>
+      <c r="C643" s="61"/>
+      <c r="D643" s="63"/>
     </row>
     <row r="644" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A644" s="56"/>
-      <c r="B644" s="57"/>
-      <c r="C644" s="57"/>
-      <c r="D644" s="58"/>
+      <c r="A644" s="60"/>
+      <c r="B644" s="61"/>
+      <c r="C644" s="61"/>
+      <c r="D644" s="63"/>
     </row>
     <row r="645" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A645" s="56"/>
-      <c r="B645" s="57"/>
-      <c r="C645" s="57"/>
-      <c r="D645" s="58"/>
+      <c r="A645" s="60"/>
+      <c r="B645" s="61"/>
+      <c r="C645" s="61"/>
+      <c r="D645" s="63"/>
     </row>
     <row r="646" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A646" s="56"/>
-      <c r="B646" s="57"/>
-      <c r="C646" s="57"/>
-      <c r="D646" s="58"/>
+      <c r="A646" s="60"/>
+      <c r="B646" s="61"/>
+      <c r="C646" s="61"/>
+      <c r="D646" s="63"/>
     </row>
     <row r="647" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A647" s="56"/>
-      <c r="B647" s="57"/>
-      <c r="C647" s="57"/>
-      <c r="D647" s="58"/>
+      <c r="A647" s="60"/>
+      <c r="B647" s="61"/>
+      <c r="C647" s="61"/>
+      <c r="D647" s="63"/>
     </row>
     <row r="648" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A648" s="56"/>
-      <c r="B648" s="57"/>
-      <c r="C648" s="57"/>
-      <c r="D648" s="58"/>
+      <c r="A648" s="60"/>
+      <c r="B648" s="61"/>
+      <c r="C648" s="61"/>
+      <c r="D648" s="63"/>
     </row>
     <row r="649" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A649" s="56"/>
-      <c r="B649" s="57"/>
-      <c r="C649" s="57"/>
-      <c r="D649" s="58"/>
+      <c r="A649" s="60"/>
+      <c r="B649" s="61"/>
+      <c r="C649" s="61"/>
+      <c r="D649" s="63"/>
     </row>
     <row r="650" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A650" s="56"/>
-      <c r="B650" s="57"/>
-      <c r="C650" s="57"/>
-      <c r="D650" s="58"/>
+      <c r="A650" s="60"/>
+      <c r="B650" s="61"/>
+      <c r="C650" s="61"/>
+      <c r="D650" s="63"/>
     </row>
     <row r="651" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A651" s="56"/>
-      <c r="B651" s="57"/>
-      <c r="C651" s="57"/>
-      <c r="D651" s="58"/>
+      <c r="A651" s="60"/>
+      <c r="B651" s="61"/>
+      <c r="C651" s="61"/>
+      <c r="D651" s="63"/>
     </row>
     <row r="652" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A652" s="56"/>
-      <c r="B652" s="57"/>
-      <c r="C652" s="57"/>
-      <c r="D652" s="58"/>
+      <c r="A652" s="60"/>
+      <c r="B652" s="61"/>
+      <c r="C652" s="61"/>
+      <c r="D652" s="63"/>
     </row>
     <row r="653" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A653" s="56"/>
-      <c r="B653" s="57"/>
-      <c r="C653" s="57"/>
-      <c r="D653" s="58"/>
+      <c r="A653" s="60"/>
+      <c r="B653" s="61"/>
+      <c r="C653" s="61"/>
+      <c r="D653" s="63"/>
     </row>
     <row r="654" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A654" s="56"/>
-      <c r="B654" s="57"/>
-      <c r="C654" s="57"/>
-      <c r="D654" s="58"/>
+      <c r="A654" s="60"/>
+      <c r="B654" s="61"/>
+      <c r="C654" s="61"/>
+      <c r="D654" s="63"/>
     </row>
     <row r="655" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A655" s="56"/>
-      <c r="B655" s="57"/>
-      <c r="C655" s="57"/>
-      <c r="D655" s="58"/>
+      <c r="A655" s="60"/>
+      <c r="B655" s="61"/>
+      <c r="C655" s="61"/>
+      <c r="D655" s="63"/>
     </row>
     <row r="656" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A656" s="56"/>
-      <c r="B656" s="57"/>
-      <c r="C656" s="57"/>
-      <c r="D656" s="58"/>
+      <c r="A656" s="60"/>
+      <c r="B656" s="61"/>
+      <c r="C656" s="61"/>
+      <c r="D656" s="63"/>
     </row>
     <row r="657" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A657" s="56"/>
-      <c r="B657" s="57"/>
-      <c r="C657" s="57"/>
-      <c r="D657" s="58"/>
+      <c r="A657" s="60"/>
+      <c r="B657" s="61"/>
+      <c r="C657" s="61"/>
+      <c r="D657" s="63"/>
     </row>
     <row r="658" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A658" s="56"/>
-      <c r="B658" s="57"/>
-      <c r="C658" s="57"/>
-      <c r="D658" s="58"/>
+      <c r="A658" s="60"/>
+      <c r="B658" s="61"/>
+      <c r="C658" s="61"/>
+      <c r="D658" s="63"/>
     </row>
     <row r="659" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A659" s="56"/>
-      <c r="B659" s="57"/>
-      <c r="C659" s="57"/>
-      <c r="D659" s="58"/>
+      <c r="A659" s="60"/>
+      <c r="B659" s="61"/>
+      <c r="C659" s="61"/>
+      <c r="D659" s="63"/>
     </row>
     <row r="660" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A660" s="56"/>
-      <c r="B660" s="57"/>
-      <c r="C660" s="57"/>
-      <c r="D660" s="58"/>
+      <c r="A660" s="60"/>
+      <c r="B660" s="61"/>
+      <c r="C660" s="61"/>
+      <c r="D660" s="63"/>
     </row>
     <row r="661" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A661" s="56"/>
-      <c r="B661" s="57"/>
-      <c r="C661" s="57"/>
-      <c r="D661" s="58"/>
+      <c r="A661" s="60"/>
+      <c r="B661" s="61"/>
+      <c r="C661" s="61"/>
+      <c r="D661" s="63"/>
     </row>
     <row r="662" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A662" s="56"/>
-      <c r="B662" s="57"/>
-      <c r="C662" s="57"/>
-      <c r="D662" s="58"/>
+      <c r="A662" s="60"/>
+      <c r="B662" s="61"/>
+      <c r="C662" s="61"/>
+      <c r="D662" s="63"/>
     </row>
     <row r="663" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A663" s="56"/>
-      <c r="B663" s="57"/>
-      <c r="C663" s="57"/>
-      <c r="D663" s="58"/>
+      <c r="A663" s="60"/>
+      <c r="B663" s="61"/>
+      <c r="C663" s="61"/>
+      <c r="D663" s="63"/>
     </row>
     <row r="664" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A664" s="56"/>
-      <c r="B664" s="57"/>
-      <c r="C664" s="57"/>
-      <c r="D664" s="58"/>
+      <c r="A664" s="60"/>
+      <c r="B664" s="61"/>
+      <c r="C664" s="61"/>
+      <c r="D664" s="63"/>
     </row>
     <row r="665" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A665" s="56"/>
-      <c r="B665" s="57"/>
-      <c r="C665" s="57"/>
-      <c r="D665" s="58"/>
+      <c r="A665" s="60"/>
+      <c r="B665" s="61"/>
+      <c r="C665" s="61"/>
+      <c r="D665" s="63"/>
     </row>
     <row r="666" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A666" s="56"/>
-      <c r="B666" s="57"/>
-      <c r="C666" s="57"/>
-      <c r="D666" s="58"/>
+      <c r="A666" s="60"/>
+      <c r="B666" s="61"/>
+      <c r="C666" s="61"/>
+      <c r="D666" s="63"/>
     </row>
     <row r="667" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A667" s="56"/>
-      <c r="B667" s="57"/>
-      <c r="C667" s="57"/>
-      <c r="D667" s="58"/>
+      <c r="A667" s="60"/>
+      <c r="B667" s="61"/>
+      <c r="C667" s="61"/>
+      <c r="D667" s="63"/>
     </row>
     <row r="668" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A668" s="56"/>
-      <c r="B668" s="57"/>
-      <c r="C668" s="57"/>
-      <c r="D668" s="58"/>
+      <c r="A668" s="60"/>
+      <c r="B668" s="61"/>
+      <c r="C668" s="61"/>
+      <c r="D668" s="63"/>
     </row>
     <row r="669" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A669" s="56"/>
-      <c r="B669" s="57"/>
-      <c r="C669" s="57"/>
-      <c r="D669" s="58"/>
+      <c r="A669" s="60"/>
+      <c r="B669" s="61"/>
+      <c r="C669" s="61"/>
+      <c r="D669" s="63"/>
     </row>
     <row r="670" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A670" s="56"/>
-      <c r="B670" s="57"/>
-      <c r="C670" s="57"/>
-      <c r="D670" s="58"/>
+      <c r="A670" s="60"/>
+      <c r="B670" s="61"/>
+      <c r="C670" s="61"/>
+      <c r="D670" s="63"/>
     </row>
     <row r="671" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A671" s="56"/>
-      <c r="B671" s="57"/>
-      <c r="C671" s="57"/>
-      <c r="D671" s="58"/>
+      <c r="A671" s="60"/>
+      <c r="B671" s="61"/>
+      <c r="C671" s="61"/>
+      <c r="D671" s="63"/>
     </row>
     <row r="672" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A672" s="56"/>
-      <c r="B672" s="57"/>
-      <c r="C672" s="57"/>
-      <c r="D672" s="58"/>
+      <c r="A672" s="60"/>
+      <c r="B672" s="61"/>
+      <c r="C672" s="61"/>
+      <c r="D672" s="63"/>
     </row>
     <row r="673" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A673" s="56"/>
-      <c r="B673" s="57"/>
-      <c r="C673" s="57"/>
-      <c r="D673" s="58"/>
+      <c r="A673" s="60"/>
+      <c r="B673" s="61"/>
+      <c r="C673" s="61"/>
+      <c r="D673" s="63"/>
     </row>
     <row r="674" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A674" s="56"/>
-      <c r="B674" s="57"/>
-      <c r="C674" s="57"/>
-      <c r="D674" s="58"/>
+      <c r="A674" s="60"/>
+      <c r="B674" s="61"/>
+      <c r="C674" s="61"/>
+      <c r="D674" s="63"/>
     </row>
     <row r="675" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A675" s="56"/>
-      <c r="B675" s="57"/>
-      <c r="C675" s="57"/>
-      <c r="D675" s="58"/>
+      <c r="A675" s="60"/>
+      <c r="B675" s="61"/>
+      <c r="C675" s="61"/>
+      <c r="D675" s="63"/>
     </row>
     <row r="676" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A676" s="56"/>
-      <c r="B676" s="57"/>
-      <c r="C676" s="57"/>
-      <c r="D676" s="58"/>
+      <c r="A676" s="60"/>
+      <c r="B676" s="61"/>
+      <c r="C676" s="61"/>
+      <c r="D676" s="63"/>
     </row>
     <row r="677" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A677" s="56"/>
-      <c r="B677" s="57"/>
-      <c r="C677" s="57"/>
-      <c r="D677" s="58"/>
+      <c r="A677" s="60"/>
+      <c r="B677" s="61"/>
+      <c r="C677" s="61"/>
+      <c r="D677" s="63"/>
     </row>
     <row r="678" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A678" s="56"/>
-      <c r="B678" s="57"/>
-      <c r="C678" s="57"/>
-      <c r="D678" s="58"/>
+      <c r="A678" s="60"/>
+      <c r="B678" s="61"/>
+      <c r="C678" s="61"/>
+      <c r="D678" s="63"/>
     </row>
     <row r="679" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A679" s="56"/>
-      <c r="B679" s="57"/>
-      <c r="C679" s="57"/>
-      <c r="D679" s="58"/>
+      <c r="A679" s="60"/>
+      <c r="B679" s="61"/>
+      <c r="C679" s="61"/>
+      <c r="D679" s="63"/>
     </row>
     <row r="680" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A680" s="56"/>
-      <c r="B680" s="57"/>
-      <c r="C680" s="57"/>
-      <c r="D680" s="58"/>
+      <c r="A680" s="60"/>
+      <c r="B680" s="61"/>
+      <c r="C680" s="61"/>
+      <c r="D680" s="63"/>
     </row>
     <row r="681" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A681" s="56"/>
-      <c r="B681" s="57"/>
-      <c r="C681" s="57"/>
-      <c r="D681" s="58"/>
+      <c r="A681" s="60"/>
+      <c r="B681" s="61"/>
+      <c r="C681" s="61"/>
+      <c r="D681" s="63"/>
     </row>
     <row r="682" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A682" s="56"/>
-      <c r="B682" s="57"/>
-      <c r="C682" s="57"/>
-      <c r="D682" s="58"/>
+      <c r="A682" s="60"/>
+      <c r="B682" s="61"/>
+      <c r="C682" s="61"/>
+      <c r="D682" s="63"/>
     </row>
     <row r="683" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A683" s="56"/>
-      <c r="B683" s="57"/>
-      <c r="C683" s="57"/>
-      <c r="D683" s="58"/>
+      <c r="A683" s="60"/>
+      <c r="B683" s="61"/>
+      <c r="C683" s="61"/>
+      <c r="D683" s="63"/>
     </row>
     <row r="684" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A684" s="56"/>
-      <c r="B684" s="57"/>
-      <c r="C684" s="57"/>
-      <c r="D684" s="58"/>
+      <c r="A684" s="60"/>
+      <c r="B684" s="61"/>
+      <c r="C684" s="61"/>
+      <c r="D684" s="63"/>
     </row>
     <row r="685" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A685" s="56"/>
-      <c r="B685" s="57"/>
-      <c r="C685" s="57"/>
-      <c r="D685" s="58"/>
+      <c r="A685" s="60"/>
+      <c r="B685" s="61"/>
+      <c r="C685" s="61"/>
+      <c r="D685" s="63"/>
     </row>
     <row r="686" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A686" s="56"/>
-      <c r="B686" s="57"/>
-      <c r="C686" s="57"/>
-      <c r="D686" s="58"/>
+      <c r="A686" s="60"/>
+      <c r="B686" s="61"/>
+      <c r="C686" s="61"/>
+      <c r="D686" s="63"/>
     </row>
     <row r="687" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A687" s="56"/>
-      <c r="B687" s="57"/>
-      <c r="C687" s="57"/>
-      <c r="D687" s="58"/>
+      <c r="A687" s="60"/>
+      <c r="B687" s="61"/>
+      <c r="C687" s="61"/>
+      <c r="D687" s="63"/>
     </row>
     <row r="688" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A688" s="56"/>
-      <c r="B688" s="57"/>
-      <c r="C688" s="57"/>
-      <c r="D688" s="58"/>
+      <c r="A688" s="60"/>
+      <c r="B688" s="61"/>
+      <c r="C688" s="61"/>
+      <c r="D688" s="63"/>
     </row>
     <row r="689" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A689" s="56"/>
-      <c r="B689" s="57"/>
-      <c r="C689" s="57"/>
-      <c r="D689" s="58"/>
+      <c r="A689" s="60"/>
+      <c r="B689" s="61"/>
+      <c r="C689" s="61"/>
+      <c r="D689" s="63"/>
     </row>
     <row r="690" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A690" s="56"/>
-      <c r="B690" s="57"/>
-      <c r="C690" s="57"/>
-      <c r="D690" s="58"/>
+      <c r="A690" s="60"/>
+      <c r="B690" s="61"/>
+      <c r="C690" s="61"/>
+      <c r="D690" s="63"/>
     </row>
     <row r="691" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A691" s="56"/>
-      <c r="B691" s="57"/>
-      <c r="C691" s="57"/>
-      <c r="D691" s="58"/>
+      <c r="A691" s="60"/>
+      <c r="B691" s="61"/>
+      <c r="C691" s="61"/>
+      <c r="D691" s="63"/>
     </row>
     <row r="692" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A692" s="56"/>
-      <c r="B692" s="57"/>
-      <c r="C692" s="57"/>
-      <c r="D692" s="58"/>
+      <c r="A692" s="60"/>
+      <c r="B692" s="61"/>
+      <c r="C692" s="61"/>
+      <c r="D692" s="63"/>
     </row>
     <row r="693" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A693" s="56"/>
-      <c r="B693" s="57"/>
-      <c r="C693" s="57"/>
-      <c r="D693" s="58"/>
+      <c r="A693" s="60"/>
+      <c r="B693" s="61"/>
+      <c r="C693" s="61"/>
+      <c r="D693" s="63"/>
     </row>
     <row r="694" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A694" s="56"/>
-      <c r="B694" s="57"/>
-      <c r="C694" s="57"/>
-      <c r="D694" s="58"/>
+      <c r="A694" s="60"/>
+      <c r="B694" s="61"/>
+      <c r="C694" s="61"/>
+      <c r="D694" s="63"/>
     </row>
     <row r="695" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A695" s="56"/>
-      <c r="B695" s="57"/>
-      <c r="C695" s="57"/>
-      <c r="D695" s="58"/>
+      <c r="A695" s="60"/>
+      <c r="B695" s="61"/>
+      <c r="C695" s="61"/>
+      <c r="D695" s="63"/>
     </row>
     <row r="696" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A696" s="56"/>
-      <c r="B696" s="57"/>
-      <c r="C696" s="57"/>
-      <c r="D696" s="58"/>
+      <c r="A696" s="60"/>
+      <c r="B696" s="61"/>
+      <c r="C696" s="61"/>
+      <c r="D696" s="63"/>
     </row>
     <row r="697" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A697" s="56"/>
-      <c r="B697" s="57"/>
-      <c r="C697" s="57"/>
-      <c r="D697" s="58"/>
+      <c r="A697" s="60"/>
+      <c r="B697" s="61"/>
+      <c r="C697" s="61"/>
+      <c r="D697" s="63"/>
     </row>
     <row r="698" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A698" s="56"/>
-      <c r="B698" s="57"/>
-      <c r="C698" s="57"/>
-      <c r="D698" s="58"/>
+      <c r="A698" s="60"/>
+      <c r="B698" s="61"/>
+      <c r="C698" s="61"/>
+      <c r="D698" s="63"/>
     </row>
     <row r="699" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A699" s="56"/>
-      <c r="B699" s="57"/>
-      <c r="C699" s="57"/>
-      <c r="D699" s="58"/>
+      <c r="A699" s="60"/>
+      <c r="B699" s="61"/>
+      <c r="C699" s="61"/>
+      <c r="D699" s="63"/>
     </row>
     <row r="700" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A700" s="56"/>
-      <c r="B700" s="57"/>
-      <c r="C700" s="57"/>
-      <c r="D700" s="58"/>
+      <c r="A700" s="60"/>
+      <c r="B700" s="61"/>
+      <c r="C700" s="61"/>
+      <c r="D700" s="63"/>
     </row>
     <row r="701" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A701" s="56"/>
-      <c r="B701" s="57"/>
-      <c r="C701" s="57"/>
-      <c r="D701" s="58"/>
+      <c r="A701" s="60"/>
+      <c r="B701" s="61"/>
+      <c r="C701" s="61"/>
+      <c r="D701" s="63"/>
     </row>
     <row r="702" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A702" s="56"/>
-      <c r="B702" s="57"/>
-      <c r="C702" s="57"/>
-      <c r="D702" s="58"/>
+      <c r="A702" s="60"/>
+      <c r="B702" s="61"/>
+      <c r="C702" s="61"/>
+      <c r="D702" s="63"/>
     </row>
     <row r="703" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A703" s="56"/>
-      <c r="B703" s="57"/>
-      <c r="C703" s="57"/>
-      <c r="D703" s="58"/>
+      <c r="A703" s="60"/>
+      <c r="B703" s="61"/>
+      <c r="C703" s="61"/>
+      <c r="D703" s="63"/>
     </row>
     <row r="704" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A704" s="56"/>
-      <c r="B704" s="57"/>
-      <c r="C704" s="57"/>
-      <c r="D704" s="58"/>
+      <c r="A704" s="60"/>
+      <c r="B704" s="61"/>
+      <c r="C704" s="61"/>
+      <c r="D704" s="63"/>
     </row>
     <row r="705" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A705" s="56"/>
-      <c r="B705" s="57"/>
-      <c r="C705" s="57"/>
-      <c r="D705" s="58"/>
+      <c r="A705" s="60"/>
+      <c r="B705" s="61"/>
+      <c r="C705" s="61"/>
+      <c r="D705" s="63"/>
     </row>
     <row r="706" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A706" s="56"/>
-      <c r="B706" s="57"/>
-      <c r="C706" s="57"/>
-      <c r="D706" s="58"/>
+      <c r="A706" s="60"/>
+      <c r="B706" s="61"/>
+      <c r="C706" s="61"/>
+      <c r="D706" s="63"/>
     </row>
     <row r="707" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A707" s="56"/>
-      <c r="B707" s="57"/>
-      <c r="C707" s="57"/>
-      <c r="D707" s="58"/>
+      <c r="A707" s="60"/>
+      <c r="B707" s="61"/>
+      <c r="C707" s="61"/>
+      <c r="D707" s="63"/>
     </row>
     <row r="708" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A708" s="56"/>
-      <c r="B708" s="57"/>
-      <c r="C708" s="57"/>
-      <c r="D708" s="58"/>
+      <c r="A708" s="60"/>
+      <c r="B708" s="61"/>
+      <c r="C708" s="61"/>
+      <c r="D708" s="63"/>
     </row>
     <row r="709" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A709" s="56"/>
-      <c r="B709" s="57"/>
-      <c r="C709" s="57"/>
-      <c r="D709" s="58"/>
+      <c r="A709" s="60"/>
+      <c r="B709" s="61"/>
+      <c r="C709" s="61"/>
+      <c r="D709" s="63"/>
     </row>
     <row r="710" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A710" s="56"/>
-      <c r="B710" s="57"/>
-      <c r="C710" s="57"/>
-      <c r="D710" s="58"/>
+      <c r="A710" s="60"/>
+      <c r="B710" s="61"/>
+      <c r="C710" s="61"/>
+      <c r="D710" s="63"/>
     </row>
     <row r="711" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A711" s="56"/>
-      <c r="B711" s="57"/>
-      <c r="C711" s="57"/>
-      <c r="D711" s="58"/>
+      <c r="A711" s="60"/>
+      <c r="B711" s="61"/>
+      <c r="C711" s="61"/>
+      <c r="D711" s="63"/>
     </row>
     <row r="712" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A712" s="56"/>
-      <c r="B712" s="57"/>
-      <c r="C712" s="57"/>
-      <c r="D712" s="58"/>
+      <c r="A712" s="60"/>
+      <c r="B712" s="61"/>
+      <c r="C712" s="61"/>
+      <c r="D712" s="63"/>
     </row>
     <row r="713" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A713" s="56"/>
-      <c r="B713" s="57"/>
-      <c r="C713" s="57"/>
-      <c r="D713" s="58"/>
+      <c r="A713" s="60"/>
+      <c r="B713" s="61"/>
+      <c r="C713" s="61"/>
+      <c r="D713" s="63"/>
     </row>
     <row r="714" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A714" s="56"/>
-      <c r="B714" s="57"/>
-      <c r="C714" s="57"/>
-      <c r="D714" s="58"/>
+      <c r="A714" s="60"/>
+      <c r="B714" s="61"/>
+      <c r="C714" s="61"/>
+      <c r="D714" s="63"/>
     </row>
     <row r="715" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A715" s="56"/>
-      <c r="B715" s="57"/>
-      <c r="C715" s="57"/>
-      <c r="D715" s="58"/>
+      <c r="A715" s="60"/>
+      <c r="B715" s="61"/>
+      <c r="C715" s="61"/>
+      <c r="D715" s="63"/>
     </row>
     <row r="716" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A716" s="56"/>
-      <c r="B716" s="57"/>
-      <c r="C716" s="57"/>
-      <c r="D716" s="58"/>
+      <c r="A716" s="60"/>
+      <c r="B716" s="61"/>
+      <c r="C716" s="61"/>
+      <c r="D716" s="63"/>
     </row>
     <row r="717" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A717" s="56"/>
-      <c r="B717" s="57"/>
-      <c r="C717" s="57"/>
-      <c r="D717" s="58"/>
+      <c r="A717" s="60"/>
+      <c r="B717" s="61"/>
+      <c r="C717" s="61"/>
+      <c r="D717" s="63"/>
     </row>
     <row r="718" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A718" s="56"/>
-      <c r="B718" s="57"/>
-      <c r="C718" s="57"/>
-      <c r="D718" s="58"/>
+      <c r="A718" s="60"/>
+      <c r="B718" s="61"/>
+      <c r="C718" s="61"/>
+      <c r="D718" s="63"/>
     </row>
     <row r="719" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A719" s="56"/>
-      <c r="B719" s="57"/>
-      <c r="C719" s="57"/>
-      <c r="D719" s="58"/>
+      <c r="A719" s="60"/>
+      <c r="B719" s="61"/>
+      <c r="C719" s="61"/>
+      <c r="D719" s="63"/>
     </row>
     <row r="720" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A720" s="56"/>
-      <c r="B720" s="57"/>
-      <c r="C720" s="57"/>
-      <c r="D720" s="58"/>
+      <c r="A720" s="60"/>
+      <c r="B720" s="61"/>
+      <c r="C720" s="61"/>
+      <c r="D720" s="63"/>
     </row>
     <row r="721" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A721" s="56"/>
-      <c r="B721" s="57"/>
-      <c r="C721" s="57"/>
-      <c r="D721" s="58"/>
+      <c r="A721" s="60"/>
+      <c r="B721" s="61"/>
+      <c r="C721" s="61"/>
+      <c r="D721" s="63"/>
     </row>
     <row r="722" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A722" s="56"/>
-      <c r="B722" s="57"/>
-      <c r="C722" s="57"/>
-      <c r="D722" s="58"/>
+      <c r="A722" s="60"/>
+      <c r="B722" s="61"/>
+      <c r="C722" s="61"/>
+      <c r="D722" s="63"/>
     </row>
     <row r="723" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A723" s="56"/>
-      <c r="B723" s="57"/>
-      <c r="C723" s="57"/>
-      <c r="D723" s="58"/>
+      <c r="A723" s="60"/>
+      <c r="B723" s="61"/>
+      <c r="C723" s="61"/>
+      <c r="D723" s="63"/>
     </row>
     <row r="724" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A724" s="56"/>
-      <c r="B724" s="57"/>
-      <c r="C724" s="57"/>
-      <c r="D724" s="58"/>
+      <c r="A724" s="60"/>
+      <c r="B724" s="61"/>
+      <c r="C724" s="61"/>
+      <c r="D724" s="63"/>
     </row>
     <row r="725" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A725" s="56"/>
-      <c r="B725" s="57"/>
-      <c r="C725" s="57"/>
-      <c r="D725" s="58"/>
+      <c r="A725" s="60"/>
+      <c r="B725" s="61"/>
+      <c r="C725" s="61"/>
+      <c r="D725" s="63"/>
     </row>
     <row r="726" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A726" s="56"/>
-      <c r="B726" s="57"/>
-      <c r="C726" s="57"/>
-      <c r="D726" s="58"/>
+      <c r="A726" s="60"/>
+      <c r="B726" s="61"/>
+      <c r="C726" s="61"/>
+      <c r="D726" s="63"/>
     </row>
     <row r="727" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A727" s="56"/>
-      <c r="B727" s="57"/>
-      <c r="C727" s="57"/>
-      <c r="D727" s="58"/>
+      <c r="A727" s="60"/>
+      <c r="B727" s="61"/>
+      <c r="C727" s="61"/>
+      <c r="D727" s="63"/>
     </row>
     <row r="728" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A728" s="56"/>
-      <c r="B728" s="57"/>
-      <c r="C728" s="57"/>
-      <c r="D728" s="58"/>
+      <c r="A728" s="60"/>
+      <c r="B728" s="61"/>
+      <c r="C728" s="61"/>
+      <c r="D728" s="63"/>
     </row>
     <row r="729" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A729" s="56"/>
-      <c r="B729" s="57"/>
-      <c r="C729" s="57"/>
-      <c r="D729" s="58"/>
+      <c r="A729" s="60"/>
+      <c r="B729" s="61"/>
+      <c r="C729" s="61"/>
+      <c r="D729" s="63"/>
     </row>
     <row r="730" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A730" s="56"/>
-      <c r="B730" s="57"/>
-      <c r="C730" s="57"/>
-      <c r="D730" s="58"/>
+      <c r="A730" s="60"/>
+      <c r="B730" s="61"/>
+      <c r="C730" s="61"/>
+      <c r="D730" s="63"/>
     </row>
     <row r="731" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A731" s="56"/>
-      <c r="B731" s="57"/>
-      <c r="C731" s="57"/>
-      <c r="D731" s="58"/>
+      <c r="A731" s="60"/>
+      <c r="B731" s="61"/>
+      <c r="C731" s="61"/>
+      <c r="D731" s="63"/>
     </row>
     <row r="732" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A732" s="56"/>
-      <c r="B732" s="57"/>
-      <c r="C732" s="57"/>
-      <c r="D732" s="58"/>
+      <c r="A732" s="60"/>
+      <c r="B732" s="61"/>
+      <c r="C732" s="61"/>
+      <c r="D732" s="63"/>
     </row>
     <row r="733" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A733" s="56"/>
-      <c r="B733" s="57"/>
-      <c r="C733" s="57"/>
-      <c r="D733" s="58"/>
+      <c r="A733" s="60"/>
+      <c r="B733" s="61"/>
+      <c r="C733" s="61"/>
+      <c r="D733" s="63"/>
     </row>
     <row r="734" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A734" s="56"/>
-      <c r="B734" s="57"/>
-      <c r="C734" s="57"/>
-      <c r="D734" s="58"/>
+      <c r="A734" s="60"/>
+      <c r="B734" s="61"/>
+      <c r="C734" s="61"/>
+      <c r="D734" s="63"/>
     </row>
     <row r="735" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A735" s="56"/>
-      <c r="B735" s="57"/>
-      <c r="C735" s="57"/>
-      <c r="D735" s="58"/>
+      <c r="A735" s="60"/>
+      <c r="B735" s="61"/>
+      <c r="C735" s="61"/>
+      <c r="D735" s="63"/>
     </row>
     <row r="736" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A736" s="56"/>
-      <c r="B736" s="57"/>
-      <c r="C736" s="57"/>
-      <c r="D736" s="58"/>
+      <c r="A736" s="60"/>
+      <c r="B736" s="61"/>
+      <c r="C736" s="61"/>
+      <c r="D736" s="63"/>
     </row>
     <row r="737" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A737" s="56"/>
-      <c r="B737" s="57"/>
-      <c r="C737" s="57"/>
-      <c r="D737" s="58"/>
+      <c r="A737" s="60"/>
+      <c r="B737" s="61"/>
+      <c r="C737" s="61"/>
+      <c r="D737" s="63"/>
     </row>
     <row r="738" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A738" s="56"/>
-      <c r="B738" s="57"/>
-      <c r="C738" s="57"/>
-      <c r="D738" s="58"/>
+      <c r="A738" s="60"/>
+      <c r="B738" s="61"/>
+      <c r="C738" s="61"/>
+      <c r="D738" s="63"/>
     </row>
     <row r="739" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A739" s="56"/>
-      <c r="B739" s="57"/>
-      <c r="C739" s="57"/>
-      <c r="D739" s="58"/>
+      <c r="A739" s="60"/>
+      <c r="B739" s="61"/>
+      <c r="C739" s="61"/>
+      <c r="D739" s="63"/>
     </row>
     <row r="740" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A740" s="56"/>
-      <c r="B740" s="57"/>
-      <c r="C740" s="57"/>
-      <c r="D740" s="58"/>
+      <c r="A740" s="60"/>
+      <c r="B740" s="61"/>
+      <c r="C740" s="61"/>
+      <c r="D740" s="63"/>
     </row>
     <row r="741" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A741" s="56"/>
-      <c r="B741" s="57"/>
-      <c r="C741" s="57"/>
-      <c r="D741" s="58"/>
+      <c r="A741" s="60"/>
+      <c r="B741" s="61"/>
+      <c r="C741" s="61"/>
+      <c r="D741" s="63"/>
     </row>
     <row r="742" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A742" s="56"/>
-      <c r="B742" s="57"/>
-      <c r="C742" s="57"/>
-      <c r="D742" s="58"/>
+      <c r="A742" s="60"/>
+      <c r="B742" s="61"/>
+      <c r="C742" s="61"/>
+      <c r="D742" s="63"/>
     </row>
     <row r="743" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A743" s="56"/>
-      <c r="B743" s="57"/>
-      <c r="C743" s="57"/>
-      <c r="D743" s="58"/>
+      <c r="A743" s="60"/>
+      <c r="B743" s="61"/>
+      <c r="C743" s="61"/>
+      <c r="D743" s="63"/>
     </row>
     <row r="744" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A744" s="56"/>
-      <c r="B744" s="57"/>
-      <c r="C744" s="57"/>
-      <c r="D744" s="58"/>
+      <c r="A744" s="60"/>
+      <c r="B744" s="61"/>
+      <c r="C744" s="61"/>
+      <c r="D744" s="63"/>
     </row>
     <row r="745" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A745" s="56"/>
-      <c r="B745" s="57"/>
-      <c r="C745" s="57"/>
-      <c r="D745" s="58"/>
+      <c r="A745" s="60"/>
+      <c r="B745" s="61"/>
+      <c r="C745" s="61"/>
+      <c r="D745" s="63"/>
     </row>
     <row r="746" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A746" s="56"/>
-      <c r="B746" s="57"/>
-      <c r="C746" s="57"/>
-      <c r="D746" s="58"/>
+      <c r="A746" s="60"/>
+      <c r="B746" s="61"/>
+      <c r="C746" s="61"/>
+      <c r="D746" s="63"/>
     </row>
     <row r="747" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A747" s="56"/>
-      <c r="B747" s="57"/>
-      <c r="C747" s="57"/>
-      <c r="D747" s="58"/>
+      <c r="A747" s="60"/>
+      <c r="B747" s="61"/>
+      <c r="C747" s="61"/>
+      <c r="D747" s="63"/>
     </row>
     <row r="748" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A748" s="56"/>
-      <c r="B748" s="57"/>
-      <c r="C748" s="57"/>
-      <c r="D748" s="58"/>
+      <c r="A748" s="60"/>
+      <c r="B748" s="61"/>
+      <c r="C748" s="61"/>
+      <c r="D748" s="63"/>
     </row>
     <row r="749" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A749" s="56"/>
-      <c r="B749" s="57"/>
-      <c r="C749" s="57"/>
-      <c r="D749" s="58"/>
+      <c r="A749" s="60"/>
+      <c r="B749" s="61"/>
+      <c r="C749" s="61"/>
+      <c r="D749" s="63"/>
     </row>
     <row r="750" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A750" s="56"/>
-      <c r="B750" s="57"/>
-      <c r="C750" s="57"/>
-      <c r="D750" s="58"/>
+      <c r="A750" s="60"/>
+      <c r="B750" s="61"/>
+      <c r="C750" s="61"/>
+      <c r="D750" s="63"/>
     </row>
     <row r="751" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A751" s="56"/>
-      <c r="B751" s="57"/>
-      <c r="C751" s="57"/>
-      <c r="D751" s="58"/>
+      <c r="A751" s="60"/>
+      <c r="B751" s="61"/>
+      <c r="C751" s="61"/>
+      <c r="D751" s="63"/>
     </row>
     <row r="752" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A752" s="56"/>
-      <c r="B752" s="57"/>
-      <c r="C752" s="57"/>
-      <c r="D752" s="58"/>
+      <c r="A752" s="60"/>
+      <c r="B752" s="61"/>
+      <c r="C752" s="61"/>
+      <c r="D752" s="63"/>
     </row>
     <row r="753" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A753" s="56"/>
-      <c r="B753" s="57"/>
-      <c r="C753" s="57"/>
-      <c r="D753" s="58"/>
+      <c r="A753" s="60"/>
+      <c r="B753" s="61"/>
+      <c r="C753" s="61"/>
+      <c r="D753" s="63"/>
     </row>
     <row r="754" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A754" s="56"/>
-      <c r="B754" s="57"/>
-      <c r="C754" s="57"/>
-      <c r="D754" s="58"/>
+      <c r="A754" s="60"/>
+      <c r="B754" s="61"/>
+      <c r="C754" s="61"/>
+      <c r="D754" s="63"/>
     </row>
     <row r="755" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A755" s="56"/>
-      <c r="B755" s="57"/>
-      <c r="C755" s="57"/>
-      <c r="D755" s="58"/>
+      <c r="A755" s="60"/>
+      <c r="B755" s="61"/>
+      <c r="C755" s="61"/>
+      <c r="D755" s="63"/>
     </row>
     <row r="756" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A756" s="56"/>
-      <c r="B756" s="57"/>
-      <c r="C756" s="57"/>
-      <c r="D756" s="58"/>
+      <c r="A756" s="60"/>
+      <c r="B756" s="61"/>
+      <c r="C756" s="61"/>
+      <c r="D756" s="63"/>
     </row>
     <row r="757" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A757" s="56"/>
-      <c r="B757" s="57"/>
-      <c r="C757" s="57"/>
-      <c r="D757" s="58"/>
+      <c r="A757" s="60"/>
+      <c r="B757" s="61"/>
+      <c r="C757" s="61"/>
+      <c r="D757" s="63"/>
     </row>
     <row r="758" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A758" s="56"/>
-      <c r="B758" s="57"/>
-      <c r="C758" s="57"/>
-      <c r="D758" s="58"/>
+      <c r="A758" s="60"/>
+      <c r="B758" s="61"/>
+      <c r="C758" s="61"/>
+      <c r="D758" s="63"/>
     </row>
     <row r="759" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A759" s="56"/>
-      <c r="B759" s="57"/>
-      <c r="C759" s="57"/>
-      <c r="D759" s="58"/>
+      <c r="A759" s="60"/>
+      <c r="B759" s="61"/>
+      <c r="C759" s="61"/>
+      <c r="D759" s="63"/>
     </row>
     <row r="760" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A760" s="56"/>
-      <c r="B760" s="57"/>
-      <c r="C760" s="57"/>
-      <c r="D760" s="58"/>
+      <c r="A760" s="60"/>
+      <c r="B760" s="61"/>
+      <c r="C760" s="61"/>
+      <c r="D760" s="63"/>
     </row>
     <row r="761" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A761" s="56"/>
-      <c r="B761" s="57"/>
-      <c r="C761" s="57"/>
-      <c r="D761" s="58"/>
+      <c r="A761" s="60"/>
+      <c r="B761" s="61"/>
+      <c r="C761" s="61"/>
+      <c r="D761" s="63"/>
     </row>
     <row r="762" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A762" s="56"/>
-      <c r="B762" s="57"/>
-      <c r="C762" s="57"/>
-      <c r="D762" s="58"/>
+      <c r="A762" s="60"/>
+      <c r="B762" s="61"/>
+      <c r="C762" s="61"/>
+      <c r="D762" s="63"/>
     </row>
     <row r="763" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A763" s="56"/>
-      <c r="B763" s="57"/>
-      <c r="C763" s="57"/>
-      <c r="D763" s="58"/>
+      <c r="A763" s="60"/>
+      <c r="B763" s="61"/>
+      <c r="C763" s="61"/>
+      <c r="D763" s="63"/>
     </row>
     <row r="764" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A764" s="56"/>
-      <c r="B764" s="57"/>
-      <c r="C764" s="57"/>
-      <c r="D764" s="58"/>
+      <c r="A764" s="60"/>
+      <c r="B764" s="61"/>
+      <c r="C764" s="61"/>
+      <c r="D764" s="63"/>
     </row>
     <row r="765" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A765" s="56"/>
-      <c r="B765" s="57"/>
-      <c r="C765" s="57"/>
-      <c r="D765" s="58"/>
+      <c r="A765" s="60"/>
+      <c r="B765" s="61"/>
+      <c r="C765" s="61"/>
+      <c r="D765" s="63"/>
     </row>
     <row r="766" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A766" s="56"/>
-      <c r="B766" s="57"/>
-      <c r="C766" s="57"/>
-      <c r="D766" s="58"/>
+      <c r="A766" s="60"/>
+      <c r="B766" s="61"/>
+      <c r="C766" s="61"/>
+      <c r="D766" s="63"/>
     </row>
     <row r="767" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A767" s="56"/>
-      <c r="B767" s="57"/>
-      <c r="C767" s="57"/>
-      <c r="D767" s="58"/>
+      <c r="A767" s="60"/>
+      <c r="B767" s="61"/>
+      <c r="C767" s="61"/>
+      <c r="D767" s="63"/>
     </row>
     <row r="768" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A768" s="56"/>
-      <c r="B768" s="57"/>
-      <c r="C768" s="57"/>
-      <c r="D768" s="58"/>
+      <c r="A768" s="60"/>
+      <c r="B768" s="61"/>
+      <c r="C768" s="61"/>
+      <c r="D768" s="63"/>
     </row>
     <row r="769" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A769" s="56"/>
-      <c r="B769" s="57"/>
-      <c r="C769" s="57"/>
-      <c r="D769" s="58"/>
+      <c r="A769" s="60"/>
+      <c r="B769" s="61"/>
+      <c r="C769" s="61"/>
+      <c r="D769" s="63"/>
     </row>
     <row r="770" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A770" s="56"/>
-      <c r="B770" s="57"/>
-      <c r="C770" s="57"/>
-      <c r="D770" s="58"/>
+      <c r="A770" s="60"/>
+      <c r="B770" s="61"/>
+      <c r="C770" s="61"/>
+      <c r="D770" s="63"/>
     </row>
     <row r="771" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A771" s="56"/>
-      <c r="B771" s="57"/>
-      <c r="C771" s="57"/>
-      <c r="D771" s="58"/>
+      <c r="A771" s="60"/>
+      <c r="B771" s="61"/>
+      <c r="C771" s="61"/>
+      <c r="D771" s="63"/>
     </row>
     <row r="772" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A772" s="56"/>
-      <c r="B772" s="57"/>
-      <c r="C772" s="57"/>
-      <c r="D772" s="58"/>
+      <c r="A772" s="60"/>
+      <c r="B772" s="61"/>
+      <c r="C772" s="61"/>
+      <c r="D772" s="63"/>
     </row>
     <row r="773" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A773" s="56"/>
-      <c r="B773" s="57"/>
-      <c r="C773" s="57"/>
-      <c r="D773" s="58"/>
+      <c r="A773" s="60"/>
+      <c r="B773" s="61"/>
+      <c r="C773" s="61"/>
+      <c r="D773" s="63"/>
     </row>
     <row r="774" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A774" s="56"/>
-      <c r="B774" s="57"/>
-      <c r="C774" s="57"/>
-      <c r="D774" s="58"/>
+      <c r="A774" s="60"/>
+      <c r="B774" s="61"/>
+      <c r="C774" s="61"/>
+      <c r="D774" s="63"/>
     </row>
     <row r="775" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A775" s="56"/>
-      <c r="B775" s="57"/>
-      <c r="C775" s="57"/>
-      <c r="D775" s="58"/>
+      <c r="A775" s="60"/>
+      <c r="B775" s="61"/>
+      <c r="C775" s="61"/>
+      <c r="D775" s="63"/>
     </row>
     <row r="776" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A776" s="56"/>
-      <c r="B776" s="57"/>
-      <c r="C776" s="57"/>
-      <c r="D776" s="58"/>
+      <c r="A776" s="60"/>
+      <c r="B776" s="61"/>
+      <c r="C776" s="61"/>
+      <c r="D776" s="63"/>
     </row>
     <row r="777" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A777" s="56"/>
-      <c r="B777" s="57"/>
-      <c r="C777" s="57"/>
-      <c r="D777" s="58"/>
+      <c r="A777" s="60"/>
+      <c r="B777" s="61"/>
+      <c r="C777" s="61"/>
+      <c r="D777" s="63"/>
     </row>
     <row r="778" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A778" s="56"/>
-      <c r="B778" s="57"/>
-      <c r="C778" s="57"/>
-      <c r="D778" s="58"/>
+      <c r="A778" s="60"/>
+      <c r="B778" s="61"/>
+      <c r="C778" s="61"/>
+      <c r="D778" s="63"/>
     </row>
     <row r="779" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A779" s="56"/>
-      <c r="B779" s="57"/>
-      <c r="C779" s="57"/>
-      <c r="D779" s="58"/>
+      <c r="A779" s="60"/>
+      <c r="B779" s="61"/>
+      <c r="C779" s="61"/>
+      <c r="D779" s="63"/>
     </row>
     <row r="780" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A780" s="56"/>
-      <c r="B780" s="57"/>
-      <c r="C780" s="57"/>
-      <c r="D780" s="58"/>
+      <c r="A780" s="60"/>
+      <c r="B780" s="61"/>
+      <c r="C780" s="61"/>
+      <c r="D780" s="63"/>
     </row>
     <row r="781" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A781" s="56"/>
-      <c r="B781" s="57"/>
-      <c r="C781" s="57"/>
-      <c r="D781" s="58"/>
+      <c r="A781" s="60"/>
+      <c r="B781" s="61"/>
+      <c r="C781" s="61"/>
+      <c r="D781" s="63"/>
     </row>
     <row r="782" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A782" s="56"/>
-      <c r="B782" s="57"/>
-      <c r="C782" s="57"/>
-      <c r="D782" s="58"/>
+      <c r="A782" s="60"/>
+      <c r="B782" s="61"/>
+      <c r="C782" s="61"/>
+      <c r="D782" s="63"/>
     </row>
     <row r="783" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A783" s="56"/>
-      <c r="B783" s="57"/>
-      <c r="C783" s="57"/>
-      <c r="D783" s="58"/>
+      <c r="A783" s="60"/>
+      <c r="B783" s="61"/>
+      <c r="C783" s="61"/>
+      <c r="D783" s="63"/>
     </row>
     <row r="784" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A784" s="56"/>
-      <c r="B784" s="57"/>
-      <c r="C784" s="57"/>
-      <c r="D784" s="58"/>
+      <c r="A784" s="60"/>
+      <c r="B784" s="61"/>
+      <c r="C784" s="61"/>
+      <c r="D784" s="63"/>
     </row>
     <row r="785" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A785" s="56"/>
-      <c r="B785" s="57"/>
-      <c r="C785" s="57"/>
-      <c r="D785" s="58"/>
+      <c r="A785" s="60"/>
+      <c r="B785" s="61"/>
+      <c r="C785" s="61"/>
+      <c r="D785" s="63"/>
     </row>
     <row r="786" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A786" s="56"/>
-      <c r="B786" s="57"/>
-      <c r="C786" s="57"/>
-      <c r="D786" s="58"/>
+      <c r="A786" s="60"/>
+      <c r="B786" s="61"/>
+      <c r="C786" s="61"/>
+      <c r="D786" s="63"/>
     </row>
     <row r="787" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A787" s="56"/>
-      <c r="B787" s="57"/>
-      <c r="C787" s="57"/>
-      <c r="D787" s="58"/>
+      <c r="A787" s="60"/>
+      <c r="B787" s="61"/>
+      <c r="C787" s="61"/>
+      <c r="D787" s="63"/>
     </row>
     <row r="788" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A788" s="56"/>
-      <c r="B788" s="57"/>
-      <c r="C788" s="57"/>
-      <c r="D788" s="58"/>
+      <c r="A788" s="60"/>
+      <c r="B788" s="61"/>
+      <c r="C788" s="61"/>
+      <c r="D788" s="63"/>
     </row>
     <row r="789" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A789" s="56"/>
-      <c r="B789" s="57"/>
-      <c r="C789" s="57"/>
-      <c r="D789" s="58"/>
+      <c r="A789" s="60"/>
+      <c r="B789" s="61"/>
+      <c r="C789" s="61"/>
+      <c r="D789" s="63"/>
     </row>
     <row r="790" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A790" s="56"/>
-      <c r="B790" s="57"/>
-      <c r="C790" s="57"/>
-      <c r="D790" s="58"/>
+      <c r="A790" s="60"/>
+      <c r="B790" s="61"/>
+      <c r="C790" s="61"/>
+      <c r="D790" s="63"/>
     </row>
     <row r="791" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A791" s="56"/>
-      <c r="B791" s="57"/>
-      <c r="C791" s="57"/>
-      <c r="D791" s="58"/>
+      <c r="A791" s="60"/>
+      <c r="B791" s="61"/>
+      <c r="C791" s="61"/>
+      <c r="D791" s="63"/>
     </row>
     <row r="792" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A792" s="56"/>
-      <c r="B792" s="57"/>
-      <c r="C792" s="57"/>
-      <c r="D792" s="58"/>
+      <c r="A792" s="60"/>
+      <c r="B792" s="61"/>
+      <c r="C792" s="61"/>
+      <c r="D792" s="63"/>
     </row>
     <row r="793" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A793" s="56"/>
-      <c r="B793" s="57"/>
-      <c r="C793" s="57"/>
-      <c r="D793" s="58"/>
+      <c r="A793" s="60"/>
+      <c r="B793" s="61"/>
+      <c r="C793" s="61"/>
+      <c r="D793" s="63"/>
     </row>
     <row r="794" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A794" s="56"/>
-      <c r="B794" s="57"/>
-      <c r="C794" s="57"/>
-      <c r="D794" s="58"/>
+      <c r="A794" s="60"/>
+      <c r="B794" s="61"/>
+      <c r="C794" s="61"/>
+      <c r="D794" s="63"/>
     </row>
     <row r="795" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A795" s="56"/>
-      <c r="B795" s="57"/>
-      <c r="C795" s="57"/>
-      <c r="D795" s="58"/>
+      <c r="A795" s="60"/>
+      <c r="B795" s="61"/>
+      <c r="C795" s="61"/>
+      <c r="D795" s="63"/>
     </row>
     <row r="796" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A796" s="56"/>
-      <c r="B796" s="57"/>
-      <c r="C796" s="57"/>
-      <c r="D796" s="58"/>
+      <c r="A796" s="60"/>
+      <c r="B796" s="61"/>
+      <c r="C796" s="61"/>
+      <c r="D796" s="63"/>
     </row>
     <row r="797" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A797" s="56"/>
-      <c r="B797" s="57"/>
-      <c r="C797" s="57"/>
-      <c r="D797" s="58"/>
+      <c r="A797" s="60"/>
+      <c r="B797" s="61"/>
+      <c r="C797" s="61"/>
+      <c r="D797" s="63"/>
     </row>
     <row r="798" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A798" s="56"/>
-      <c r="B798" s="57"/>
-      <c r="C798" s="57"/>
-      <c r="D798" s="58"/>
+      <c r="A798" s="60"/>
+      <c r="B798" s="61"/>
+      <c r="C798" s="61"/>
+      <c r="D798" s="63"/>
     </row>
     <row r="799" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A799" s="56"/>
-      <c r="B799" s="57"/>
-      <c r="C799" s="57"/>
-      <c r="D799" s="58"/>
+      <c r="A799" s="60"/>
+      <c r="B799" s="61"/>
+      <c r="C799" s="61"/>
+      <c r="D799" s="63"/>
     </row>
     <row r="800" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A800" s="56"/>
-      <c r="B800" s="57"/>
-      <c r="C800" s="57"/>
-      <c r="D800" s="58"/>
+      <c r="A800" s="60"/>
+      <c r="B800" s="61"/>
+      <c r="C800" s="61"/>
+      <c r="D800" s="63"/>
     </row>
     <row r="801" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A801" s="56"/>
-      <c r="B801" s="57"/>
-      <c r="C801" s="57"/>
-      <c r="D801" s="58"/>
+      <c r="A801" s="60"/>
+      <c r="B801" s="61"/>
+      <c r="C801" s="61"/>
+      <c r="D801" s="63"/>
     </row>
     <row r="802" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A802" s="56"/>
-      <c r="B802" s="57"/>
-      <c r="C802" s="57"/>
-      <c r="D802" s="58"/>
+      <c r="A802" s="60"/>
+      <c r="B802" s="61"/>
+      <c r="C802" s="61"/>
+      <c r="D802" s="63"/>
     </row>
     <row r="803" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A803" s="56"/>
-      <c r="B803" s="57"/>
-      <c r="C803" s="57"/>
-      <c r="D803" s="58"/>
+      <c r="A803" s="60"/>
+      <c r="B803" s="61"/>
+      <c r="C803" s="61"/>
+      <c r="D803" s="63"/>
     </row>
     <row r="804" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A804" s="56"/>
-      <c r="B804" s="57"/>
-      <c r="C804" s="57"/>
-      <c r="D804" s="58"/>
+      <c r="A804" s="60"/>
+      <c r="B804" s="61"/>
+      <c r="C804" s="61"/>
+      <c r="D804" s="63"/>
     </row>
     <row r="805" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A805" s="56"/>
-      <c r="B805" s="57"/>
-      <c r="C805" s="57"/>
-      <c r="D805" s="58"/>
+      <c r="A805" s="60"/>
+      <c r="B805" s="61"/>
+      <c r="C805" s="61"/>
+      <c r="D805" s="63"/>
     </row>
     <row r="806" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A806" s="56"/>
-      <c r="B806" s="57"/>
-      <c r="C806" s="57"/>
-      <c r="D806" s="58"/>
+      <c r="A806" s="60"/>
+      <c r="B806" s="61"/>
+      <c r="C806" s="61"/>
+      <c r="D806" s="63"/>
     </row>
     <row r="807" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A807" s="56"/>
-      <c r="B807" s="57"/>
-      <c r="C807" s="57"/>
-      <c r="D807" s="58"/>
+      <c r="A807" s="60"/>
+      <c r="B807" s="61"/>
+      <c r="C807" s="61"/>
+      <c r="D807" s="63"/>
     </row>
     <row r="808" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A808" s="56"/>
-      <c r="B808" s="57"/>
-      <c r="C808" s="57"/>
-      <c r="D808" s="58"/>
+      <c r="A808" s="60"/>
+      <c r="B808" s="61"/>
+      <c r="C808" s="61"/>
+      <c r="D808" s="63"/>
     </row>
     <row r="809" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A809" s="56"/>
-      <c r="B809" s="57"/>
-      <c r="C809" s="57"/>
-      <c r="D809" s="58"/>
+      <c r="A809" s="60"/>
+      <c r="B809" s="61"/>
+      <c r="C809" s="61"/>
+      <c r="D809" s="63"/>
     </row>
     <row r="810" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A810" s="56"/>
-      <c r="B810" s="57"/>
-      <c r="C810" s="57"/>
-      <c r="D810" s="58"/>
+      <c r="A810" s="60"/>
+      <c r="B810" s="61"/>
+      <c r="C810" s="61"/>
+      <c r="D810" s="63"/>
     </row>
     <row r="811" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A811" s="56"/>
-      <c r="B811" s="57"/>
-      <c r="C811" s="57"/>
-      <c r="D811" s="58"/>
+      <c r="A811" s="60"/>
+      <c r="B811" s="61"/>
+      <c r="C811" s="61"/>
+      <c r="D811" s="63"/>
     </row>
     <row r="812" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A812" s="56"/>
-      <c r="B812" s="57"/>
-      <c r="C812" s="57"/>
-      <c r="D812" s="58"/>
+      <c r="A812" s="60"/>
+      <c r="B812" s="61"/>
+      <c r="C812" s="61"/>
+      <c r="D812" s="63"/>
     </row>
     <row r="813" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A813" s="56"/>
-      <c r="B813" s="57"/>
-      <c r="C813" s="57"/>
-      <c r="D813" s="58"/>
+      <c r="A813" s="60"/>
+      <c r="B813" s="61"/>
+      <c r="C813" s="61"/>
+      <c r="D813" s="63"/>
     </row>
     <row r="814" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A814" s="56"/>
-      <c r="B814" s="57"/>
-      <c r="C814" s="57"/>
-      <c r="D814" s="58"/>
+      <c r="A814" s="60"/>
+      <c r="B814" s="61"/>
+      <c r="C814" s="61"/>
+      <c r="D814" s="63"/>
     </row>
     <row r="815" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A815" s="56"/>
-      <c r="B815" s="57"/>
-      <c r="C815" s="57"/>
-      <c r="D815" s="58"/>
+      <c r="A815" s="60"/>
+      <c r="B815" s="61"/>
+      <c r="C815" s="61"/>
+      <c r="D815" s="63"/>
     </row>
     <row r="816" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A816" s="56"/>
-      <c r="B816" s="57"/>
-      <c r="C816" s="57"/>
-      <c r="D816" s="58"/>
+      <c r="A816" s="60"/>
+      <c r="B816" s="61"/>
+      <c r="C816" s="61"/>
+      <c r="D816" s="63"/>
     </row>
     <row r="817" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A817" s="56"/>
-      <c r="B817" s="57"/>
-      <c r="C817" s="57"/>
-      <c r="D817" s="58"/>
+      <c r="A817" s="60"/>
+      <c r="B817" s="61"/>
+      <c r="C817" s="61"/>
+      <c r="D817" s="63"/>
     </row>
     <row r="818" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A818" s="56"/>
-      <c r="B818" s="57"/>
-      <c r="C818" s="57"/>
-      <c r="D818" s="58"/>
+      <c r="A818" s="60"/>
+      <c r="B818" s="61"/>
+      <c r="C818" s="61"/>
+      <c r="D818" s="63"/>
     </row>
     <row r="819" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A819" s="56"/>
-      <c r="B819" s="57"/>
-      <c r="C819" s="57"/>
-      <c r="D819" s="58"/>
+      <c r="A819" s="60"/>
+      <c r="B819" s="61"/>
+      <c r="C819" s="61"/>
+      <c r="D819" s="63"/>
     </row>
     <row r="820" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A820" s="56"/>
-      <c r="B820" s="57"/>
-      <c r="C820" s="57"/>
-      <c r="D820" s="58"/>
+      <c r="A820" s="60"/>
+      <c r="B820" s="61"/>
+      <c r="C820" s="61"/>
+      <c r="D820" s="63"/>
     </row>
     <row r="821" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A821" s="56"/>
-      <c r="B821" s="57"/>
-      <c r="C821" s="57"/>
-      <c r="D821" s="58"/>
+      <c r="A821" s="60"/>
+      <c r="B821" s="61"/>
+      <c r="C821" s="61"/>
+      <c r="D821" s="63"/>
     </row>
     <row r="822" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A822" s="56"/>
-      <c r="B822" s="57"/>
-      <c r="C822" s="57"/>
-      <c r="D822" s="58"/>
+      <c r="A822" s="60"/>
+      <c r="B822" s="61"/>
+      <c r="C822" s="61"/>
+      <c r="D822" s="63"/>
     </row>
     <row r="823" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A823" s="56"/>
-      <c r="B823" s="57"/>
-      <c r="C823" s="57"/>
-      <c r="D823" s="58"/>
+      <c r="A823" s="60"/>
+      <c r="B823" s="61"/>
+      <c r="C823" s="61"/>
+      <c r="D823" s="63"/>
     </row>
     <row r="824" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A824" s="56"/>
-      <c r="B824" s="57"/>
-      <c r="C824" s="57"/>
-      <c r="D824" s="58"/>
+      <c r="A824" s="60"/>
+      <c r="B824" s="61"/>
+      <c r="C824" s="61"/>
+      <c r="D824" s="63"/>
     </row>
     <row r="825" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A825" s="56"/>
-      <c r="B825" s="57"/>
-      <c r="C825" s="57"/>
-      <c r="D825" s="58"/>
+      <c r="A825" s="60"/>
+      <c r="B825" s="61"/>
+      <c r="C825" s="61"/>
+      <c r="D825" s="63"/>
     </row>
     <row r="826" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A826" s="56"/>
-      <c r="B826" s="57"/>
-      <c r="C826" s="57"/>
-      <c r="D826" s="58"/>
+      <c r="A826" s="60"/>
+      <c r="B826" s="61"/>
+      <c r="C826" s="61"/>
+      <c r="D826" s="63"/>
     </row>
     <row r="827" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A827" s="56"/>
-      <c r="B827" s="57"/>
-      <c r="C827" s="57"/>
-      <c r="D827" s="58"/>
+      <c r="A827" s="60"/>
+      <c r="B827" s="61"/>
+      <c r="C827" s="61"/>
+      <c r="D827" s="63"/>
     </row>
     <row r="828" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A828" s="56"/>
-      <c r="B828" s="57"/>
-      <c r="C828" s="57"/>
-      <c r="D828" s="58"/>
+      <c r="A828" s="60"/>
+      <c r="B828" s="61"/>
+      <c r="C828" s="61"/>
+      <c r="D828" s="63"/>
     </row>
     <row r="829" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A829" s="56"/>
-      <c r="B829" s="57"/>
-      <c r="C829" s="57"/>
-      <c r="D829" s="58"/>
+      <c r="A829" s="60"/>
+      <c r="B829" s="61"/>
+      <c r="C829" s="61"/>
+      <c r="D829" s="63"/>
     </row>
     <row r="830" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A830" s="56"/>
-      <c r="B830" s="57"/>
-      <c r="C830" s="57"/>
-      <c r="D830" s="58"/>
+      <c r="A830" s="60"/>
+      <c r="B830" s="61"/>
+      <c r="C830" s="61"/>
+      <c r="D830" s="63"/>
     </row>
     <row r="831" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A831" s="56"/>
-      <c r="B831" s="57"/>
-      <c r="C831" s="57"/>
-      <c r="D831" s="58"/>
+      <c r="A831" s="60"/>
+      <c r="B831" s="61"/>
+      <c r="C831" s="61"/>
+      <c r="D831" s="63"/>
     </row>
     <row r="832" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A832" s="56"/>
-      <c r="B832" s="57"/>
-      <c r="C832" s="57"/>
-      <c r="D832" s="58"/>
+      <c r="A832" s="60"/>
+      <c r="B832" s="61"/>
+      <c r="C832" s="61"/>
+      <c r="D832" s="63"/>
     </row>
     <row r="833" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A833" s="56"/>
-      <c r="B833" s="57"/>
-      <c r="C833" s="57"/>
-      <c r="D833" s="58"/>
+      <c r="A833" s="60"/>
+      <c r="B833" s="61"/>
+      <c r="C833" s="61"/>
+      <c r="D833" s="63"/>
     </row>
     <row r="834" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A834" s="56"/>
-      <c r="B834" s="57"/>
-      <c r="C834" s="57"/>
-      <c r="D834" s="58"/>
+      <c r="A834" s="60"/>
+      <c r="B834" s="61"/>
+      <c r="C834" s="61"/>
+      <c r="D834" s="63"/>
     </row>
     <row r="835" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A835" s="56"/>
-      <c r="B835" s="57"/>
-      <c r="C835" s="57"/>
-      <c r="D835" s="58"/>
+      <c r="A835" s="60"/>
+      <c r="B835" s="61"/>
+      <c r="C835" s="61"/>
+      <c r="D835" s="63"/>
     </row>
     <row r="836" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A836" s="56"/>
-      <c r="B836" s="57"/>
-      <c r="C836" s="57"/>
-      <c r="D836" s="58"/>
+      <c r="A836" s="60"/>
+      <c r="B836" s="61"/>
+      <c r="C836" s="61"/>
+      <c r="D836" s="63"/>
     </row>
     <row r="837" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A837" s="56"/>
-      <c r="B837" s="57"/>
-      <c r="C837" s="57"/>
-      <c r="D837" s="58"/>
+      <c r="A837" s="60"/>
+      <c r="B837" s="61"/>
+      <c r="C837" s="61"/>
+      <c r="D837" s="63"/>
     </row>
     <row r="838" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A838" s="56"/>
-      <c r="B838" s="57"/>
-      <c r="C838" s="57"/>
-      <c r="D838" s="58"/>
+      <c r="A838" s="60"/>
+      <c r="B838" s="61"/>
+      <c r="C838" s="61"/>
+      <c r="D838" s="63"/>
     </row>
     <row r="839" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A839" s="56"/>
-      <c r="B839" s="57"/>
-      <c r="C839" s="57"/>
-      <c r="D839" s="58"/>
+      <c r="A839" s="60"/>
+      <c r="B839" s="61"/>
+      <c r="C839" s="61"/>
+      <c r="D839" s="63"/>
     </row>
     <row r="840" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A840" s="56"/>
-      <c r="B840" s="57"/>
-      <c r="C840" s="57"/>
-      <c r="D840" s="58"/>
+      <c r="A840" s="60"/>
+      <c r="B840" s="61"/>
+      <c r="C840" s="61"/>
+      <c r="D840" s="63"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -14049,456 +14358,473 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C297" r:id="rId1" display="https://apply.workable.com/gohenry/" tooltip="https://apply.workable.com/gohenry/"/>
-    <hyperlink ref="C303" r:id="rId2" display="https://careers.lta.org.uk/vacancies/vacancy-search-results.aspx?_gl=1*1u8zpgc*_ga*MzA5NzUyNjgzLjE3MTIzMDg0Njc.*_ga_R8CDFT1V4H*MTcxMjMwODQ2Ny4xLjAuMTcxMjMwODQ2Ny42MC4wLjA." tooltip="https://careers.lta.org.uk/vacancies/vacancy-search-results.aspx?_gl=1*1u8zpgc*_ga*MzA5NzUyNjgzLjE3MTIzMDg0Njc.*_ga_R8CDFT1V4H*MTcxMjMwODQ2Ny4xLjAuMTcxMjMwODQ2Ny42MC4wLjA."/>
-    <hyperlink ref="C208" r:id="rId3" display="https://apply.monsoonjobs.com/search_and_apply/vacancies/" tooltip="https://apply.monsoonjobs.com/search_and_apply/vacancies/"/>
-    <hyperlink ref="C222" r:id="rId4" display="https://partners.bridebook.com/uk/careers#openroles"/>
-    <hyperlink ref="C211" r:id="rId5" display="https://careers.lightricks.com/careers"/>
-    <hyperlink ref="C215" r:id="rId6" display="https://www.scandit.com/careers/current-openings/" tooltip="https://www.scandit.com/careers/current-openings/"/>
-    <hyperlink ref="C126" r:id="rId7" display="https://www.workspace.co.uk/job-vacancies" tooltip="https://www.workspace.co.uk/job-vacancies"/>
-    <hyperlink ref="C230" r:id="rId8" display="https://faculty.ai/join-the-team/#ashby_embed"/>
-    <hyperlink ref="C206" r:id="rId9" display="https://greshamhouse.com/join-our-team/"/>
-    <hyperlink ref="C7" r:id="rId10" display="https://jobs.lever.co/cfgi" tooltip="https://jobs.lever.co/cfgi"/>
-    <hyperlink ref="C12" r:id="rId11" display="https://www.kfh.co.uk/careers/vacancies/"/>
-    <hyperlink ref="C13" r:id="rId12" display="https://3s.money/join/careers" tooltip="https://3s.money/join/careers"/>
-    <hyperlink ref="C14" r:id="rId13" display="https://4global.com/company/#" tooltip="https://4global.com/company/#"/>
-    <hyperlink ref="C15" r:id="rId14" display="https://4cassociates.teamtailor.com/jobs" tooltip="https://4cassociates.teamtailor.com/jobs"/>
-    <hyperlink ref="C16" r:id="rId15" display="https://www.aswatsoncareers.com/search" tooltip="https://www.aswatsoncareers.com/search"/>
-    <hyperlink ref="C17" r:id="rId16" display="https://abel-cole.breezy.hr/" tooltip="https://abel-cole.breezy.hr/"/>
-    <hyperlink ref="C19" r:id="rId17" display="https://careers.achievetogether.co.uk/Search.aspx" tooltip="https://careers.achievetogether.co.uk/Search.aspx"/>
-    <hyperlink ref="C23" r:id="rId18" display="https://careers.adyen.com/vacancies" tooltip="https://careers.adyen.com/vacancies"/>
-    <hyperlink ref="C24" r:id="rId19" display="https://careers.allianz.com/UK/search/?searchby=location&amp;createNewAlert=false&amp;q=&amp;locationsearch=GB%2C%20US&amp;optionsFacetsDD_department=&amp;optionsFacetsDD_shifttype=&amp;optionsFacetsDD_customfield3=&amp;optionsFacetsDD_customfield2=&amp;optionsFacetsDD_facility=&amp;optionsFacetsDD_customfield4=&amp;optionsFacetsDD_dept=&amp;inputSearchValue=GB%2C%20US&amp;quatFlag=false" tooltip="https://careers.allianz.com/UK/search/?searchby=location&amp;createNewAlert=false&amp;q=&amp;locationsearch=GB%2C%20US&amp;optionsFacetsDD_department=&amp;optionsFacetsDD_shifttype=&amp;optionsFacetsDD_customfield3=&amp;optionsFacetsDD_customfield2=&amp;optionsFacetsDD_facility=&amp;options"/>
-    <hyperlink ref="C25" r:id="rId20" display="https://myndyou.com/about-us/careers/" tooltip="https://myndyou.com/about-us/careers/"/>
-    <hyperlink ref="C27" r:id="rId21" display="https://www.hungerrush.com/careers/?an_fb_exaud=an_fb_hungerrushe46sdg56&amp;an_exaud0=an_fb_hungerrush6rsf5dhrd698" tooltip="https://www.hungerrush.com/careers/?an_fb_exaud=an_fb_hungerrushe46sdg56&amp;an_exaud0=an_fb_hungerrush6rsf5dhrd698"/>
-    <hyperlink ref="C28" r:id="rId22" display="https://work.life/careers/"/>
-    <hyperlink ref="C29" r:id="rId23" display="https://careers.next15.com/jobs" tooltip="https://careers.next15.com/jobs"/>
-    <hyperlink ref="C33" r:id="rId24" display="https://careers.iqstudentaccommodation.com/jobs/vacancy/find/results/" tooltip="https://careers.iqstudentaccommodation.com/jobs/vacancy/find/results/"/>
-    <hyperlink ref="C34" r:id="rId25" display="https://careers.isio.com/en-GB/jobs"/>
-    <hyperlink ref="C36" r:id="rId26" display="https://www.airwallex.com/careers#roles" tooltip="https://www.airwallex.com/careers#roles"/>
-    <hyperlink ref="C38" r:id="rId27" display="https://www.allwyn.co.uk/job-board"/>
-    <hyperlink ref="C48" r:id="rId28" display="https://www.appearhere.co.uk/about/careers"/>
-    <hyperlink ref="C49" r:id="rId29" display="https://careers.arbor-education.com/#jobs"/>
-    <hyperlink ref="C52" r:id="rId30" display="https://artek.uk/careers" tooltip="https://artek.uk/careers"/>
-    <hyperlink ref="C53" r:id="rId31" display="https://us232.dayforcehcm.com/CandidatePortal/en-US/comptia" tooltip="https://us232.dayforcehcm.com/CandidatePortal/en-US/comptia"/>
-    <hyperlink ref="C55" r:id="rId32" display="https://atelierfinance.co.uk/careers/" tooltip="https://atelierfinance.co.uk/careers/"/>
-    <hyperlink ref="C56" r:id="rId33" display="https://ejjl.fa.ap1.oraclecloud.com/hcmUI/CandidateExperience/en/sites/CX_1/requisitions?lastSelectedFacet=LOCATIONS&amp;mode=location&amp;selectedLocationsFacet=300000000296420%3B300000000294958"/>
-    <hyperlink ref="C57" r:id="rId34" display="https://isw.changeworknow.co.uk/awayresorts/vms/e/careers/search/edit"/>
-    <hyperlink ref="C59" r:id="rId35" display="https://transitwireless.taleo.net/careersection/ex/jobsearch.ftl?lang=en" tooltip="https://transitwireless.taleo.net/careersection/ex/jobsearch.ftl?lang=en"/>
-    <hyperlink ref="C60" r:id="rId36" display="https://apply.workable.com/ballingerco/#jobs"/>
-    <hyperlink ref="C63" r:id="rId37" display="https://baxendale.co.uk/careers/" tooltip="https://baxendale.co.uk/careers/"/>
-    <hyperlink ref="C64" r:id="rId38" display="https://bcis.co.uk/about-us/careers/"/>
-    <hyperlink ref="C65" r:id="rId39" display="https://www.beacon.com/vacancies" tooltip="https://www.beacon.com/vacancies"/>
-    <hyperlink ref="C66" r:id="rId40" display="https://careers.beamery.com/jobs/"/>
-    <hyperlink ref="C67" r:id="rId41" display="https://www.adverity.com/careers" tooltip="https://www.adverity.com/careers"/>
-    <hyperlink ref="C68" r:id="rId42" display="https://www.togetherforgirls.org/en/careers" tooltip="https://www.togetherforgirls.org/en/careers"/>
-    <hyperlink ref="C69" r:id="rId43" display="https://www.rcseng.ac.uk/about-the-rcs/working-at-the-college/current-rcs-vacancies/" tooltip="https://www.rcseng.ac.uk/about-the-rcs/working-at-the-college/current-rcs-vacancies/"/>
-    <hyperlink ref="C71" r:id="rId44" display="https://jobs.bentley.com/search" tooltip="https://jobs.bentley.com/search"/>
-    <hyperlink ref="C72" r:id="rId45" display="https://apply.workable.com/volt-dot-i-o/#jobs"/>
-    <hyperlink ref="C77" r:id="rId46" display="https://learnamp.com/careers#open-positions" tooltip="https://learnamp.com/careers#open-positions"/>
-    <hyperlink ref="C84" r:id="rId47" display="https://www.apprentify.com/internal-vacancies/" tooltip="https://www.apprentify.com/internal-vacancies/"/>
-    <hyperlink ref="C87" r:id="rId48" display="https://www.rethinkfirst.com/careers/" tooltip="https://www.rethinkfirst.com/careers/"/>
-    <hyperlink ref="C89" r:id="rId49" display="https://www.vitechinc.com/careers/view-opportunities/"/>
-    <hyperlink ref="C91" r:id="rId50" display="https://boards.greenhouse.io/prefect"/>
-    <hyperlink ref="C83" r:id="rId51" display="https://fortnum-and-mason.staging.krakatoa.eu-2.volcanic.cloud/jobs?source=careers.fortnumandmason.com"/>
-    <hyperlink ref="C85" r:id="rId52" display="https://ghd.livevacancies.co.uk/#/"/>
-    <hyperlink ref="C81" r:id="rId53" display="https://powerleaguegroup.postingpanda.uk/" tooltip="https://powerleaguegroup.postingpanda.uk/"/>
-    <hyperlink ref="C80" r:id="rId54" display="https://netacea.com/careers/" tooltip="https://netacea.com/careers/"/>
-    <hyperlink ref="C177" r:id="rId55" display="https://boards.greenhouse.io/heycar/"/>
-    <hyperlink ref="C114" r:id="rId56" display="https://harri.com/grind-careers" tooltip="https://harri.com/grind-careers"/>
-    <hyperlink ref="C326" r:id="rId57" display="https://jobs.ashbyhq.com/metaview"/>
-    <hyperlink ref="C288" r:id="rId58" display="https://boards.eu.greenhouse.io/bitpanda"/>
-    <hyperlink ref="C30" r:id="rId59" display="https://www.prime-propertygroup.com/contacts/"/>
-    <hyperlink ref="C74" r:id="rId60" display="https://careers.hansonwadegroup.com/jobs"/>
-    <hyperlink ref="C75" r:id="rId61" display="https://getmagic.com/careers/" tooltip="https://getmagic.com/careers/"/>
-    <hyperlink ref="C88" r:id="rId62" display="https://canarywharf.wd3.myworkdayjobs.com/CanaryWharf" tooltip="https://canarywharf.wd3.myworkdayjobs.com/CanaryWharf"/>
-    <hyperlink ref="C93" r:id="rId63" display="https://jobs.workable.com/company/vbFZaR6cPm46s3pMMdSotv/jobs-at-the-very-group"/>
-    <hyperlink ref="C98" r:id="rId64" display="https://jobs.lever.co/treecard" tooltip="https://jobs.lever.co/treecard"/>
-    <hyperlink ref="C99" r:id="rId65" display="https://careers.scs.co.uk/all-openings"/>
-    <hyperlink ref="C100" r:id="rId66" display="https://corporate.lastminute.com/careers/jobs/?utm_source=lastminute&amp;_gl=1*ozugby*_ga*MTE0MTE2MTkxNS4xNzEwNzIwNzE4*_ga_66BMGPKMTR*MTcxMDcyMDcxNy4xLjAuMTcxMDcyMDgzMS4wLjAuMA..*_fplc*aWYlMkZSMVRhSVQlMkJFSktZQWNRQjhiSXhnelJmVUlHVFF0VUg3dWlQZWtMYXAxQUJWQ0xROCUyRk9UYlJGcXVSNWl3OWRjVnJLOU5DS2UxazE1ZEhKRzlPOE9lbjlmZ2VobWhkd1VCJTJGaWhIVnpnVnFNQ0J3ZzF3d0FsSXNLa2ozJTJGZyUzRCUzRA..&amp;_ga=2.250966918.1438506767.1710720718-1141161915.1710720718&amp;_gac=1.53775706.1710720718.CjwKCAiA0PuuBhBsEiwAS7fsNUBcK-u-irmaNJ8YfoBMQjHXX35iigABH04TXkR1Iz0HyWwv4kLPjxoC3M0QAvD_BwE"/>
-    <hyperlink ref="C101" r:id="rId67" display="https://cityfibre.com/careers/all-jobs"/>
-    <hyperlink ref="C102" r:id="rId68" display="https://harri.com/Biscuiteers-careers"/>
-    <hyperlink ref="C103" r:id="rId69" display="https://careers.cargill.com/en/search-jobs"/>
-    <hyperlink ref="C108" r:id="rId70" display="https://www.aireymiller.com/careers"/>
-    <hyperlink ref="C109" r:id="rId71" display="https://wearemtm.com/careers/" tooltip="https://wearemtm.com/careers/"/>
-    <hyperlink ref="C111" r:id="rId72" display="https://jobs.cityoflondon.gov.uk"/>
-    <hyperlink ref="C113" r:id="rId73" display="https://www.hush-uk.com/work-at-hush.html"/>
-    <hyperlink ref="C115" r:id="rId74" display="https://www.ibisworld.com/careers/" tooltip="https://www.ibisworld.com/careers/"/>
-    <hyperlink ref="C117" r:id="rId75" display="https://www.vouchercodes.co.uk/careers" tooltip="https://www.vouchercodes.co.uk/careers"/>
-    <hyperlink ref="C118" r:id="rId76" display="https://jobs.lever.co/joinzoe"/>
-    <hyperlink ref="C120" r:id="rId77" display="https://www.multiverse.io/en-GB/careers#job-list"/>
-    <hyperlink ref="C121" r:id="rId78" display="https://www.simplybusiness.co.uk/about-us/careers/jobs/" tooltip="https://www.simplybusiness.co.uk/about-us/careers/jobs/"/>
-    <hyperlink ref="C122" r:id="rId79" display="https://munichre-jobs.com/en/MunichRe"/>
-    <hyperlink ref="C123" r:id="rId80" display="https://apply.workable.com/fenergocareers/"/>
-    <hyperlink ref="C124" r:id="rId81" display="https://www.thoughtworks.com/en-gb/careers" tooltip="https://www.thoughtworks.com/en-gb/careers"/>
-    <hyperlink ref="C127" r:id="rId82" display="https://impact.com/careers/#global-opportunities"/>
-    <hyperlink ref="C128" r:id="rId83" display="https://supercharge.io/careers/positions"/>
-    <hyperlink ref="C130" r:id="rId84" display="https://apply.workable.com/starling-bank/#jobs"/>
-    <hyperlink ref="C131" r:id="rId85" display="https://symphony.com/company/careers/"/>
-    <hyperlink ref="C132" r:id="rId86" display="https://careers.cynergybank.co.uk/jobs?location=London"/>
-    <hyperlink ref="C134" r:id="rId87" display="https://jobs.ashbyhq.com/myurbanjungle.com" tooltip="https://jobs.ashbyhq.com/myurbanjungle.com"/>
-    <hyperlink ref="C136" r:id="rId88" display="https://www.yonder.com/careers#open-positions"/>
-    <hyperlink ref="C137" r:id="rId89" display="https://careers.ovo.com/opportunities "/>
-    <hyperlink ref="C138" r:id="rId90" display="https://workingatedge.com/careers/"/>
-    <hyperlink ref="C139" r:id="rId91" display="https://pelorusx.co/about/careers" tooltip="https://pelorusx.co/about/careers"/>
-    <hyperlink ref="C140" r:id="rId92" display="https://www.peldonrose.com/about/jobs" tooltip="https://www.peldonrose.com/about/jobs"/>
-    <hyperlink ref="C141" r:id="rId93" display="https://www.naturalhr.net/hr/recruitment/roles/8279302e80a62ccde7ee587a4f382535"/>
-    <hyperlink ref="C142" r:id="rId94" display="https://www.industrialsreit.com/careers"/>
-    <hyperlink ref="C143" r:id="rId95" display="https://www.oka.com/uk/careers/opportunities"/>
-    <hyperlink ref="C144" r:id="rId96" display="https://www.capgemini.com/gb-en/careers/join-us/" tooltip="https://www.capgemini.com/gb-en/careers/join-us/"/>
-    <hyperlink ref="C145" r:id="rId97" display="https://jobs.amundi.com/homepage.aspx?LCID=2057" tooltip="https://jobs.amundi.com/homepage.aspx?LCID=2057"/>
-    <hyperlink ref="C146" r:id="rId98" display="https://jobs.pphe.com/careers/?country=united-kingdom" tooltip="https://jobs.pphe.com/careers/?country=united-kingdom"/>
-    <hyperlink ref="C148" r:id="rId99" display="https://www.freddiesflowers.com/about-us/jobs#openings"/>
-    <hyperlink ref="C149" r:id="rId100" display="https://www.iabuk.com/vacancies" tooltip="https://www.iabuk.com/vacancies"/>
-    <hyperlink ref="C150" r:id="rId101" display="https://channel3consulting.livevacancies.co.uk/jobsIframe" tooltip="https://channel3consulting.livevacancies.co.uk/jobsIframe"/>
-    <hyperlink ref="C151" r:id="rId102" display="https://careers.domesticandgeneral.com/search-jobs/"/>
-    <hyperlink ref="C152" r:id="rId103" display="https://patchwork.teamtailor.com/jobs" tooltip="https://patchwork.teamtailor.com/jobs"/>
-    <hyperlink ref="C154" r:id="rId104" display="https://www.palantir.com/careers/#open-positions" tooltip="https://www.palantir.com/careers/#open-positions"/>
-    <hyperlink ref="C156" r:id="rId105" display="https://profinda.bamboohr.com/careers" tooltip="https://profinda.bamboohr.com/careers"/>
-    <hyperlink ref="C157" r:id="rId106" display="https://hymans.current-vacancies.com/Careers/Hymans%20external%20VSP-2054#"/>
-    <hyperlink ref="C159" r:id="rId107" display="https://www.downing.co.uk/careers#open-positions"/>
-    <hyperlink ref="C160" r:id="rId108" display="https://www.turnerandtownsend.com/en/careers/apply-now/"/>
-    <hyperlink ref="C161" r:id="rId109" display="https://jobs.petscorner.co.uk/job-list/"/>
-    <hyperlink ref="C164" r:id="rId110" display="https://jobs.reachplc.com/jobs"/>
-    <hyperlink ref="C165" r:id="rId111" display="https://www.connellsgroup.co.uk/careers/job-search/?radius=5&amp;page=1&amp;sort=posted&amp;direction=desc" tooltip="https://www.connellsgroup.co.uk/careers/job-search/?radius=5&amp;page=1&amp;sort=posted&amp;direction=desc"/>
-    <hyperlink ref="C167" r:id="rId112" display="https://www.semble.io/careers" tooltip="https://www.semble.io/careers"/>
-    <hyperlink ref="C166" r:id="rId113" display="https://careers.savills.com/jobs"/>
-    <hyperlink ref="C170" r:id="rId114" display="https://clear.bank/join-clearbank/careers"/>
-    <hyperlink ref="C171" r:id="rId115" display="https://www.quantexa.com/careers/vacancies/" tooltip="https://www.quantexa.com/careers/vacancies/"/>
-    <hyperlink ref="C172" r:id="rId116" display="https://jajafinance.bamboohr.com/careers" tooltip="https://jajafinance.bamboohr.com/careers"/>
-    <hyperlink ref="C173" r:id="rId117" display="https://careers.phished.io/l/en" tooltip="https://careers.phished.io/l/en"/>
-    <hyperlink ref="C176" r:id="rId118" display="https://careers.scienceinsport.com/jobs"/>
-    <hyperlink ref="C178" r:id="rId119" display="https://boards.eu.greenhouse.io/convera/"/>
-    <hyperlink ref="C179" r:id="rId120" display="https://volarisgroup.wd3.myworkdayjobs.com/CompanyWatch" tooltip="https://volarisgroup.wd3.myworkdayjobs.com/CompanyWatch"/>
-    <hyperlink ref="C180" r:id="rId121" display="https://www.verkeer.co/about-us/careers/"/>
-    <hyperlink ref="C181" r:id="rId122" display="https://careers.cbre.com/en_US/careers/SearchJobs/?9577=%5B17276%2C17117%5D&amp;9577_format=10224&amp;listFilterMode=1&amp;jobSort=relevancy&amp;jobRecordsPerPage=25&amp;" tooltip="https://careers.cbre.com/en_US/careers/SearchJobs/?9577=%5B17276%2C17117%5D&amp;9577_format=10224&amp;listFilterMode=1&amp;jobSort=relevancy&amp;jobRecordsPerPage=25&amp;"/>
-    <hyperlink ref="C183" r:id="rId123" display="https://montaguevans.jibeapply.com/careers-home/jobs?keywords=&amp;location=&amp;page=1&amp;sortBy=relevance&amp;limit=100"/>
-    <hyperlink ref="C187" r:id="rId124" display="https://ichoosr.recruitee.com/"/>
-    <hyperlink ref="C188" r:id="rId125" display="https://www.ospreycharging.co.uk/careers-at-osprey-charging"/>
-    <hyperlink ref="C192" r:id="rId126" display="https://jobs.yougov.com/jobs"/>
-    <hyperlink ref="C207" r:id="rId127" display="https://jobs.thecignagroup.com/us/en/search-results" tooltip="https://jobs.thecignagroup.com/us/en/search-results"/>
-    <hyperlink ref="C210" r:id="rId128" display="https://www.kpmgcareers.co.uk/search/" tooltip="https://www.kpmgcareers.co.uk/search/"/>
-    <hyperlink ref="C216" r:id="rId129" display="https://ryman.ats.emea1.fourth.com"/>
-    <hyperlink ref="C218" r:id="rId130" display="https://job-boards.greenhouse.io/fountain"/>
-    <hyperlink ref="C220" r:id="rId131" display="https://freetrade.io/careers#job-openings"/>
-    <hyperlink ref="C223" r:id="rId132" display="https://jobs.decathlon.co.uk/go/View-all-Jobs/4978001/"/>
-    <hyperlink ref="C224" r:id="rId133" display="https://www.theaacareers.co.uk/apply/?s_Keywords="/>
-    <hyperlink ref="C226" r:id="rId134" display="https://www.lhh.com/uk/en/search-jobs/"/>
-    <hyperlink ref="C227" r:id="rId135" display="https://careers.telegraph.co.uk/jobs/job-search?location=London"/>
-    <hyperlink ref="C229" r:id="rId136" display="https://careers.deliveroo.co.uk/jobs/" tooltip="https://careers.deliveroo.co.uk/jobs/"/>
-    <hyperlink ref="C231" r:id="rId137" display="https://www.family-institute.org/about-us/careers"/>
-    <hyperlink ref="C232" r:id="rId138" display="https://thegymgroup.wd3.myworkdayjobs.com/TGG_External_Career_Site" tooltip="https://thegymgroup.wd3.myworkdayjobs.com/TGG_External_Career_Site"/>
-    <hyperlink ref="C233" r:id="rId139" display="https://cmcmarkets.wd3.myworkdayjobs.com/CMC_Markets_Careers"/>
-    <hyperlink ref="C235" r:id="rId140" display="https://turo.com/gb/en/careers#job_openings" tooltip="https://turo.com/gb/en/careers#job_openings"/>
-    <hyperlink ref="C236" r:id="rId141" display="https://www.mollymaid.co.uk/working-for-molly-maid/"/>
-    <hyperlink ref="C237" r:id="rId142" display="https://www.newscareers.co.uk/vacancies/vacancy-search-results.aspx" tooltip="https://www.newscareers.co.uk/vacancies/vacancy-search-results.aspx"/>
-    <hyperlink ref="C238" r:id="rId143" display="https://jobs.greystar.com/search-jobs/" tooltip="https://jobs.greystar.com/search-jobs/"/>
-    <hyperlink ref="C239" r:id="rId144" display="https://careers.upmc.com/job-search-results/" tooltip="https://careers.upmc.com/job-search-results/"/>
-    <hyperlink ref="C240" r:id="rId145" display="https://natterbox.com/careers/"/>
-    <hyperlink ref="C241" r:id="rId146" display="https://www.constellationcold.com/vacancies/"/>
-    <hyperlink ref="C242" r:id="rId147" display="https://www.neudata.co/careers#Jobs"/>
-    <hyperlink ref="C244" r:id="rId148" display="https://www.thredd.com/about-us/careers/vacancies"/>
-    <hyperlink ref="C246" r:id="rId149" display="https://careers.marshmclennan.com/global/en/oliver-wyman-search"/>
-    <hyperlink ref="C250" r:id="rId150" display="https://mileway.com/careers/opportunities/"/>
-    <hyperlink ref="C251" r:id="rId151" display="https://www.efficioconsulting.com/en-gb/careers/apply/" tooltip="https://www.efficioconsulting.com/en-gb/careers/apply/"/>
-    <hyperlink ref="C253" r:id="rId152" display="https://thelostestate.com/jobs/"/>
-    <hyperlink ref="C254" r:id="rId153" display="https://www.elixirr.com/en-gb/job-openings/" tooltip="https://www.elixirr.com/en-gb/job-openings/"/>
-    <hyperlink ref="C256" r:id="rId154" display="https://jobs.lever.co/enable"/>
-    <hyperlink ref="C259" r:id="rId155" display="https://www.busybeerecruitment.co.uk/vacancies"/>
-    <hyperlink ref="C264" r:id="rId156" display="https://www.capitalontap.com/en/company/careers/#careers-jobs"/>
-    <hyperlink ref="C265" r:id="rId157" display="https://careers.learnatnoon.com/jobs"/>
-    <hyperlink ref="C269" r:id="rId158" display="https://www.tussell.com/careers#jobs" tooltip="https://www.tussell.com/careers#jobs"/>
-    <hyperlink ref="C272" r:id="rId159" display="https://www.doddgroup.com/jobs"/>
-    <hyperlink ref="C282" r:id="rId160" display="https://www.speechmatics.com/company/careers/roles"/>
-    <hyperlink ref="C284" r:id="rId161" display="https://thecrownestate.teamtailor.com/jobs"/>
-    <hyperlink ref="C290" r:id="rId162" display="https://www.tilda.com/about-us/careers/" tooltip="https://www.tilda.com/about-us/careers/"/>
-    <hyperlink ref="C291" r:id="rId163" display="https://apply.workable.com/koothjobs/" tooltip="https://apply.workable.com/koothjobs/"/>
-    <hyperlink ref="C293" r:id="rId164" display="https://www.kkr.com/careers/career-opportunities"/>
-    <hyperlink ref="C294" r:id="rId165" display="https://app.otta.com/companies/GetHarley#company-mission-section" tooltip="https://app.otta.com/companies/GetHarley#company-mission-section"/>
-    <hyperlink ref="C296" r:id="rId166" display="https://dt-consulting.com/open-positions/" tooltip="https://dt-consulting.com/open-positions/"/>
-    <hyperlink ref="C298" r:id="rId167" display="https://www.realestate.bnpparibas.co.uk/find-job"/>
-    <hyperlink ref="C301" r:id="rId168" display="https://ts.wd5.myworkdayjobs.com/en-US/tishmanspeyer"/>
-    <hyperlink ref="C306" r:id="rId169" display="https://www.charliehr.com/careers#Vacancies" tooltip="https://www.charliehr.com/careers#Vacancies"/>
-    <hyperlink ref="C307" r:id="rId170" display="https://milltechfx.com/company/careers/"/>
-    <hyperlink ref="C308" r:id="rId171" display="https://harri.com/The-Delaunay-BYtcttE0b35i" tooltip="https://harri.com/The-Delaunay-BYtcttE0b35i"/>
-    <hyperlink ref="C309" r:id="rId172" display="https://careers.legalandgeneral.com/jobs?options=203"/>
-    <hyperlink ref="C311" r:id="rId173" display="https://www.amazon.jobs/content/en/teams/amazon-entertainment/music?country%5B%5D=US&amp;country%5B%5D=GB"/>
-    <hyperlink ref="C312" r:id="rId174" display="https://hyve.group/lifeathyve/join-our-team/" tooltip="https://hyve.group/lifeathyve/join-our-team/"/>
-    <hyperlink ref="C315" r:id="rId175" display="https://www.harrodscareers.com/jobs" tooltip="https://www.harrodscareers.com/jobs"/>
-    <hyperlink ref="C317" r:id="rId176" display="https://vistaglobal.com/careers/" tooltip="https://vistaglobal.com/careers/"/>
-    <hyperlink ref="C319" r:id="rId177" display="https://join.modsquad.com/careers/"/>
-    <hyperlink ref="C321" r:id="rId178" display="https://shieldpay.teamtailor.com/jobs"/>
-    <hyperlink ref="C325" r:id="rId179" display="https://jll.wd1.myworkdayjobs.com/jllcareers"/>
-    <hyperlink ref="C327" r:id="rId180" display="https://hdfg.fa.em3.oraclecloud.com/hcmUI/CandidateExperience/en/sites/CX/requisitions?mode=location"/>
-    <hyperlink ref="C328" r:id="rId181" display="https://www.envitia.com/careers/job-opportunities/"/>
-    <hyperlink ref="C335" r:id="rId182" display="https://careers.northhighland.com/jobs/" tooltip="https://careers.northhighland.com/jobs/"/>
-    <hyperlink ref="C336" r:id="rId183" display="https://careers.captify.co.uk/#jobs"/>
-    <hyperlink ref="C338" r:id="rId184" display="https://fa-evng-saasfaprod1.fa.ocs.oraclecloud.com/hcmUI/CandidateExperience/en/sites/LBWF/requisitions?location=United+Kingdom&amp;locationId=300000000471661&amp;locationLevel=country&amp;mode=location"/>
-    <hyperlink ref="C339" r:id="rId185" display="https://channel3consulting.co.uk/work-with-us/careers/"/>
-    <hyperlink ref="C340" r:id="rId186" display="https://www.gwi.com/careers#job-list"/>
-    <hyperlink ref="C341" r:id="rId187" display="https://polestar.teamtailor.com/jobs"/>
-    <hyperlink ref="C110" r:id="rId188" display="https://www.alphagroup.com/about/careers/" tooltip="https://www.alphagroup.com/about/careers/"/>
-    <hyperlink ref="C342" r:id="rId189" display="https://www.11fs.com/careers/vacancies" tooltip="https://www.11fs.com/careers/vacancies"/>
-    <hyperlink ref="C343" r:id="rId190" display="https://careers.7im.co.uk/vacancies/vacancy-search-results.aspx"/>
-    <hyperlink ref="C347" r:id="rId191" display="https://jobs.amadeuscapital.com/"/>
-    <hyperlink ref="C348" r:id="rId192" display="https://recruiting.ultipro.com/AME1095ACHM/JobBoard/c52f9a39-fdc5-4ae2-9eaf-cb8a7bda923e/?q=&amp;o=postedDateDesc&amp;w=&amp;wc=&amp;we=&amp;wpst="/>
-    <hyperlink ref="C349" r:id="rId193" display="https://arthur.co.uk/live-jobs/" tooltip="https://arthur.co.uk/live-jobs/"/>
-    <hyperlink ref="C350" r:id="rId194" display="https://aztec.group/us/careers/current-vacancies/"/>
-    <hyperlink ref="C351" r:id="rId195" display="https://www.barbican.org.uk/our-story/about-us/careers"/>
-    <hyperlink ref="C352" r:id="rId196" display="https://baringa.csod.com/ux/ats/careersite/4/home?c=baringa" tooltip="https://baringa.csod.com/ux/ats/careersite/4/home?c=baringa"/>
-    <hyperlink ref="C353" r:id="rId197" display="https://www.bellaandduke.com/join-our-team/" tooltip="https://www.bellaandduke.com/join-our-team/"/>
-    <hyperlink ref="C354" r:id="rId198" display="https://job-boards.eu.greenhouse.io/theberkeleypartnership" tooltip="https://job-boards.eu.greenhouse.io/theberkeleypartnership"/>
-    <hyperlink ref="C355" r:id="rId199" display="https://bespoke-bids.com/careers/"/>
-    <hyperlink ref="C356" r:id="rId200" display="https://big.dk/careers"/>
-    <hyperlink ref="C360" r:id="rId201" display="https://baicommunications.wd3.myworkdayjobs.com/External"/>
-    <hyperlink ref="C361" r:id="rId202" display="https://careers.boohoogroup.com/search-jobs"/>
-    <hyperlink ref="C362" r:id="rId203" display="https://workfor.brightnetwork.co.uk/join-us"/>
-    <hyperlink ref="C363" r:id="rId204" display="https://www.broadwaymalyan.com/people/vacancies/"/>
-    <hyperlink ref="C364" r:id="rId205" display="https://www.burtonsbiscuits.com/life-at-burtons/current-vacancies/burton-s-bakeries/"/>
-    <hyperlink ref="C365" r:id="rId206" display="https://jobs.lever.co/moonpig"/>
-    <hyperlink ref="C366" r:id="rId207" display="https://careers.oniverse.it/en-GB/home"/>
-    <hyperlink ref="C367" r:id="rId208" display="https://camillaelphick.com/pages/careers-1" tooltip="https://camillaelphick.com/pages/careers-1"/>
-    <hyperlink ref="C368" r:id="rId209" display="https://www.cartwrightpickard.com/careers"/>
-    <hyperlink ref="C369" r:id="rId210" display="https://www.celigo.com/careers/#job-listings"/>
-    <hyperlink ref="C370" r:id="rId211" display="https://www.channelbakers.com/careers" tooltip="https://www.channelbakers.com/careers"/>
-    <hyperlink ref="C371" r:id="rId212" display="https://www.careers-page.com/chelsea-peers#openings" tooltip="https://www.careers-page.com/chelsea-peers#openings"/>
-    <hyperlink ref="C372" r:id="rId213" display="https://careers.churchdwight.com/jobs/?search=&amp;country=GBR&amp;location=&amp;team=&amp;position=&amp;type="/>
-    <hyperlink ref="C373" r:id="rId214" display="https://cinchona.com/careers/"/>
-    <hyperlink ref="C374" r:id="rId215" display="https://cipfa.teamtailor.com/jobs?query="/>
-    <hyperlink ref="C375" r:id="rId216" display="https://jobs.cliffordchance.com/jobs?options=49,58&amp;page=1"/>
-    <hyperlink ref="C376" r:id="rId217" display="https://work-clockwise.com/careers/"/>
-    <hyperlink ref="C377" r:id="rId218" display="https://www.clubmedjobs.com/en/search-jobs/" tooltip="https://www.clubmedjobs.com/en/search-jobs/"/>
-    <hyperlink ref="C378" r:id="rId219" display="https://fsr.cvmailuk.com/clydecocareers/main.cfm?page=jobBoard&amp;fo=1&amp;groupType_21=&amp;groupType_33=&amp;filter=&amp;srxksl=1"/>
-    <hyperlink ref="C380" r:id="rId220" display="https://www.couvertureandthegarbstore.com/pages/careers"/>
-    <hyperlink ref="C381" r:id="rId221" display="https://crawfordtech.pinpointhq.com/#js-careers-jobs-block"/>
-    <hyperlink ref="C383" r:id="rId222" display="https://globaleur242.dayforcehcm.com/CandidatePortal/en-GB/crippspeople/" tooltip="https://globaleur242.dayforcehcm.com/CandidatePortal/en-GB/crippspeople/"/>
-    <hyperlink ref="C384" r:id="rId223" display="https://www.csl-group.com/uk/careers/"/>
-    <hyperlink ref="C386" r:id="rId224" display="https://cumminggroup.wd1.myworkdayjobs.com/CGC" tooltip="https://cumminggroup.wd1.myworkdayjobs.com/CGC"/>
-    <hyperlink ref="C387" r:id="rId225" display="https://www.redpincompany.com/careers?department=&amp;location=&amp;company=currencies-direct&amp;page=1"/>
-    <hyperlink ref="C388" r:id="rId226" display="https://www.dae.mn/openings"/>
-    <hyperlink ref="C389" r:id="rId227" display="https://datatonic.com/careers/vacancies/" tooltip="https://datatonic.com/careers/vacancies/"/>
-    <hyperlink ref="C390" r:id="rId228" display="https://careers.dcc.ie/dccvital/search/"/>
-    <hyperlink ref="C391" r:id="rId229" display="https://www.dechert.com/careers.html"/>
-    <hyperlink ref="C393" r:id="rId230" display="https://apply.workable.com/demellier-ltd/?lng=en"/>
-    <hyperlink ref="C395" r:id="rId231" display="https://downing.com/work-for-us/#work-for-us-6"/>
-    <hyperlink ref="C396" r:id="rId232" display="https://drdoctor.teamtailor.com/jobs" tooltip="https://drdoctor.teamtailor.com/jobs"/>
-    <hyperlink ref="C397" r:id="rId233" display="https://careers.dufry.com/go/Dufry-Main/9035601/"/>
-    <hyperlink ref="C398" r:id="rId234" display="https://careers-dwfgroup.icims.com/jobs/search?hashed=-625886029&amp;mobile=false&amp;width=1011&amp;height=500&amp;bga=true&amp;needsRedirect=false&amp;jan1offset=0&amp;jun1offset=60" tooltip="https://careers-dwfgroup.icims.com/jobs/search?hashed=-625886029&amp;mobile=false&amp;width=1011&amp;height=500&amp;bga=true&amp;needsRedirect=false&amp;jan1offset=0&amp;jun1offset=60"/>
-    <hyperlink ref="C400" r:id="rId235" display="https://empiricstudentpropertyplc.talosats-careers.com/vacancies"/>
-    <hyperlink ref="C401" r:id="rId236" display="https://careers.enginuity.org/jobs"/>
-    <hyperlink ref="C402" r:id="rId237" display="https://careers.ensek.com/" tooltip="https://careers.ensek.com/"/>
-    <hyperlink ref="C403" r:id="rId238" display="https://eo-group.co.uk/opportunities/"/>
-    <hyperlink ref="C404" r:id="rId239" display="https://equita.co.uk/about-us/work-with-us/"/>
-    <hyperlink ref="C405" r:id="rId240" display="https://equiteq.careers.hibob.com/" tooltip="https://equiteq.careers.hibob.com/"/>
-    <hyperlink ref="C406" r:id="rId241" display="https://join.estrid.com/jobs?_gl=1*o2mc52*_gcl_au*NTQ1NjA2NDYxLjE3MjA1MzY1NDQ.*_ga*MTUwMjg1NTAyOS4xNzIwNTM2NTQ0*_fplc*SzNYUEpUcU84dCUyRkJQcGRtRmJzU3JvelRaRjhWZ2NPUyUyRmh2N2pvTTclMkJDeEZoQmd4ZUJTMkVXVGhyV2I4aklFbkV6N1d4cyUyQnUxY2pYMlpneXViMWxGajRZdWVsaEFDaWl5VFZRaUxmaTFwdFN4dWs2emtralF6U3klMkZHcVhmQSUzRCUzRA.."/>
-    <hyperlink ref="C407" r:id="rId242" display="https://www.euromonitor.com/careers"/>
-    <hyperlink ref="C408" r:id="rId243" display="https://careers.emjreviews.com/#jobs"/>
-    <hyperlink ref="C409" r:id="rId244" display="https://euroviacareers.appellia.com/?ous="/>
-    <hyperlink ref="C410" r:id="rId245" display="https://fadel.com/careers/"/>
-    <hyperlink ref="C411" r:id="rId246" display="https://farrer.allhires.com/Default.aspx?b=l"/>
-    <hyperlink ref="C412" r:id="rId247" display="https://careers.theaccessgroup.com/jobs/"/>
-    <hyperlink ref="C413" r:id="rId248" display="https://www.filefoundation.org/careers"/>
-    <hyperlink ref="C414" r:id="rId249" display="https://www.floww.io/careers/" tooltip="https://www.floww.io/careers/"/>
-    <hyperlink ref="C415" r:id="rId250" display="https://careers.flutteruki.com/search-jobs/" tooltip="https://careers.flutteruki.com/search-jobs/"/>
-    <hyperlink ref="C416" r:id="rId251" display="https://www.fdf.org.uk/fdf/about-fdf/work-for-us/"/>
-    <hyperlink ref="C418" r:id="rId252" display="https://freesoul.teamtailor.com/jobs"/>
-    <hyperlink ref="C420" r:id="rId253" display="https://careers.fundpath.com/jobs"/>
-    <hyperlink ref="C421" r:id="rId254" display="https://gensler.wd1.myworkdayjobs.com/genslercareers"/>
-    <hyperlink ref="C422" r:id="rId255" display="https://careers.glanbia.com/search/?createNewAlert=false&amp;q=&amp;locationsearch=&amp;optionsFacetsDD_facility=&amp;optionsFacetsDD_department="/>
-    <hyperlink ref="C423" r:id="rId256" display="https://bbinsurance.wd1.myworkdayjobs.com/en-US/Careers_Europe?locationCountry=29247e57dbaf46fb855b224e03170bc7" tooltip="https://bbinsurance.wd1.myworkdayjobs.com/en-US/Careers_Europe?locationCountry=29247e57dbaf46fb855b224e03170bc7"/>
-    <hyperlink ref="C424" r:id="rId257" display="https://www.global-e.com/careers/"/>
-    <hyperlink ref="C425" r:id="rId258" display="https://corporate.graingerplc.co.uk/people-and-careers/opportunities"/>
-    <hyperlink ref="C427" r:id="rId259" display="https://recruiting.paylocity.com/recruiting/jobs/All/6c97a7d4-bb9e-4185-b871-59e5ddcf8143/Green-Street-Advisors-LLC"/>
-    <hyperlink ref="C428" r:id="rId260" display="https://careers.jobscore.com/careers/grimshawarchitects"/>
-    <hyperlink ref="C429" r:id="rId261" display="https://grosvenor.wd3.myworkdayjobs.com/External_careers_site_Grosvenor?locationCountry=29247e57dbaf46fb855b224e03170bc7" tooltip="https://grosvenor.wd3.myworkdayjobs.com/External_careers_site_Grosvenor?locationCountry=29247e57dbaf46fb855b224e03170bc7"/>
-    <hyperlink ref="C430" r:id="rId262" display="https://www.hamptons.co.uk/recruitment/vacancySearch.php#/"/>
-    <hyperlink ref="C431" r:id="rId263" display="https://www.hightekers.com/en-gb/careers"/>
-    <hyperlink ref="C432" r:id="rId264" display="https://careers.hlmarchitects.com/jobs"/>
-    <hyperlink ref="C433" r:id="rId265" display="https://iconic-sales.com/en/karriere/"/>
-    <hyperlink ref="C426" r:id="rId266" display="https://careers.ineos.com/?jobtitle=&amp;countryid=All&amp;siteid=All&amp;businessid=56&amp;Language=All"/>
-    <hyperlink ref="C417" r:id="rId267" display="https://www.intelligentchange.com/pages/careers"/>
-    <hyperlink ref="C399" r:id="rId268" display="https://careers.smartrecruiters.com/InternationalSOSGovernmentMedicalServices"/>
-    <hyperlink ref="C419" r:id="rId269" display="https://www.irbureau.com/about-irb/careers/"/>
-    <hyperlink ref="C394" r:id="rId270" display="https://isaac.hiringplatform.ca/list/isaac-jobs"/>
-    <hyperlink ref="C392" r:id="rId271" display="https://isg.wd3.myworkdayjobs.com/ISG" tooltip="https://isg.wd3.myworkdayjobs.com/ISG"/>
-    <hyperlink ref="C385" r:id="rId272" display="https://careers.itv.com/jobs"/>
-    <hyperlink ref="C382" r:id="rId273" display="https://cdpq.wd10.myworkdayjobs.com/en-US/CDPQ"/>
-    <hyperlink ref="C379" r:id="rId274" display="https://jadedldn.com/pages/careers-old"/>
-    <hyperlink ref="C359" r:id="rId275" display="https://careers.kellydeli.com/jobs" tooltip="https://careers.kellydeli.com/jobs"/>
-    <hyperlink ref="C358" r:id="rId276" display="https://careers.kennedyslaw.com/jobs/vacancy/find/results/"/>
-    <hyperlink ref="C357" r:id="rId277" display="https://fr.keycraftglobal.com/careers"/>
-    <hyperlink ref="C345" r:id="rId278" display="https://careers.kindredgroup.com/vacancy/find/results/"/>
-    <hyperlink ref="C346" r:id="rId279" display="https://kirkiss.ky/careers/"/>
-    <hyperlink ref="C434" r:id="rId280" display="https://instituteofwater.org.uk/all/institute-of-water-job-vacancy/"/>
-    <hyperlink ref="C436" r:id="rId281" display="https://lawo.softgarden.io/en/widgets/jobs" tooltip="https://lawo.softgarden.io/en/widgets/jobs"/>
-    <hyperlink ref="C437" r:id="rId282" display="https://recruiting.ultipro.com/LEG1003LGNDS/JobBoard/7cb7e3f4-053b-4339-af7b-1c62dc39bfc9/?q=&amp;o=postedDateDesc&amp;w=&amp;wc=&amp;we=&amp;wpst="/>
-    <hyperlink ref="C438" r:id="rId283" display="https://careers.lendable.com/jobs" tooltip="https://careers.lendable.com/jobs"/>
-    <hyperlink ref="C439" r:id="rId284" display="https://lhc.livevacancies.co.uk/#/"/>
-    <hyperlink ref="C440" r:id="rId285" display="https://www.lincolninternational.com/careers-and-culture/careers/experienced-professionals/"/>
-    <hyperlink ref="C442" r:id="rId286" display="https://careers.lockton.com/gb/en/browsejobs"/>
-    <hyperlink ref="C443" r:id="rId287" display="https://www.lotusbakeriesjobs.com/en/careers"/>
-    <hyperlink ref="C445" r:id="rId288" display="https://mangroupplc.wd3.myworkdayjobs.com/Man_Group_Careers"/>
-    <hyperlink ref="C446" r:id="rId289" display="https://www.marex.com/careers/"/>
-    <hyperlink ref="C447" r:id="rId290" display="https://jobs.mazars.co.uk/jobs/vacancy/find/results/"/>
-    <hyperlink ref="C448" r:id="rId291" display="https://medica.co.uk/work-with-us/careers"/>
-    <hyperlink ref="C449" r:id="rId292" display="https://www.medicaltracker.co.uk/careers"/>
-    <hyperlink ref="C450" r:id="rId293" display="https://careers.medivet.co.uk/search-jobs/" tooltip="https://careers.medivet.co.uk/search-jobs/"/>
-    <hyperlink ref="C452" r:id="rId294" display="https://www.mixtiles.com/careers#positions"/>
-    <hyperlink ref="C453" r:id="rId295" display="https://jobs.jobvite.com/monicavinader"/>
-    <hyperlink ref="C454" r:id="rId296" display="https://careers.morningstar.com/us/en/search-results"/>
-    <hyperlink ref="C455" r:id="rId297" display="https://careers.nationalexpress.com/search"/>
-    <hyperlink ref="C456" r:id="rId298" display="https://www.newcrosshealthcare.com/jobs/"/>
-    <hyperlink ref="C457" r:id="rId299" display="https://www.careers-page.com/nexgen-group"/>
-    <hyperlink ref="C458" r:id="rId300" display="https://oakfurnitureland.kallidusrecruit.com/Search.aspx"/>
-    <hyperlink ref="C459" r:id="rId301" display="https://www.jobtrain.co.uk/odeon5/Home/Job?lstRegion=&amp;chkCategory="/>
-    <hyperlink ref="C461" r:id="rId302" display="https://careers.optimahealth.co.uk/jobs/vacancy/find/results/"/>
-    <hyperlink ref="C462" r:id="rId303" display="https://optionsforsupportedliving.org/join-us/current-vacancies "/>
-    <hyperlink ref="C463" r:id="rId304" display="https://www.opus2.com/company/careers/#current-opportunities" tooltip="https://www.opus2.com/company/careers/#current-opportunities"/>
-    <hyperlink ref="C464" r:id="rId305" display="https://ordnancesurvey.wd3.myworkdayjobs.com/OS_Careers" tooltip="https://ordnancesurvey.wd3.myworkdayjobs.com/OS_Careers"/>
-    <hyperlink ref="C460" r:id="rId306" display="https://opencastsoftware.com/careers/vacancies/all-vacancies/?Commitment=&amp;Department=" tooltip="https://opencastsoftware.com/careers/vacancies/all-vacancies/?Commitment=&amp;Department="/>
-    <hyperlink ref="C465" r:id="rId307" display="https://www.outsystems.com/careers/job-list/?page=1"/>
-    <hyperlink ref="C466" r:id="rId308" display="https://harri.com/Oxygen-BXDKqMwzDPo0" tooltip="https://harri.com/Oxygen-BXDKqMwzDPo0"/>
-    <hyperlink ref="C467" r:id="rId309" display="https://pattern.wd1.myworkdayjobs.com/en-US/Pattern_Careers" tooltip="https://pattern.wd1.myworkdayjobs.com/en-US/Pattern_Careers"/>
-    <hyperlink ref="C468" r:id="rId310" display="https://pearson.jobs/jobs/" tooltip="https://pearson.jobs/jobs/"/>
-    <hyperlink ref="C471" r:id="rId311" display="https://www.playter.co/careers" tooltip="https://www.playter.co/careers"/>
-    <hyperlink ref="C472" r:id="rId312" display="https://careers.pod-point.com/#js-careers-jobs-block"/>
-    <hyperlink ref="C473" r:id="rId313" display="https://populous.com/careers#jobs" tooltip="https://populous.com/careers#jobs"/>
-    <hyperlink ref="C475" r:id="rId314" display="https://www.potawatomiventures.com/careers" tooltip="https://www.potawatomiventures.com/careers"/>
-    <hyperlink ref="C476" r:id="rId315" display="https://qudo.ai/team/" tooltip="https://qudo.ai/team/"/>
-    <hyperlink ref="C477" r:id="rId316" display="https://careers.ralphlauren.com/CareersCorporate/SearchJobsCorporate"/>
-    <hyperlink ref="C478" r:id="rId317" display="https://www.regal.co.uk/careers/" tooltip="https://www.regal.co.uk/careers/"/>
-    <hyperlink ref="C479" r:id="rId318" display="http://careers.reiss.com/" tooltip="http://careers.reiss.com/"/>
-    <hyperlink ref="C481" r:id="rId319" display="https://rlb.current-vacancies.com/Careers/RLB%20VSP-2028" tooltip="https://rlb.current-vacancies.com/Careers/RLB%20VSP-2028"/>
-    <hyperlink ref="C483" r:id="rId320" display="https://rhsocli.webitrent.com/rhsocli_webrecruitment/wrd/run/ETREC179GF.open?WVID=9962857kSa"/>
-    <hyperlink ref="C484" r:id="rId321" display="https://careers.rsgroup.com/search" tooltip="https://careers.rsgroup.com/search"/>
-    <hyperlink ref="C485" r:id="rId322" display="https://careers.rsmuk.com/uk/en/search-results"/>
-    <hyperlink ref="C486" r:id="rId323" display="https://sandersondesign.group/careers/" tooltip="https://sandersondesign.group/careers/"/>
-    <hyperlink ref="C487" r:id="rId324" display="https://sauna360.com/careers" tooltip="https://sauna360.com/careers"/>
-    <hyperlink ref="C488" r:id="rId325" display="https://careers.sb-fm.co.uk/vacancies/vacancy-search-results.aspx" tooltip="https://careers.sb-fm.co.uk/vacancies/vacancy-search-results.aspx"/>
-    <hyperlink ref="C489" r:id="rId326" display="https://seccl.tech/careers/#jobs" tooltip="https://seccl.tech/careers/#jobs"/>
-    <hyperlink ref="C490" r:id="rId327" display="https://www.servicepower.com/open-positions?hsCtaTracking=c66bea59-48b7-4539-b4db-a057ca6178d9%7Ce5504d0e-4b23-4ad2-9670-a39f13cf3dc5" tooltip="https://www.servicepower.com/open-positions?hsCtaTracking=c66bea59-48b7-4539-b4db-a057ca6178d9%7Ce5504d0e-4b23-4ad2-9670-a39f13cf3dc5"/>
-    <hyperlink ref="C491" r:id="rId328" display="https://severfield.current-vacancies.com/Careers/Severfield%20vacancy%20search%20page-2072" tooltip="https://severfield.current-vacancies.com/Careers/Severfield%20vacancy%20search%20page-2072"/>
-    <hyperlink ref="C492" r:id="rId329" display="https://www.silverdcc.com/careers/job-vacancies/"/>
-    <hyperlink ref="C494" r:id="rId330" display="https://skuuudle.bamboohr.com/careers" tooltip="https://skuuudle.bamboohr.com/careers"/>
-    <hyperlink ref="C495" r:id="rId331" display="https://careers.slaughterandmay.com/V2/Vacancy"/>
-    <hyperlink ref="C497" r:id="rId332" display="https://jobs.softcat.com/jobs/vacancy/find/results/"/>
-    <hyperlink ref="C499" r:id="rId333" display="https://careers.soprasteria.co.uk/uk/en/search-results"/>
-    <hyperlink ref="C500" r:id="rId334" display="https://jobs.lever.co/splend"/>
-    <hyperlink ref="C501" r:id="rId335" display="https://www.stace.co.uk/careers/current-opportunities/"/>
-    <hyperlink ref="C502" r:id="rId336" display="https://stlpartners.com/stl-careers/" tooltip="https://stlpartners.com/stl-careers/"/>
-    <hyperlink ref="C504" r:id="rId337" display="https://apply.workable.com/structureflow/?lng=en#jobs"/>
-    <hyperlink ref="C505" r:id="rId338" display="https://studentcribs.livevacancies.co.uk/#/"/>
-    <hyperlink ref="C506" r:id="rId339" display="https://careers.superbet.com/careers"/>
-    <hyperlink ref="C508" r:id="rId340" display="https://www.tambo.io/joinus"/>
-    <hyperlink ref="C509" r:id="rId341" display="https://careers.tangleteezer.com/jobs" tooltip="https://careers.tangleteezer.com/jobs"/>
-    <hyperlink ref="C511" r:id="rId342" display="https://careers.teemill.com/jobs" tooltip="https://careers.teemill.com/jobs"/>
-    <hyperlink ref="C512" r:id="rId343" display="https://tetratech.referrals.selectminds.com/jobs/search" tooltip="https://tetratech.referrals.selectminds.com/jobs/search"/>
-    <hyperlink ref="C513" r:id="rId344" display="https://tfpfertilitygroup.recruitee.com/"/>
-    <hyperlink ref="C514" r:id="rId345" display="https://bargrli.webitrent.com/bargrli_webrecruitment/" tooltip="https://bargrli.webitrent.com/bargrli_webrecruitment/"/>
-    <hyperlink ref="C515" r:id="rId346" display="https://www.woburn.co.uk/careers/"/>
-    <hyperlink ref="C516" r:id="rId347" display="https://ce0499li.webitrent.com/ce0499li_webrecruitment/"/>
-    <hyperlink ref="C518" r:id="rId348" display="https://www.hill.co.uk/finance-0"/>
-    <hyperlink ref="C519" r:id="rId349" display="https://theinsightsfamily.com/about/careers" tooltip="https://theinsightsfamily.com/about/careers"/>
-    <hyperlink ref="C520" r:id="rId350" display="https://thekeysupport.com/careers/?marker=fromWWWFooter"/>
-    <hyperlink ref="C521" r:id="rId351" display="https://livegroup.co.uk/recruitment-careers/" tooltip="https://livegroup.co.uk/recruitment-careers/"/>
-    <hyperlink ref="C522" r:id="rId352" display="https://www.thelondonclinic-careers.co.uk/VacancyPosting/Search#!/"/>
-    <hyperlink ref="C523" r:id="rId353" display="https://apply.workable.com/the-office-group/"/>
-    <hyperlink ref="C525" r:id="rId354" display="https://www.jobtrain.co.uk/theroyalparks/Home/Job?"/>
-    <hyperlink ref="C526" r:id="rId355" display="https://careers.thewhitecompany.com/opportunities"/>
-    <hyperlink ref="C527" r:id="rId356" display="https://threepipereply.com/careers/"/>
-    <hyperlink ref="C528" r:id="rId357" display="https://team.ticker.co.uk/"/>
-    <hyperlink ref="C529" r:id="rId358" display="https://careers.timeshighereducation.com/jobs"/>
-    <hyperlink ref="C530" r:id="rId359" display="https://www.thetonicconsultancy.com/careers"/>
-    <hyperlink ref="C531" r:id="rId360" display="https://www.toscaltd.com/en-gb/jobs/"/>
-    <hyperlink ref="C533" r:id="rId361" display="https://apply.workable.com/totallymoney/?lng=en" tooltip="https://apply.workable.com/totallymoney/?lng=en"/>
-    <hyperlink ref="C534" r:id="rId362" display="https://www.treyapartners.com/careers.html"/>
-    <hyperlink ref="C535" r:id="rId363" display="https://www.tskgroup.co.uk/careers#open"/>
-    <hyperlink ref="C536" r:id="rId364" display="https://www.turnkeyconsulting.com/careers"/>
-    <hyperlink ref="C537" r:id="rId365" display="https://www.unstudio.com/en/career"/>
-    <hyperlink ref="C538" r:id="rId366" display="https://up3.co.uk/about/servicenow-careers-with-up3/"/>
-    <hyperlink ref="C540" r:id="rId367" display="https://fullyvested.com/join-the-team/"/>
-    <hyperlink ref="C541" r:id="rId368" display="https://www.viber.com/en/careers-global/"/>
-    <hyperlink ref="C542" r:id="rId369" display="https://visualdatamedia.bamboohr.com/careers" tooltip="https://visualdatamedia.bamboohr.com/careers"/>
-    <hyperlink ref="C543" r:id="rId370" display="https://www.vitabiotics.com/pages/careers" tooltip="https://www.vitabiotics.com/pages/careers"/>
-    <hyperlink ref="C539" r:id="rId371" display="https://careers.vivobarefoot.com/jobs"/>
-    <hyperlink ref="C532" r:id="rId372" display="https://apply.workable.com/weflex-ltd/#jobs" tooltip="https://apply.workable.com/weflex-ltd/#jobs"/>
-    <hyperlink ref="C524" r:id="rId373" display="https://welbeckhealthpartners.com/careers/#careers"/>
-    <hyperlink ref="C510" r:id="rId374" display="https://westrockta.avature.net/en_US/careers/SearchJobs/" tooltip="https://westrockta.avature.net/en_US/careers/SearchJobs/"/>
-    <hyperlink ref="C507" r:id="rId375" display="https://jobs.ashbyhq.com/wonderbly.com" tooltip="https://jobs.ashbyhq.com/wonderbly.com"/>
-    <hyperlink ref="C503" r:id="rId376" display="https://worknest.com/about-us/careers/"/>
-    <hyperlink ref="C498" r:id="rId377" display="https://wowcher-1676895404.teamtailor.com/jobs"/>
-    <hyperlink ref="C496" r:id="rId378" display="https://apply.workable.com/yapily/#jobs"/>
-    <hyperlink ref="C493" r:id="rId379" display="https://yokoy.io/careers/" tooltip="https://yokoy.io/careers/"/>
-    <hyperlink ref="C482" r:id="rId380" display="https://careers.yoobic.com/jobs"/>
-    <hyperlink ref="C474" r:id="rId381" display="https://youngones.com/uk/careers/"/>
-    <hyperlink ref="C470" r:id="rId382" display="https://www.zpb-associates.com/job-opportunities" tooltip="https://www.zpb-associates.com/job-opportunities"/>
-    <hyperlink ref="C441" r:id="rId383" display="https://hoganlovells.wd3.myworkdayjobs.com/Search" tooltip="https://hoganlovells.wd3.myworkdayjobs.com/Search"/>
-    <hyperlink ref="C435" r:id="rId384" display="https://www.imperial.ac.uk/jobs/search-jobs/?searchCriteria[0][key]=LOV72&amp;searchCriteria[0][values][]=280734"/>
-    <hyperlink ref="C444" r:id="rId385" display="https://jobs.helpinghandshomecare.co.uk/search" tooltip="https://jobs.helpinghandshomecare.co.uk/search"/>
-    <hyperlink ref="C451" r:id="rId386" display="https://zyrofisher.co.uk/vacancies/" tooltip="https://zyrofisher.co.uk/vacancies/"/>
-    <hyperlink ref="C469" r:id="rId387" display="https://recruiting2.ultipro.com/PER1007PWILL/JobBoard/0ca393a4-bf82-4db6-acae-91e6a0315a4a/?q=&amp;o=postedDateDesc&amp;w=&amp;wc=&amp;we=&amp;wpst=&amp;f4=EpG9lh8U21ueW7EALgmPJw"/>
-    <hyperlink ref="C480" r:id="rId388" display="https://careers.rgp.com/Careers/SearchJobs" tooltip="https://careers.rgp.com/Careers/SearchJobs"/>
-    <hyperlink ref="C517" r:id="rId389" display="https://www.hill.co.uk/group"/>
-    <hyperlink ref="C70" r:id="rId390" display="https://unlockedgrads.org.uk/about/vacancies/#current-vacancies" tooltip="https://unlockedgrads.org.uk/about/vacancies/#current-vacancies"/>
-    <hyperlink ref="C2" r:id="rId391" display="https://careers.techwolf.ai/" tooltip="https://careers.techwolf.ai/"/>
-    <hyperlink ref="C4" r:id="rId392" display="https://mycareer.hsbc.com/en_GB/external/SearchJobs/?1017=%5B67222%2C67234%5D&amp;1017_format=812&amp;1023=%5B1248547%5D&amp;1023_format=913&amp;listFilterMode=1&amp;pipelineRecordsPerPage=10&amp;#anchor__search-jobs"/>
-    <hyperlink ref="C5" r:id="rId393" display="https://www.ardenthire.com/careers/our-careers/#"/>
-    <hyperlink ref="C6" r:id="rId394" display="https://www.biogen.com/careers/careers-search.html?country=United%2520Kingdom%2CUnited%2520States"/>
-    <hyperlink ref="C8" r:id="rId395" display="https://careerssearch.saga.co.uk/"/>
-    <hyperlink ref="C9" r:id="rId396" display="https://globalus232.dayforcehcm.com/CandidatePortal/en-US/caventures/SITE/caventurescareers"/>
-    <hyperlink ref="C10" r:id="rId397" display="https://landsecurities.wd3.myworkdayjobs.com/Landseccareers" tooltip="https://landsecurities.wd3.myworkdayjobs.com/Landseccareers"/>
-    <hyperlink ref="C11" r:id="rId398" display="https://lendlease.wd3.myworkdayjobs.com/LendleaseCareers"/>
-    <hyperlink ref="C18" r:id="rId399" display="https://careers.acco.com/go/All-ACCO-Brands-Job-Search-Results/9104500/"/>
-    <hyperlink ref="C20" r:id="rId400" display="https://acumen.org/work-with-us/" tooltip="https://acumen.org/work-with-us/"/>
-    <hyperlink ref="C21" r:id="rId401" display="https://addland.com/careers"/>
-    <hyperlink ref="C22" r:id="rId402" display="https://www.admiraljobs.co.uk/Jobs?options=26&amp;page=1"/>
-    <hyperlink ref="C31" r:id="rId403" display="https://frasers.group/careers/jobs"/>
-    <hyperlink ref="C37" r:id="rId404" display="https://alchemmy.com/careers/#positions"/>
-    <hyperlink ref="C61" r:id="rId405" display="https://career.barnebys.com/jobs"/>
-    <hyperlink ref="C78" r:id="rId406" display="https://www.veeve.com/en-gb/careers"/>
-    <hyperlink ref="C96" r:id="rId407" display="https://lwtheatres.csod.com/ux/ats/careersite/5/home?c=lwtheatres"/>
-    <hyperlink ref="C116" r:id="rId408" display="https://careers.occstrategy.com/vacancies/vacancy-search-results.aspx"/>
-    <hyperlink ref="C135" r:id="rId409" display="https://harbourvest.wd5.myworkdayjobs.com/HVP"/>
-    <hyperlink ref="C153" r:id="rId410" display="https://hgcapital.pinpointhq.com"/>
-    <hyperlink ref="C158" r:id="rId411" display="https://nordcloud.com/company/careers/"/>
-    <hyperlink ref="C162" r:id="rId412" display="https://cezanneondemand.intervieweb.it/junglecreations/en/career"/>
-    <hyperlink ref="C168" r:id="rId413" display="https://www.lenusehealth.com/careers#openings"/>
-    <hyperlink ref="C174" r:id="rId414" display="https://www.wates.co.uk/careers/vacancies/"/>
-    <hyperlink ref="C175" r:id="rId415" display="https://careers.macegroup.com/current-vacancies"/>
-    <hyperlink ref="C194" r:id="rId416" display="https://www.cvpartner.com/company/careers#join_us" tooltip="https://www.cvpartner.com/company/careers#join_us"/>
-    <hyperlink ref="C195" r:id="rId417" display="https://www.sosandar.com/careers/"/>
-    <hyperlink ref="C197" r:id="rId418" display="https://www.clarasys.com/jobs/"/>
-    <hyperlink ref="C198" r:id="rId419" display="https://www.rvu.co.uk/careers"/>
-    <hyperlink ref="C199" r:id="rId420" display="https://wd1.myworkdaysite.com/recruiting/ssctech/SSCTechnologies"/>
-    <hyperlink ref="C202" r:id="rId421" display="https://careers.roccofortehotels.com/jobs" tooltip="https://careers.roccofortehotels.com/jobs"/>
-    <hyperlink ref="C209" r:id="rId422" display="https://tapi.bamboohr.com/careers"/>
-    <hyperlink ref="C212" r:id="rId423" display="https://careers.edgardcooper.com/jobs"/>
-    <hyperlink ref="C213" r:id="rId424" display="https://hiscox.wd3.myworkdayjobs.com/Hiscox_External_Site"/>
-    <hyperlink ref="C214" r:id="rId425" display="https://www.bjss.com/careers/search"/>
-    <hyperlink ref="C217" r:id="rId426" display="https://careers.caesarstone.com/positions/"/>
-    <hyperlink ref="C228" r:id="rId427" display="https://manual.recruitee.com"/>
-    <hyperlink ref="C234" r:id="rId428" display="https://www.montacapital.com/search-jobs"/>
-    <hyperlink ref="C243" r:id="rId429" display="https://www.dartmouthpartners.com/jobs"/>
-    <hyperlink ref="C258" r:id="rId430" display="https://apply.workable.com/fergus/?lng=en#jobs"/>
-    <hyperlink ref="C261" r:id="rId431" display="https://www.accenture.com/gb-en/careers/jobsearch?jk=&amp;sb=1&amp;vw=0&amp;is_rj=0&amp;pg=1" tooltip="https://www.accenture.com/gb-en/careers/jobsearch?jk=&amp;sb=1&amp;vw=0&amp;is_rj=0&amp;pg=1"/>
-    <hyperlink ref="C273" r:id="rId432" display="https://apply.workable.com/extremereach/"/>
-    <hyperlink ref="C274" r:id="rId433" display="https://managementors.co.uk/careers/"/>
-    <hyperlink ref="C275" r:id="rId434" display="https://hillgroupuk.teamtailor.com/en-GB/jobs?utm_campaign=page_2740767_cta_21935141&amp;utm_content=https%3A//hillgroupuk.teamtailor.com&amp;utm_medium=cta-block&amp;utm_source=teamtailor-page"/>
-    <hyperlink ref="C277" r:id="rId435" display="https://careers.dazn.com/jobs/"/>
-    <hyperlink ref="C278" r:id="rId436" display="https://www.segro.com/careers/current-vacancies"/>
-    <hyperlink ref="C280" r:id="rId437" display="https://www.monument.co/careers"/>
-    <hyperlink ref="C281" r:id="rId438" display="https://www.mention-me.com/careers#roles"/>
-    <hyperlink ref="C285" r:id="rId439" display="https://www.visualsoft.co.uk/careers-overview"/>
-    <hyperlink ref="C287" r:id="rId440" display="https://careers.smartrecruiters.com/Freshworks" tooltip="https://careers.smartrecruiters.com/Freshworks"/>
-    <hyperlink ref="C316" r:id="rId441" display="https://www.native-residential.com/careers/"/>
-    <hyperlink ref="C318" r:id="rId442" display="https://careers.justeattakeaway.com/global/en/search-results?keywords=" tooltip="https://careers.justeattakeaway.com/global/en/search-results?keywords="/>
-    <hyperlink ref="C322" r:id="rId443" display="https://apply.workable.com/pensionbee/?lng=en" tooltip="https://apply.workable.com/pensionbee/?lng=en"/>
-    <hyperlink ref="C334" r:id="rId444" display="https://www.worldfirst.com/uk/careers/"/>
-    <hyperlink ref="C337" r:id="rId445" display="https://careers.sycurio.com/#jobs"/>
+    <hyperlink ref="C542" r:id="rId1" display="https://visualdatamedia.bamboohr.com/careers" tooltip="https://visualdatamedia.bamboohr.com/careers"/>
+    <hyperlink ref="C541" r:id="rId2" display="https://www.viber.com/en/careers-global/"/>
+    <hyperlink ref="C540" r:id="rId3" display="https://fullyvested.com/join-the-team/"/>
+    <hyperlink ref="C539" r:id="rId4" display="https://careers.vivobarefoot.com/jobs"/>
+    <hyperlink ref="C538" r:id="rId5" display="https://up3.co.uk/about/servicenow-careers-with-up3/"/>
+    <hyperlink ref="C537" r:id="rId6" display="https://www.unstudio.com/en/career"/>
+    <hyperlink ref="C536" r:id="rId7" display="https://www.turnkeyconsulting.com/careers"/>
+    <hyperlink ref="C535" r:id="rId8" display="https://www.tskgroup.co.uk/careers#open"/>
+    <hyperlink ref="C534" r:id="rId9" display="https://www.treyapartners.com/careers.html"/>
+    <hyperlink ref="C533" r:id="rId10" display="https://apply.workable.com/totallymoney/?lng=en" tooltip="https://apply.workable.com/totallymoney/?lng=en"/>
+    <hyperlink ref="C532" r:id="rId11" display="https://apply.workable.com/weflex-ltd/#jobs" tooltip="https://apply.workable.com/weflex-ltd/#jobs"/>
+    <hyperlink ref="C531" r:id="rId12" display="https://www.toscaltd.com/en-gb/jobs/"/>
+    <hyperlink ref="C530" r:id="rId13" display="https://www.thetonicconsultancy.com/careers"/>
+    <hyperlink ref="C529" r:id="rId14" display="https://careers.timeshighereducation.com/jobs"/>
+    <hyperlink ref="C528" r:id="rId15" display="https://team.ticker.co.uk/"/>
+    <hyperlink ref="C527" r:id="rId16" display="https://threepipereply.com/careers/"/>
+    <hyperlink ref="C526" r:id="rId17" display="https://careers.thewhitecompany.com/opportunities"/>
+    <hyperlink ref="C525" r:id="rId18" display="https://www.jobtrain.co.uk/theroyalparks/Home/Job?"/>
+    <hyperlink ref="C524" r:id="rId19" display="https://welbeckhealthpartners.com/careers/#careers"/>
+    <hyperlink ref="C523" r:id="rId20" display="https://apply.workable.com/the-office-group/"/>
+    <hyperlink ref="C522" r:id="rId21" display="https://www.thelondonclinic-careers.co.uk/VacancyPosting/Search#!/"/>
+    <hyperlink ref="C521" r:id="rId22" display="https://livegroup.co.uk/recruitment-careers/" tooltip="https://livegroup.co.uk/recruitment-careers/"/>
+    <hyperlink ref="C520" r:id="rId23" display="https://thekeysupport.com/careers/?marker=fromWWWFooter"/>
+    <hyperlink ref="C519" r:id="rId24" display="https://theinsightsfamily.com/about/careers" tooltip="https://theinsightsfamily.com/about/careers"/>
+    <hyperlink ref="C518" r:id="rId25" display="https://www.hill.co.uk/finance-0"/>
+    <hyperlink ref="C517" r:id="rId26" display="https://www.hill.co.uk/group"/>
+    <hyperlink ref="C516" r:id="rId27" display="https://ce0499li.webitrent.com/ce0499li_webrecruitment/"/>
+    <hyperlink ref="C515" r:id="rId28" display="https://www.woburn.co.uk/careers/"/>
+    <hyperlink ref="C514" r:id="rId29" display="https://bargrli.webitrent.com/bargrli_webrecruitment/" tooltip="https://bargrli.webitrent.com/bargrli_webrecruitment/"/>
+    <hyperlink ref="C513" r:id="rId30" display="https://tfpfertilitygroup.recruitee.com/"/>
+    <hyperlink ref="C512" r:id="rId31" display="https://tetratech.referrals.selectminds.com/jobs/search" tooltip="https://tetratech.referrals.selectminds.com/jobs/search"/>
+    <hyperlink ref="C511" r:id="rId32" display="https://careers.teemill.com/jobs" tooltip="https://careers.teemill.com/jobs"/>
+    <hyperlink ref="C510" r:id="rId33" display="https://westrockta.avature.net/en_US/careers/SearchJobs/" tooltip="https://westrockta.avature.net/en_US/careers/SearchJobs/"/>
+    <hyperlink ref="C509" r:id="rId34" display="https://careers.tangleteezer.com/jobs" tooltip="https://careers.tangleteezer.com/jobs"/>
+    <hyperlink ref="C508" r:id="rId35" display="https://www.tambo.io/joinus"/>
+    <hyperlink ref="C507" r:id="rId36" display="https://jobs.ashbyhq.com/wonderbly.com" tooltip="https://jobs.ashbyhq.com/wonderbly.com"/>
+    <hyperlink ref="C506" r:id="rId37" display="https://careers.superbet.com/careers"/>
+    <hyperlink ref="C505" r:id="rId38" display="https://studentcribs.livevacancies.co.uk/#/"/>
+    <hyperlink ref="C504" r:id="rId39" display="https://apply.workable.com/structureflow/?lng=en#jobs"/>
+    <hyperlink ref="C503" r:id="rId40" display="https://worknest.com/about-us/careers/"/>
+    <hyperlink ref="C502" r:id="rId41" display="https://stlpartners.com/stl-careers/" tooltip="https://stlpartners.com/stl-careers/"/>
+    <hyperlink ref="C501" r:id="rId42" display="https://www.stace.co.uk/careers/current-opportunities/"/>
+    <hyperlink ref="C500" r:id="rId43" display="https://jobs.lever.co/splend"/>
+    <hyperlink ref="C499" r:id="rId44" display="https://careers.soprasteria.co.uk/uk/en/search-results"/>
+    <hyperlink ref="C498" r:id="rId45" display="https://wowcher-1676895404.teamtailor.com/jobs"/>
+    <hyperlink ref="C497" r:id="rId46" display="https://jobs.softcat.com/jobs/vacancy/find/results/"/>
+    <hyperlink ref="C496" r:id="rId47" display="https://apply.workable.com/yapily/#jobs"/>
+    <hyperlink ref="C495" r:id="rId48" display="https://careers.slaughterandmay.com/V2/Vacancy"/>
+    <hyperlink ref="C494" r:id="rId49" display="https://skuuudle.bamboohr.com/careers" tooltip="https://skuuudle.bamboohr.com/careers"/>
+    <hyperlink ref="C493" r:id="rId50" display="https://yokoy.io/careers/" tooltip="https://yokoy.io/careers/"/>
+    <hyperlink ref="C492" r:id="rId51" display="https://www.silverdcc.com/careers/job-vacancies/"/>
+    <hyperlink ref="C491" r:id="rId52" display="https://severfield.current-vacancies.com/Careers/Severfield%20vacancy%20search%20page-2072" tooltip="https://severfield.current-vacancies.com/Careers/Severfield%20vacancy%20search%20page-2072"/>
+    <hyperlink ref="C490" r:id="rId53" display="https://www.servicepower.com/open-positions?hsCtaTracking=c66bea59-48b7-4539-b4db-a057ca6178d9%7Ce5504d0e-4b23-4ad2-9670-a39f13cf3dc5" tooltip="https://www.servicepower.com/open-positions?hsCtaTracking=c66bea59-48b7-4539-b4db-a057ca6178d9%7Ce5504d0e-4b23-4ad2-9670-a39f13cf3dc5"/>
+    <hyperlink ref="C489" r:id="rId54" display="https://seccl.tech/careers/#jobs" tooltip="https://seccl.tech/careers/#jobs"/>
+    <hyperlink ref="C488" r:id="rId55" display="https://careers.sb-fm.co.uk/vacancies/vacancy-search-results.aspx" tooltip="https://careers.sb-fm.co.uk/vacancies/vacancy-search-results.aspx"/>
+    <hyperlink ref="C487" r:id="rId56" display="https://sauna360.com/careers" tooltip="https://sauna360.com/careers"/>
+    <hyperlink ref="C486" r:id="rId57" display="https://sandersondesign.group/careers/" tooltip="https://sandersondesign.group/careers/"/>
+    <hyperlink ref="C485" r:id="rId58" display="https://careers.rsmuk.com/uk/en/search-results"/>
+    <hyperlink ref="C484" r:id="rId59" display="https://careers.rsgroup.com/search" tooltip="https://careers.rsgroup.com/search"/>
+    <hyperlink ref="C483" r:id="rId60" display="https://rhsocli.webitrent.com/rhsocli_webrecruitment/wrd/run/ETREC179GF.open?WVID=9962857kSa"/>
+    <hyperlink ref="C482" r:id="rId61" display="https://careers.yoobic.com/jobs"/>
+    <hyperlink ref="C481" r:id="rId62" display="https://rlb.current-vacancies.com/Careers/RLB%20VSP-2028" tooltip="https://rlb.current-vacancies.com/Careers/RLB%20VSP-2028"/>
+    <hyperlink ref="C480" r:id="rId63" display="https://careers.rgp.com/Careers/SearchJobs" tooltip="https://careers.rgp.com/Careers/SearchJobs"/>
+    <hyperlink ref="C479" r:id="rId64" display="http://careers.reiss.com/" tooltip="http://careers.reiss.com/"/>
+    <hyperlink ref="C478" r:id="rId65" display="https://www.regal.co.uk/careers/" tooltip="https://www.regal.co.uk/careers/"/>
+    <hyperlink ref="C477" r:id="rId66" display="https://careers.ralphlauren.com/CareersCorporate/SearchJobsCorporate"/>
+    <hyperlink ref="C476" r:id="rId67" display="https://qudo.ai/team/" tooltip="https://qudo.ai/team/"/>
+    <hyperlink ref="C475" r:id="rId68" display="https://www.potawatomiventures.com/careers" tooltip="https://www.potawatomiventures.com/careers"/>
+    <hyperlink ref="C474" r:id="rId69" display="https://youngones.com/uk/careers/"/>
+    <hyperlink ref="C473" r:id="rId70" display="https://populous.com/careers#jobs" tooltip="https://populous.com/careers#jobs"/>
+    <hyperlink ref="C472" r:id="rId71" display="https://careers.pod-point.com/#js-careers-jobs-block"/>
+    <hyperlink ref="C471" r:id="rId72" display="https://www.playter.co/careers" tooltip="https://www.playter.co/careers"/>
+    <hyperlink ref="C470" r:id="rId73" display="https://www.zpb-associates.com/job-opportunities" tooltip="https://www.zpb-associates.com/job-opportunities"/>
+    <hyperlink ref="C469" r:id="rId74" display="https://recruiting2.ultipro.com/PER1007PWILL/JobBoard/0ca393a4-bf82-4db6-acae-91e6a0315a4a/?q=&amp;o=postedDateDesc&amp;w=&amp;wc=&amp;we=&amp;wpst=&amp;f4=EpG9lh8U21ueW7EALgmPJw"/>
+    <hyperlink ref="C468" r:id="rId75" display="https://pearson.jobs/jobs/" tooltip="https://pearson.jobs/jobs/"/>
+    <hyperlink ref="C467" r:id="rId76" display="https://pattern.wd1.myworkdayjobs.com/en-US/Pattern_Careers" tooltip="https://pattern.wd1.myworkdayjobs.com/en-US/Pattern_Careers"/>
+    <hyperlink ref="C466" r:id="rId77" display="https://harri.com/Oxygen-BXDKqMwzDPo0" tooltip="https://harri.com/Oxygen-BXDKqMwzDPo0"/>
+    <hyperlink ref="C465" r:id="rId78" display="https://www.outsystems.com/careers/job-list/?page=1"/>
+    <hyperlink ref="C464" r:id="rId79" display="https://ordnancesurvey.wd3.myworkdayjobs.com/OS_Careers" tooltip="https://ordnancesurvey.wd3.myworkdayjobs.com/OS_Careers"/>
+    <hyperlink ref="C463" r:id="rId80" display="https://www.opus2.com/company/careers/#current-opportunities" tooltip="https://www.opus2.com/company/careers/#current-opportunities"/>
+    <hyperlink ref="C462" r:id="rId81" display="https://optionsforsupportedliving.org/join-us/current-vacancies "/>
+    <hyperlink ref="C461" r:id="rId82" display="https://careers.optimahealth.co.uk/jobs/vacancy/find/results/"/>
+    <hyperlink ref="C460" r:id="rId83" display="https://opencastsoftware.com/careers/vacancies/all-vacancies/?Commitment=&amp;Department=" tooltip="https://opencastsoftware.com/careers/vacancies/all-vacancies/?Commitment=&amp;Department="/>
+    <hyperlink ref="C459" r:id="rId84" display="https://www.jobtrain.co.uk/odeon5/Home/Job?lstRegion=&amp;chkCategory="/>
+    <hyperlink ref="C458" r:id="rId85" display="https://oakfurnitureland.kallidusrecruit.com/Search.aspx"/>
+    <hyperlink ref="C457" r:id="rId86" display="https://www.careers-page.com/nexgen-group"/>
+    <hyperlink ref="C456" r:id="rId87" display="https://www.newcrosshealthcare.com/jobs/"/>
+    <hyperlink ref="C455" r:id="rId88" display="https://careers.nationalexpress.com/search"/>
+    <hyperlink ref="C454" r:id="rId89" display="https://careers.morningstar.com/us/en/search-results"/>
+    <hyperlink ref="C453" r:id="rId90" display="https://jobs.jobvite.com/monicavinader"/>
+    <hyperlink ref="C452" r:id="rId91" display="https://www.mixtiles.com/careers#positions"/>
+    <hyperlink ref="C451" r:id="rId92" display="https://zyrofisher.co.uk/vacancies/" tooltip="https://zyrofisher.co.uk/vacancies/"/>
+    <hyperlink ref="C450" r:id="rId93" display="https://careers.medivet.co.uk/search-jobs/" tooltip="https://careers.medivet.co.uk/search-jobs/"/>
+    <hyperlink ref="C449" r:id="rId94" display="https://www.medicaltracker.co.uk/careers"/>
+    <hyperlink ref="C448" r:id="rId95" display="https://medica.co.uk/work-with-us/careers"/>
+    <hyperlink ref="C447" r:id="rId96" display="https://jobs.mazars.co.uk/jobs/vacancy/find/results/"/>
+    <hyperlink ref="C446" r:id="rId97" display="https://www.marex.com/careers/"/>
+    <hyperlink ref="C445" r:id="rId98" display="https://mangroupplc.wd3.myworkdayjobs.com/Man_Group_Careers"/>
+    <hyperlink ref="C444" r:id="rId99" display="https://jobs.helpinghandshomecare.co.uk/search" tooltip="https://jobs.helpinghandshomecare.co.uk/search"/>
+    <hyperlink ref="C443" r:id="rId100" display="https://www.lotusbakeriesjobs.com/en/careers"/>
+    <hyperlink ref="C442" r:id="rId101" display="https://careers.lockton.com/gb/en/browsejobs"/>
+    <hyperlink ref="C441" r:id="rId102" display="https://hoganlovells.wd3.myworkdayjobs.com/Search" tooltip="https://hoganlovells.wd3.myworkdayjobs.com/Search"/>
+    <hyperlink ref="C440" r:id="rId103" display="https://www.lincolninternational.com/careers-and-culture/careers/experienced-professionals/"/>
+    <hyperlink ref="C439" r:id="rId104" display="https://lhc.livevacancies.co.uk/#/"/>
+    <hyperlink ref="C438" r:id="rId105" display="https://careers.lendable.com/jobs" tooltip="https://careers.lendable.com/jobs"/>
+    <hyperlink ref="C437" r:id="rId106" display="https://recruiting.ultipro.com/LEG1003LGNDS/JobBoard/7cb7e3f4-053b-4339-af7b-1c62dc39bfc9/?q=&amp;o=postedDateDesc&amp;w=&amp;wc=&amp;we=&amp;wpst="/>
+    <hyperlink ref="C436" r:id="rId107" display="https://lawo.softgarden.io/en/widgets/jobs" tooltip="https://lawo.softgarden.io/en/widgets/jobs"/>
+    <hyperlink ref="C435" r:id="rId108" display="https://www.imperial.ac.uk/jobs/search-jobs/?searchCriteria[0][key]=LOV72&amp;searchCriteria[0][values][]=280734"/>
+    <hyperlink ref="C434" r:id="rId109" display="https://instituteofwater.org.uk/all/institute-of-water-job-vacancy/"/>
+    <hyperlink ref="C433" r:id="rId110" display="https://iconic-sales.com/en/karriere/"/>
+    <hyperlink ref="C432" r:id="rId111" display="https://careers.hlmarchitects.com/jobs"/>
+    <hyperlink ref="C431" r:id="rId112" display="https://www.hightekers.com/en-gb/careers"/>
+    <hyperlink ref="C430" r:id="rId113" display="https://www.hamptons.co.uk/recruitment/vacancySearch.php#/"/>
+    <hyperlink ref="C429" r:id="rId114" display="https://grosvenor.wd3.myworkdayjobs.com/External_careers_site_Grosvenor?locationCountry=29247e57dbaf46fb855b224e03170bc7" tooltip="https://grosvenor.wd3.myworkdayjobs.com/External_careers_site_Grosvenor?locationCountry=29247e57dbaf46fb855b224e03170bc7"/>
+    <hyperlink ref="C428" r:id="rId115" display="https://careers.jobscore.com/careers/grimshawarchitects"/>
+    <hyperlink ref="C427" r:id="rId116" display="https://recruiting.paylocity.com/recruiting/jobs/All/6c97a7d4-bb9e-4185-b871-59e5ddcf8143/Green-Street-Advisors-LLC"/>
+    <hyperlink ref="C426" r:id="rId117" display="https://careers.ineos.com/?jobtitle=&amp;countryid=All&amp;siteid=All&amp;businessid=56&amp;Language=All"/>
+    <hyperlink ref="C425" r:id="rId118" display="https://corporate.graingerplc.co.uk/people-and-careers/opportunities"/>
+    <hyperlink ref="C424" r:id="rId119" display="https://www.global-e.com/careers/"/>
+    <hyperlink ref="C423" r:id="rId120" display="https://bbinsurance.wd1.myworkdayjobs.com/en-US/Careers_Europe?locationCountry=29247e57dbaf46fb855b224e03170bc7" tooltip="https://bbinsurance.wd1.myworkdayjobs.com/en-US/Careers_Europe?locationCountry=29247e57dbaf46fb855b224e03170bc7"/>
+    <hyperlink ref="C422" r:id="rId121" display="https://careers.glanbia.com/search/?createNewAlert=false&amp;q=&amp;locationsearch=&amp;optionsFacetsDD_facility=&amp;optionsFacetsDD_department="/>
+    <hyperlink ref="C421" r:id="rId122" display="https://gensler.wd1.myworkdayjobs.com/genslercareers"/>
+    <hyperlink ref="C420" r:id="rId123" display="https://careers.fundpath.com/jobs"/>
+    <hyperlink ref="C419" r:id="rId124" display="https://www.irbureau.com/about-irb/careers/"/>
+    <hyperlink ref="C418" r:id="rId125" display="https://freesoul.teamtailor.com/jobs"/>
+    <hyperlink ref="C417" r:id="rId126" display="https://www.intelligentchange.com/pages/careers"/>
+    <hyperlink ref="C416" r:id="rId127" display="https://www.fdf.org.uk/fdf/about-fdf/work-for-us/"/>
+    <hyperlink ref="C415" r:id="rId128" display="https://careers.flutteruki.com/search-jobs/" tooltip="https://careers.flutteruki.com/search-jobs/"/>
+    <hyperlink ref="C414" r:id="rId129" display="https://www.floww.io/careers/" tooltip="https://www.floww.io/careers/"/>
+    <hyperlink ref="C413" r:id="rId130" display="https://www.filefoundation.org/careers"/>
+    <hyperlink ref="C412" r:id="rId131" display="https://careers.theaccessgroup.com/jobs/"/>
+    <hyperlink ref="C411" r:id="rId132" display="https://farrer.allhires.com/Default.aspx?b=l"/>
+    <hyperlink ref="C410" r:id="rId133" display="https://fadel.com/careers/"/>
+    <hyperlink ref="C409" r:id="rId134" display="https://euroviacareers.appellia.com/?ous="/>
+    <hyperlink ref="C408" r:id="rId135" display="https://careers.emjreviews.com/#jobs"/>
+    <hyperlink ref="C407" r:id="rId136" display="https://www.euromonitor.com/careers"/>
+    <hyperlink ref="C406" r:id="rId137" display="https://join.estrid.com/jobs?_gl=1*o2mc52*_gcl_au*NTQ1NjA2NDYxLjE3MjA1MzY1NDQ.*_ga*MTUwMjg1NTAyOS4xNzIwNTM2NTQ0*_fplc*SzNYUEpUcU84dCUyRkJQcGRtRmJzU3JvelRaRjhWZ2NPUyUyRmh2N2pvTTclMkJDeEZoQmd4ZUJTMkVXVGhyV2I4aklFbkV6N1d4cyUyQnUxY2pYMlpneXViMWxGajRZdWVsaEFDaWl5VFZRaUxmaTFwdFN4dWs2emtralF6U3klMkZHcVhmQSUzRCUzRA.."/>
+    <hyperlink ref="C405" r:id="rId138" display="https://equiteq.careers.hibob.com/" tooltip="https://equiteq.careers.hibob.com/"/>
+    <hyperlink ref="C404" r:id="rId139" display="https://equita.co.uk/about-us/work-with-us/"/>
+    <hyperlink ref="C403" r:id="rId140" display="https://eo-group.co.uk/opportunities/"/>
+    <hyperlink ref="C402" r:id="rId141" display="https://careers.ensek.com/" tooltip="https://careers.ensek.com/"/>
+    <hyperlink ref="C401" r:id="rId142" display="https://careers.enginuity.org/jobs"/>
+    <hyperlink ref="C400" r:id="rId143" display="https://empiricstudentpropertyplc.talosats-careers.com/vacancies"/>
+    <hyperlink ref="C399" r:id="rId144" display="https://careers.smartrecruiters.com/InternationalSOSGovernmentMedicalServices"/>
+    <hyperlink ref="C398" r:id="rId145" display="https://careers-dwfgroup.icims.com/jobs/search?hashed=-625886029&amp;mobile=false&amp;width=1011&amp;height=500&amp;bga=true&amp;needsRedirect=false&amp;jan1offset=0&amp;jun1offset=60" tooltip="https://careers-dwfgroup.icims.com/jobs/search?hashed=-625886029&amp;mobile=false&amp;width=1011&amp;height=500&amp;bga=true&amp;needsRedirect=false&amp;jan1offset=0&amp;jun1offset=60"/>
+    <hyperlink ref="C397" r:id="rId146" display="https://careers.dufry.com/go/Dufry-Main/9035601/"/>
+    <hyperlink ref="C396" r:id="rId147" display="https://drdoctor.teamtailor.com/jobs" tooltip="https://drdoctor.teamtailor.com/jobs"/>
+    <hyperlink ref="C395" r:id="rId148" display="https://downing.com/work-for-us/#work-for-us-6"/>
+    <hyperlink ref="C394" r:id="rId149" display="https://isaac.hiringplatform.ca/list/isaac-jobs"/>
+    <hyperlink ref="C393" r:id="rId150" display="https://apply.workable.com/demellier-ltd/?lng=en"/>
+    <hyperlink ref="C392" r:id="rId151" display="https://isg.wd3.myworkdayjobs.com/ISG" tooltip="https://isg.wd3.myworkdayjobs.com/ISG"/>
+    <hyperlink ref="C391" r:id="rId152" display="https://www.dechert.com/careers.html"/>
+    <hyperlink ref="C390" r:id="rId153" display="https://careers.dcc.ie/dccvital/search/"/>
+    <hyperlink ref="C389" r:id="rId154" display="https://datatonic.com/careers/vacancies/" tooltip="https://datatonic.com/careers/vacancies/"/>
+    <hyperlink ref="C388" r:id="rId155" display="https://www.dae.mn/openings"/>
+    <hyperlink ref="C387" r:id="rId156" display="https://www.redpincompany.com/careers?department=&amp;location=&amp;company=currencies-direct&amp;page=1"/>
+    <hyperlink ref="C386" r:id="rId157" display="https://cumminggroup.wd1.myworkdayjobs.com/CGC" tooltip="https://cumminggroup.wd1.myworkdayjobs.com/CGC"/>
+    <hyperlink ref="C385" r:id="rId158" display="https://careers.itv.com/jobs"/>
+    <hyperlink ref="C384" r:id="rId159" display="https://www.csl-group.com/uk/careers/"/>
+    <hyperlink ref="C383" r:id="rId160" display="https://globaleur242.dayforcehcm.com/CandidatePortal/en-GB/crippspeople/" tooltip="https://globaleur242.dayforcehcm.com/CandidatePortal/en-GB/crippspeople/"/>
+    <hyperlink ref="C382" r:id="rId161" display="https://cdpq.wd10.myworkdayjobs.com/en-US/CDPQ"/>
+    <hyperlink ref="C381" r:id="rId162" display="https://crawfordtech.pinpointhq.com/#js-careers-jobs-block"/>
+    <hyperlink ref="C380" r:id="rId163" display="https://www.couvertureandthegarbstore.com/pages/careers"/>
+    <hyperlink ref="C379" r:id="rId164" display="https://jadedldn.com/pages/careers-old"/>
+    <hyperlink ref="C378" r:id="rId165" display="https://fsr.cvmailuk.com/clydecocareers/main.cfm?page=jobBoard&amp;fo=1&amp;groupType_21=&amp;groupType_33=&amp;filter=&amp;srxksl=1"/>
+    <hyperlink ref="C377" r:id="rId166" display="https://www.clubmedjobs.com/en/search-jobs/" tooltip="https://www.clubmedjobs.com/en/search-jobs/"/>
+    <hyperlink ref="C376" r:id="rId167" display="https://work-clockwise.com/careers/"/>
+    <hyperlink ref="C375" r:id="rId168" display="https://jobs.cliffordchance.com/jobs?options=49,58&amp;page=1"/>
+    <hyperlink ref="C374" r:id="rId169" display="https://cipfa.teamtailor.com/jobs?query="/>
+    <hyperlink ref="C373" r:id="rId170" display="https://cinchona.com/careers/"/>
+    <hyperlink ref="C372" r:id="rId171" display="https://careers.churchdwight.com/jobs/?search=&amp;country=GBR&amp;location=&amp;team=&amp;position=&amp;type="/>
+    <hyperlink ref="C371" r:id="rId172" display="https://www.careers-page.com/chelsea-peers#openings" tooltip="https://www.careers-page.com/chelsea-peers#openings"/>
+    <hyperlink ref="C370" r:id="rId173" display="https://www.channelbakers.com/careers" tooltip="https://www.channelbakers.com/careers"/>
+    <hyperlink ref="C369" r:id="rId174" display="https://www.celigo.com/careers/#job-listings"/>
+    <hyperlink ref="C368" r:id="rId175" display="https://www.cartwrightpickard.com/careers"/>
+    <hyperlink ref="C367" r:id="rId176" display="https://camillaelphick.com/pages/careers-1" tooltip="https://camillaelphick.com/pages/careers-1"/>
+    <hyperlink ref="C366" r:id="rId177" display="https://careers.oniverse.it/en-GB/home"/>
+    <hyperlink ref="C365" r:id="rId178" display="https://jobs.lever.co/moonpig"/>
+    <hyperlink ref="C364" r:id="rId179" display="https://www.burtonsbiscuits.com/life-at-burtons/current-vacancies/burton-s-bakeries/"/>
+    <hyperlink ref="C363" r:id="rId180" display="https://www.broadwaymalyan.com/people/vacancies/"/>
+    <hyperlink ref="C362" r:id="rId181" display="https://workfor.brightnetwork.co.uk/join-us"/>
+    <hyperlink ref="C361" r:id="rId182" display="https://careers.boohoogroup.com/search-jobs"/>
+    <hyperlink ref="C360" r:id="rId183" display="https://baicommunications.wd3.myworkdayjobs.com/External"/>
+    <hyperlink ref="C359" r:id="rId184" display="https://careers.kellydeli.com/jobs" tooltip="https://careers.kellydeli.com/jobs"/>
+    <hyperlink ref="C358" r:id="rId185" display="https://careers.kennedyslaw.com/jobs/vacancy/find/results/"/>
+    <hyperlink ref="C357" r:id="rId186" display="https://fr.keycraftglobal.com/careers"/>
+    <hyperlink ref="C356" r:id="rId187" display="https://big.dk/careers"/>
+    <hyperlink ref="C355" r:id="rId188" display="https://bespoke-bids.com/careers/"/>
+    <hyperlink ref="C354" r:id="rId189" display="https://job-boards.eu.greenhouse.io/theberkeleypartnership" tooltip="https://job-boards.eu.greenhouse.io/theberkeleypartnership"/>
+    <hyperlink ref="C353" r:id="rId190" display="https://www.bellaandduke.com/join-our-team/" tooltip="https://www.bellaandduke.com/join-our-team/"/>
+    <hyperlink ref="C352" r:id="rId191" display="https://baringa.csod.com/ux/ats/careersite/4/home?c=baringa" tooltip="https://baringa.csod.com/ux/ats/careersite/4/home?c=baringa"/>
+    <hyperlink ref="C351" r:id="rId192" display="https://www.barbican.org.uk/our-story/about-us/careers"/>
+    <hyperlink ref="C350" r:id="rId193" display="https://aztec.group/us/careers/current-vacancies/"/>
+    <hyperlink ref="C349" r:id="rId194" display="https://arthur.co.uk/live-jobs/" tooltip="https://arthur.co.uk/live-jobs/"/>
+    <hyperlink ref="C348" r:id="rId195" display="https://recruiting.ultipro.com/AME1095ACHM/JobBoard/c52f9a39-fdc5-4ae2-9eaf-cb8a7bda923e/?q=&amp;o=postedDateDesc&amp;w=&amp;wc=&amp;we=&amp;wpst="/>
+    <hyperlink ref="C347" r:id="rId196" display="https://jobs.amadeuscapital.com/"/>
+    <hyperlink ref="C346" r:id="rId197" display="https://kirkiss.ky/careers/"/>
+    <hyperlink ref="C345" r:id="rId198" display="https://careers.kindredgroup.com/vacancy/find/results/"/>
+    <hyperlink ref="C343" r:id="rId199" display="https://careers.7im.co.uk/vacancies/vacancy-search-results.aspx"/>
+    <hyperlink ref="C342" r:id="rId200" display="https://www.11fs.com/careers/vacancies" tooltip="https://www.11fs.com/careers/vacancies"/>
+    <hyperlink ref="C341" r:id="rId201" display="https://polestar.teamtailor.com/jobs"/>
+    <hyperlink ref="C340" r:id="rId202" display="https://www.gwi.com/careers#job-list"/>
+    <hyperlink ref="C339" r:id="rId203" display="https://channel3consulting.co.uk/work-with-us/careers/"/>
+    <hyperlink ref="C338" r:id="rId204" display="https://fa-evng-saasfaprod1.fa.ocs.oraclecloud.com/hcmUI/CandidateExperience/en/sites/LBWF/requisitions?location=United+Kingdom&amp;locationId=300000000471661&amp;locationLevel=country&amp;mode=location"/>
+    <hyperlink ref="C337" r:id="rId205" display="https://careers.sycurio.com/#jobs"/>
+    <hyperlink ref="C336" r:id="rId206" display="https://careers.captify.co.uk/#jobs"/>
+    <hyperlink ref="C335" r:id="rId207" display="https://careers.northhighland.com/jobs/" tooltip="https://careers.northhighland.com/jobs/"/>
+    <hyperlink ref="C334" r:id="rId208" display="https://www.worldfirst.com/uk/careers/"/>
+    <hyperlink ref="C328" r:id="rId209" display="https://www.envitia.com/careers/job-opportunities/"/>
+    <hyperlink ref="C327" r:id="rId210" display="https://hdfg.fa.em3.oraclecloud.com/hcmUI/CandidateExperience/en/sites/CX/requisitions?mode=location"/>
+    <hyperlink ref="C326" r:id="rId211" display="https://jobs.ashbyhq.com/metaview"/>
+    <hyperlink ref="C325" r:id="rId212" display="https://jll.wd1.myworkdayjobs.com/jllcareers"/>
+    <hyperlink ref="C322" r:id="rId213" display="https://apply.workable.com/pensionbee/?lng=en" tooltip="https://apply.workable.com/pensionbee/?lng=en"/>
+    <hyperlink ref="C321" r:id="rId214" display="https://shieldpay.teamtailor.com/jobs"/>
+    <hyperlink ref="C319" r:id="rId215" display="https://join.modsquad.com/careers/"/>
+    <hyperlink ref="C318" r:id="rId216" display="https://careers.justeattakeaway.com/global/en/search-results?keywords=" tooltip="https://careers.justeattakeaway.com/global/en/search-results?keywords="/>
+    <hyperlink ref="C317" r:id="rId217" display="https://vistaglobal.com/careers/" tooltip="https://vistaglobal.com/careers/"/>
+    <hyperlink ref="C316" r:id="rId218" display="https://www.native-residential.com/careers/"/>
+    <hyperlink ref="C315" r:id="rId219" display="https://www.harrodscareers.com/jobs" tooltip="https://www.harrodscareers.com/jobs"/>
+    <hyperlink ref="C312" r:id="rId220" display="https://hyve.group/lifeathyve/join-our-team/" tooltip="https://hyve.group/lifeathyve/join-our-team/"/>
+    <hyperlink ref="C311" r:id="rId221" display="https://www.amazon.jobs/content/en/teams/amazon-entertainment/music?country%5B%5D=US&amp;country%5B%5D=GB"/>
+    <hyperlink ref="C309" r:id="rId222" display="https://careers.legalandgeneral.com/jobs?options=203"/>
+    <hyperlink ref="C308" r:id="rId223" display="https://harri.com/The-Delaunay-BYtcttE0b35i" tooltip="https://harri.com/The-Delaunay-BYtcttE0b35i"/>
+    <hyperlink ref="C307" r:id="rId224" display="https://milltechfx.com/company/careers/"/>
+    <hyperlink ref="C306" r:id="rId225" display="https://www.charliehr.com/careers#Vacancies" tooltip="https://www.charliehr.com/careers#Vacancies"/>
+    <hyperlink ref="C303" r:id="rId226" display="https://careers.lta.org.uk/vacancies/vacancy-search-results.aspx?_gl=1*1u8zpgc*_ga*MzA5NzUyNjgzLjE3MTIzMDg0Njc.*_ga_R8CDFT1V4H*MTcxMjMwODQ2Ny4xLjAuMTcxMjMwODQ2Ny42MC4wLjA." tooltip="https://careers.lta.org.uk/vacancies/vacancy-search-results.aspx?_gl=1*1u8zpgc*_ga*MzA5NzUyNjgzLjE3MTIzMDg0Njc.*_ga_R8CDFT1V4H*MTcxMjMwODQ2Ny4xLjAuMTcxMjMwODQ2Ny42MC4wLjA."/>
+    <hyperlink ref="C301" r:id="rId227" display="https://ts.wd5.myworkdayjobs.com/en-US/tishmanspeyer"/>
+    <hyperlink ref="C298" r:id="rId228" display="https://www.realestate.bnpparibas.co.uk/find-job"/>
+    <hyperlink ref="C297" r:id="rId229" display="https://apply.workable.com/gohenry/" tooltip="https://apply.workable.com/gohenry/"/>
+    <hyperlink ref="C296" r:id="rId230" display="https://dt-consulting.com/open-positions/" tooltip="https://dt-consulting.com/open-positions/"/>
+    <hyperlink ref="C294" r:id="rId231" display="https://app.otta.com/companies/GetHarley#company-mission-section" tooltip="https://app.otta.com/companies/GetHarley#company-mission-section"/>
+    <hyperlink ref="C293" r:id="rId232" display="https://www.kkr.com/careers/career-opportunities"/>
+    <hyperlink ref="C291" r:id="rId233" display="https://apply.workable.com/koothjobs/" tooltip="https://apply.workable.com/koothjobs/"/>
+    <hyperlink ref="C290" r:id="rId234" display="https://www.tilda.com/about-us/careers/" tooltip="https://www.tilda.com/about-us/careers/"/>
+    <hyperlink ref="C288" r:id="rId235" display="https://boards.eu.greenhouse.io/bitpanda"/>
+    <hyperlink ref="C287" r:id="rId236" display="https://careers.smartrecruiters.com/Freshworks" tooltip="https://careers.smartrecruiters.com/Freshworks"/>
+    <hyperlink ref="C285" r:id="rId237" display="https://www.visualsoft.co.uk/careers-overview"/>
+    <hyperlink ref="C284" r:id="rId238" display="https://thecrownestate.teamtailor.com/jobs"/>
+    <hyperlink ref="C282" r:id="rId239" display="https://www.speechmatics.com/company/careers/roles"/>
+    <hyperlink ref="C281" r:id="rId240" display="https://www.mention-me.com/careers#roles"/>
+    <hyperlink ref="C280" r:id="rId241" display="https://www.monument.co/careers"/>
+    <hyperlink ref="C278" r:id="rId242" display="https://www.segro.com/careers/current-vacancies"/>
+    <hyperlink ref="C277" r:id="rId243" display="https://careers.dazn.com/jobs/"/>
+    <hyperlink ref="C275" r:id="rId244" display="https://hillgroupuk.teamtailor.com/en-GB/jobs?utm_campaign=page_2740767_cta_21935141&amp;utm_content=https%3A//hillgroupuk.teamtailor.com&amp;utm_medium=cta-block&amp;utm_source=teamtailor-page"/>
+    <hyperlink ref="C274" r:id="rId245" display="https://managementors.co.uk/careers/"/>
+    <hyperlink ref="C273" r:id="rId246" display="https://apply.workable.com/extremereach/"/>
+    <hyperlink ref="C272" r:id="rId247" display="https://www.doddgroup.com/jobs"/>
+    <hyperlink ref="C269" r:id="rId248" display="https://www.tussell.com/careers#jobs" tooltip="https://www.tussell.com/careers#jobs"/>
+    <hyperlink ref="C265" r:id="rId249" display="https://careers.learnatnoon.com/jobs"/>
+    <hyperlink ref="C264" r:id="rId250" display="https://www.capitalontap.com/en/company/careers/#careers-jobs"/>
+    <hyperlink ref="C261" r:id="rId251" display="https://www.accenture.com/gb-en/careers/jobsearch?jk=&amp;sb=1&amp;vw=0&amp;is_rj=0&amp;pg=1" tooltip="https://www.accenture.com/gb-en/careers/jobsearch?jk=&amp;sb=1&amp;vw=0&amp;is_rj=0&amp;pg=1"/>
+    <hyperlink ref="C259" r:id="rId252" display="https://www.busybeerecruitment.co.uk/vacancies"/>
+    <hyperlink ref="C258" r:id="rId253" display="https://apply.workable.com/fergus/?lng=en#jobs"/>
+    <hyperlink ref="C256" r:id="rId254" display="https://jobs.lever.co/enable"/>
+    <hyperlink ref="C254" r:id="rId255" display="https://www.elixirr.com/en-gb/job-openings/" tooltip="https://www.elixirr.com/en-gb/job-openings/"/>
+    <hyperlink ref="C253" r:id="rId256" display="https://thelostestate.com/jobs/"/>
+    <hyperlink ref="C251" r:id="rId257" display="https://www.efficioconsulting.com/en-gb/careers/apply/" tooltip="https://www.efficioconsulting.com/en-gb/careers/apply/"/>
+    <hyperlink ref="C250" r:id="rId258" display="https://mileway.com/careers/opportunities/"/>
+    <hyperlink ref="C246" r:id="rId259" display="https://careers.marshmclennan.com/global/en/oliver-wyman-search"/>
+    <hyperlink ref="C244" r:id="rId260" display="https://www.thredd.com/about-us/careers/vacancies"/>
+    <hyperlink ref="C243" r:id="rId261" display="https://www.dartmouthpartners.com/jobs"/>
+    <hyperlink ref="C242" r:id="rId262" display="https://www.neudata.co/careers#Jobs"/>
+    <hyperlink ref="C241" r:id="rId263" display="https://www.constellationcold.com/vacancies/"/>
+    <hyperlink ref="C240" r:id="rId264" display="https://natterbox.com/careers/"/>
+    <hyperlink ref="C239" r:id="rId265" display="https://careers.upmc.com/job-search-results/" tooltip="https://careers.upmc.com/job-search-results/"/>
+    <hyperlink ref="C238" r:id="rId266" display="https://jobs.greystar.com/search-jobs/" tooltip="https://jobs.greystar.com/search-jobs/"/>
+    <hyperlink ref="C237" r:id="rId267" display="https://www.newscareers.co.uk/vacancies/vacancy-search-results.aspx" tooltip="https://www.newscareers.co.uk/vacancies/vacancy-search-results.aspx"/>
+    <hyperlink ref="C236" r:id="rId268" display="https://www.mollymaid.co.uk/working-for-molly-maid/"/>
+    <hyperlink ref="C235" r:id="rId269" display="https://turo.com/gb/en/careers#job_openings" tooltip="https://turo.com/gb/en/careers#job_openings"/>
+    <hyperlink ref="C234" r:id="rId270" display="https://www.montacapital.com/search-jobs"/>
+    <hyperlink ref="C233" r:id="rId271" display="https://cmcmarkets.wd3.myworkdayjobs.com/CMC_Markets_Careers"/>
+    <hyperlink ref="C232" r:id="rId272" display="https://thegymgroup.wd3.myworkdayjobs.com/TGG_External_Career_Site" tooltip="https://thegymgroup.wd3.myworkdayjobs.com/TGG_External_Career_Site"/>
+    <hyperlink ref="C231" r:id="rId273" display="https://www.family-institute.org/about-us/careers"/>
+    <hyperlink ref="C230" r:id="rId274" display="https://faculty.ai/join-the-team/#ashby_embed"/>
+    <hyperlink ref="C229" r:id="rId275" display="https://careers.deliveroo.co.uk/jobs/" tooltip="https://careers.deliveroo.co.uk/jobs/"/>
+    <hyperlink ref="C228" r:id="rId276" display="https://manual.recruitee.com"/>
+    <hyperlink ref="C227" r:id="rId277" display="https://careers.telegraph.co.uk/jobs/job-search?location=London"/>
+    <hyperlink ref="C226" r:id="rId278" display="https://www.lhh.com/uk/en/search-jobs/"/>
+    <hyperlink ref="C224" r:id="rId279" display="https://www.theaacareers.co.uk/apply/?s_Keywords="/>
+    <hyperlink ref="C223" r:id="rId280" display="https://jobs.decathlon.co.uk/go/View-all-Jobs/4978001/"/>
+    <hyperlink ref="C222" r:id="rId281" display="https://partners.bridebook.com/uk/careers#openroles"/>
+    <hyperlink ref="C220" r:id="rId282" display="https://freetrade.io/careers#job-openings"/>
+    <hyperlink ref="C218" r:id="rId283" display="https://job-boards.greenhouse.io/fountain"/>
+    <hyperlink ref="C217" r:id="rId284" display="https://careers.caesarstone.com/positions/"/>
+    <hyperlink ref="C216" r:id="rId285" display="https://ryman.ats.emea1.fourth.com"/>
+    <hyperlink ref="C215" r:id="rId286" display="https://www.scandit.com/careers/current-openings/" tooltip="https://www.scandit.com/careers/current-openings/"/>
+    <hyperlink ref="C214" r:id="rId287" display="https://www.bjss.com/careers/search"/>
+    <hyperlink ref="C213" r:id="rId288" display="https://hiscox.wd3.myworkdayjobs.com/Hiscox_External_Site"/>
+    <hyperlink ref="C212" r:id="rId289" display="https://careers.edgardcooper.com/jobs"/>
+    <hyperlink ref="C211" r:id="rId290" display="https://careers.lightricks.com/careers"/>
+    <hyperlink ref="C210" r:id="rId291" display="https://www.kpmgcareers.co.uk/search/" tooltip="https://www.kpmgcareers.co.uk/search/"/>
+    <hyperlink ref="C209" r:id="rId292" display="https://tapi.bamboohr.com/careers"/>
+    <hyperlink ref="C208" r:id="rId293" display="https://apply.monsoonjobs.com/search_and_apply/vacancies/" tooltip="https://apply.monsoonjobs.com/search_and_apply/vacancies/"/>
+    <hyperlink ref="C207" r:id="rId294" display="https://jobs.thecignagroup.com/us/en/search-results" tooltip="https://jobs.thecignagroup.com/us/en/search-results"/>
+    <hyperlink ref="C206" r:id="rId295" display="https://greshamhouse.com/join-our-team/"/>
+    <hyperlink ref="C202" r:id="rId296" display="https://careers.roccofortehotels.com/jobs" tooltip="https://careers.roccofortehotels.com/jobs"/>
+    <hyperlink ref="C199" r:id="rId297" display="https://wd1.myworkdaysite.com/recruiting/ssctech/SSCTechnologies"/>
+    <hyperlink ref="C198" r:id="rId298" display="https://www.rvu.co.uk/careers"/>
+    <hyperlink ref="C197" r:id="rId299" display="https://www.clarasys.com/jobs/"/>
+    <hyperlink ref="C195" r:id="rId300" display="https://www.sosandar.com/careers/"/>
+    <hyperlink ref="C194" r:id="rId301" display="https://www.cvpartner.com/company/careers#join_us" tooltip="https://www.cvpartner.com/company/careers#join_us"/>
+    <hyperlink ref="C192" r:id="rId302" display="https://jobs.yougov.com/jobs"/>
+    <hyperlink ref="C188" r:id="rId303" display="https://www.ospreycharging.co.uk/careers-at-osprey-charging"/>
+    <hyperlink ref="C187" r:id="rId304" display="https://ichoosr.recruitee.com/"/>
+    <hyperlink ref="C183" r:id="rId305" display="https://montaguevans.jibeapply.com/careers-home/jobs?keywords=&amp;location=&amp;page=1&amp;sortBy=relevance&amp;limit=100"/>
+    <hyperlink ref="C181" r:id="rId306" display="https://careers.cbre.com/en_US/careers/SearchJobs/?9577=%5B17276%2C17117%5D&amp;9577_format=10224&amp;listFilterMode=1&amp;jobSort=relevancy&amp;jobRecordsPerPage=25&amp;" tooltip="https://careers.cbre.com/en_US/careers/SearchJobs/?9577=%5B17276%2C17117%5D&amp;9577_format=10224&amp;listFilterMode=1&amp;jobSort=relevancy&amp;jobRecordsPerPage=25&amp;"/>
+    <hyperlink ref="C180" r:id="rId307" display="https://www.verkeer.co/about-us/careers/"/>
+    <hyperlink ref="C179" r:id="rId308" display="https://volarisgroup.wd3.myworkdayjobs.com/CompanyWatch" tooltip="https://volarisgroup.wd3.myworkdayjobs.com/CompanyWatch"/>
+    <hyperlink ref="C178" r:id="rId309" display="https://boards.eu.greenhouse.io/convera/"/>
+    <hyperlink ref="C177" r:id="rId310" display="https://boards.greenhouse.io/heycar/"/>
+    <hyperlink ref="C176" r:id="rId311" display="https://careers.scienceinsport.com/jobs"/>
+    <hyperlink ref="C175" r:id="rId312" display="https://careers.macegroup.com/current-vacancies"/>
+    <hyperlink ref="C174" r:id="rId313" display="https://www.wates.co.uk/careers/vacancies/"/>
+    <hyperlink ref="C173" r:id="rId314" display="https://careers.phished.io/l/en" tooltip="https://careers.phished.io/l/en"/>
+    <hyperlink ref="C172" r:id="rId315" display="https://jajafinance.bamboohr.com/careers" tooltip="https://jajafinance.bamboohr.com/careers"/>
+    <hyperlink ref="C171" r:id="rId316" display="https://www.quantexa.com/careers/vacancies/" tooltip="https://www.quantexa.com/careers/vacancies/"/>
+    <hyperlink ref="C170" r:id="rId317" display="https://clear.bank/join-clearbank/careers"/>
+    <hyperlink ref="C168" r:id="rId318" display="https://www.lenusehealth.com/careers#openings"/>
+    <hyperlink ref="C167" r:id="rId319" display="https://www.semble.io/careers" tooltip="https://www.semble.io/careers"/>
+    <hyperlink ref="C166" r:id="rId320" display="https://careers.savills.com/jobs"/>
+    <hyperlink ref="C165" r:id="rId321" display="https://www.connellsgroup.co.uk/careers/job-search/?radius=5&amp;page=1&amp;sort=posted&amp;direction=desc" tooltip="https://www.connellsgroup.co.uk/careers/job-search/?radius=5&amp;page=1&amp;sort=posted&amp;direction=desc"/>
+    <hyperlink ref="C164" r:id="rId322" display="https://jobs.reachplc.com/jobs"/>
+    <hyperlink ref="C162" r:id="rId323" display="https://cezanneondemand.intervieweb.it/junglecreations/en/career"/>
+    <hyperlink ref="C161" r:id="rId324" display="https://jobs.petscorner.co.uk/job-list/"/>
+    <hyperlink ref="C160" r:id="rId325" display="https://www.turnerandtownsend.com/en/careers/apply-now/"/>
+    <hyperlink ref="C159" r:id="rId326" display="https://www.downing.co.uk/careers#open-positions"/>
+    <hyperlink ref="C158" r:id="rId327" display="https://nordcloud.com/company/careers/"/>
+    <hyperlink ref="C157" r:id="rId328" display="https://hymans.current-vacancies.com/Careers/Hymans%20external%20VSP-2054#"/>
+    <hyperlink ref="C156" r:id="rId329" display="https://profinda.bamboohr.com/careers" tooltip="https://profinda.bamboohr.com/careers"/>
+    <hyperlink ref="C154" r:id="rId330" display="https://www.palantir.com/careers/#open-positions" tooltip="https://www.palantir.com/careers/#open-positions"/>
+    <hyperlink ref="C153" r:id="rId331" display="https://hgcapital.pinpointhq.com"/>
+    <hyperlink ref="C152" r:id="rId332" display="https://patchwork.teamtailor.com/jobs" tooltip="https://patchwork.teamtailor.com/jobs"/>
+    <hyperlink ref="C151" r:id="rId333" display="https://careers.domesticandgeneral.com/search-jobs/"/>
+    <hyperlink ref="C150" r:id="rId334" display="https://channel3consulting.livevacancies.co.uk/jobsIframe" tooltip="https://channel3consulting.livevacancies.co.uk/jobsIframe"/>
+    <hyperlink ref="C149" r:id="rId335" display="https://www.iabuk.com/vacancies" tooltip="https://www.iabuk.com/vacancies"/>
+    <hyperlink ref="C148" r:id="rId336" display="https://www.freddiesflowers.com/about-us/jobs#openings"/>
+    <hyperlink ref="C146" r:id="rId337" display="https://jobs.pphe.com/careers/?country=united-kingdom" tooltip="https://jobs.pphe.com/careers/?country=united-kingdom"/>
+    <hyperlink ref="C145" r:id="rId338" display="https://jobs.amundi.com/homepage.aspx?LCID=2057" tooltip="https://jobs.amundi.com/homepage.aspx?LCID=2057"/>
+    <hyperlink ref="C144" r:id="rId339" display="https://www.capgemini.com/gb-en/careers/join-us/" tooltip="https://www.capgemini.com/gb-en/careers/join-us/"/>
+    <hyperlink ref="C143" r:id="rId340" display="https://www.oka.com/uk/careers/opportunities"/>
+    <hyperlink ref="C142" r:id="rId341" display="https://www.industrialsreit.com/careers"/>
+    <hyperlink ref="C141" r:id="rId342" display="https://www.naturalhr.net/hr/recruitment/roles/8279302e80a62ccde7ee587a4f382535"/>
+    <hyperlink ref="C140" r:id="rId343" display="https://www.peldonrose.com/about/jobs" tooltip="https://www.peldonrose.com/about/jobs"/>
+    <hyperlink ref="C139" r:id="rId344" display="https://pelorusx.co/about/careers" tooltip="https://pelorusx.co/about/careers"/>
+    <hyperlink ref="C138" r:id="rId345" display="https://workingatedge.com/careers/"/>
+    <hyperlink ref="C137" r:id="rId346" display="https://careers.ovo.com/opportunities "/>
+    <hyperlink ref="C136" r:id="rId347" display="https://www.yonder.com/careers#open-positions"/>
+    <hyperlink ref="C135" r:id="rId348" display="https://harbourvest.wd5.myworkdayjobs.com/HVP"/>
+    <hyperlink ref="C134" r:id="rId349" display="https://jobs.ashbyhq.com/myurbanjungle.com" tooltip="https://jobs.ashbyhq.com/myurbanjungle.com"/>
+    <hyperlink ref="C132" r:id="rId350" display="https://careers.cynergybank.co.uk/jobs?location=London"/>
+    <hyperlink ref="C131" r:id="rId351" display="https://symphony.com/company/careers/"/>
+    <hyperlink ref="C130" r:id="rId352" display="https://apply.workable.com/starling-bank/#jobs"/>
+    <hyperlink ref="C128" r:id="rId353" display="https://supercharge.io/careers/positions"/>
+    <hyperlink ref="C127" r:id="rId354" display="https://impact.com/careers/#global-opportunities"/>
+    <hyperlink ref="C126" r:id="rId355" display="https://www.workspace.co.uk/job-vacancies" tooltip="https://www.workspace.co.uk/job-vacancies"/>
+    <hyperlink ref="C124" r:id="rId356" display="https://www.thoughtworks.com/en-gb/careers" tooltip="https://www.thoughtworks.com/en-gb/careers"/>
+    <hyperlink ref="C123" r:id="rId357" display="https://apply.workable.com/fenergocareers/"/>
+    <hyperlink ref="C122" r:id="rId358" display="https://munichre-jobs.com/en/MunichRe"/>
+    <hyperlink ref="C121" r:id="rId359" display="https://www.simplybusiness.co.uk/about-us/careers/jobs/" tooltip="https://www.simplybusiness.co.uk/about-us/careers/jobs/"/>
+    <hyperlink ref="C120" r:id="rId360" display="https://www.multiverse.io/en-GB/careers#job-list"/>
+    <hyperlink ref="C118" r:id="rId361" display="https://jobs.lever.co/joinzoe"/>
+    <hyperlink ref="C117" r:id="rId362" display="https://www.vouchercodes.co.uk/careers" tooltip="https://www.vouchercodes.co.uk/careers"/>
+    <hyperlink ref="C116" r:id="rId363" display="https://careers.occstrategy.com/vacancies/vacancy-search-results.aspx"/>
+    <hyperlink ref="C115" r:id="rId364" display="https://www.ibisworld.com/careers/" tooltip="https://www.ibisworld.com/careers/"/>
+    <hyperlink ref="C114" r:id="rId365" display="https://harri.com/grind-careers" tooltip="https://harri.com/grind-careers"/>
+    <hyperlink ref="C113" r:id="rId366" display="https://www.hush-uk.com/work-at-hush.html"/>
+    <hyperlink ref="C111" r:id="rId367" display="https://jobs.cityoflondon.gov.uk"/>
+    <hyperlink ref="C110" r:id="rId368" display="https://www.alphagroup.com/about/careers/" tooltip="https://www.alphagroup.com/about/careers/"/>
+    <hyperlink ref="C109" r:id="rId369" display="https://wearemtm.com/careers/" tooltip="https://wearemtm.com/careers/"/>
+    <hyperlink ref="C108" r:id="rId370" display="https://www.aireymiller.com/careers"/>
+    <hyperlink ref="C103" r:id="rId371" display="https://careers.cargill.com/en/search-jobs"/>
+    <hyperlink ref="C102" r:id="rId372" display="https://harri.com/Biscuiteers-careers"/>
+    <hyperlink ref="C101" r:id="rId373" display="https://cityfibre.com/careers/all-jobs"/>
+    <hyperlink ref="C100" r:id="rId374" display="https://corporate.lastminute.com/careers/jobs/?utm_source=lastminute&amp;_gl=1*ozugby*_ga*MTE0MTE2MTkxNS4xNzEwNzIwNzE4*_ga_66BMGPKMTR*MTcxMDcyMDcxNy4xLjAuMTcxMDcyMDgzMS4wLjAuMA..*_fplc*aWYlMkZSMVRhSVQlMkJFSktZQWNRQjhiSXhnelJmVUlHVFF0VUg3dWlQZWtMYXAxQUJWQ0xROCUyRk9UYlJGcXVSNWl3OWRjVnJLOU5DS2UxazE1ZEhKRzlPOE9lbjlmZ2VobWhkd1VCJTJGaWhIVnpnVnFNQ0J3ZzF3d0FsSXNLa2ozJTJGZyUzRCUzRA..&amp;_ga=2.250966918.1438506767.1710720718-1141161915.1710720718&amp;_gac=1.53775706.1710720718.CjwKCAiA0PuuBhBsEiwAS7fsNUBcK-u-irmaNJ8YfoBMQjHXX35iigABH04TXkR1Iz0HyWwv4kLPjxoC3M0QAvD_BwE"/>
+    <hyperlink ref="C99" r:id="rId375" display="https://careers.scs.co.uk/all-openings"/>
+    <hyperlink ref="C98" r:id="rId376" display="https://jobs.lever.co/treecard" tooltip="https://jobs.lever.co/treecard"/>
+    <hyperlink ref="C96" r:id="rId377" display="https://lwtheatres.csod.com/ux/ats/careersite/5/home?c=lwtheatres"/>
+    <hyperlink ref="C93" r:id="rId378" display="https://jobs.workable.com/company/vbFZaR6cPm46s3pMMdSotv/jobs-at-the-very-group"/>
+    <hyperlink ref="C91" r:id="rId379" display="https://boards.greenhouse.io/prefect"/>
+    <hyperlink ref="C89" r:id="rId380" display="https://www.vitechinc.com/careers/view-opportunities/"/>
+    <hyperlink ref="C88" r:id="rId381" display="https://canarywharf.wd3.myworkdayjobs.com/CanaryWharf" tooltip="https://canarywharf.wd3.myworkdayjobs.com/CanaryWharf"/>
+    <hyperlink ref="C87" r:id="rId382" display="https://www.rethinkfirst.com/careers/" tooltip="https://www.rethinkfirst.com/careers/"/>
+    <hyperlink ref="C85" r:id="rId383" display="https://ghd.livevacancies.co.uk/#/"/>
+    <hyperlink ref="C84" r:id="rId384" display="https://www.apprentify.com/internal-vacancies/" tooltip="https://www.apprentify.com/internal-vacancies/"/>
+    <hyperlink ref="C83" r:id="rId385" display="https://fortnum-and-mason.staging.krakatoa.eu-2.volcanic.cloud/jobs?source=careers.fortnumandmason.com"/>
+    <hyperlink ref="C81" r:id="rId386" display="https://powerleaguegroup.postingpanda.uk/" tooltip="https://powerleaguegroup.postingpanda.uk/"/>
+    <hyperlink ref="C80" r:id="rId387" display="https://netacea.com/careers/" tooltip="https://netacea.com/careers/"/>
+    <hyperlink ref="C78" r:id="rId388" display="https://www.veeve.com/en-gb/careers"/>
+    <hyperlink ref="C77" r:id="rId389" display="https://learnamp.com/careers#open-positions" tooltip="https://learnamp.com/careers#open-positions"/>
+    <hyperlink ref="C75" r:id="rId390" display="https://getmagic.com/careers/" tooltip="https://getmagic.com/careers/"/>
+    <hyperlink ref="C74" r:id="rId391" display="https://careers.hansonwadegroup.com/jobs"/>
+    <hyperlink ref="C72" r:id="rId392" display="https://apply.workable.com/volt-dot-i-o/#jobs"/>
+    <hyperlink ref="C71" r:id="rId393" display="https://jobs.bentley.com/search" tooltip="https://jobs.bentley.com/search"/>
+    <hyperlink ref="C70" r:id="rId394" display="https://unlockedgrads.org.uk/about/vacancies/#current-vacancies" tooltip="https://unlockedgrads.org.uk/about/vacancies/#current-vacancies"/>
+    <hyperlink ref="C69" r:id="rId395" display="https://www.rcseng.ac.uk/about-the-rcs/working-at-the-college/current-rcs-vacancies/" tooltip="https://www.rcseng.ac.uk/about-the-rcs/working-at-the-college/current-rcs-vacancies/"/>
+    <hyperlink ref="C68" r:id="rId396" display="https://www.togetherforgirls.org/en/careers" tooltip="https://www.togetherforgirls.org/en/careers"/>
+    <hyperlink ref="C67" r:id="rId397" display="https://www.adverity.com/careers" tooltip="https://www.adverity.com/careers"/>
+    <hyperlink ref="C66" r:id="rId398" display="https://careers.beamery.com/jobs/"/>
+    <hyperlink ref="C65" r:id="rId399" display="https://www.beacon.com/vacancies" tooltip="https://www.beacon.com/vacancies"/>
+    <hyperlink ref="C64" r:id="rId400" display="https://bcis.co.uk/about-us/careers/"/>
+    <hyperlink ref="C63" r:id="rId401" display="https://baxendale.co.uk/careers/" tooltip="https://baxendale.co.uk/careers/"/>
+    <hyperlink ref="C61" r:id="rId402" display="https://career.barnebys.com/jobs"/>
+    <hyperlink ref="C60" r:id="rId403" display="https://apply.workable.com/ballingerco/#jobs"/>
+    <hyperlink ref="C59" r:id="rId404" display="https://transitwireless.taleo.net/careersection/ex/jobsearch.ftl?lang=en" tooltip="https://transitwireless.taleo.net/careersection/ex/jobsearch.ftl?lang=en"/>
+    <hyperlink ref="C57" r:id="rId405" display="https://isw.changeworknow.co.uk/awayresorts/vms/e/careers/search/edit"/>
+    <hyperlink ref="C56" r:id="rId406" display="https://ejjl.fa.ap1.oraclecloud.com/hcmUI/CandidateExperience/en/sites/CX_1/requisitions?lastSelectedFacet=LOCATIONS&amp;mode=location&amp;selectedLocationsFacet=300000000296420%3B300000000294958"/>
+    <hyperlink ref="C55" r:id="rId407" display="https://atelierfinance.co.uk/careers/" tooltip="https://atelierfinance.co.uk/careers/"/>
+    <hyperlink ref="C53" r:id="rId408" display="https://us232.dayforcehcm.com/CandidatePortal/en-US/comptia" tooltip="https://us232.dayforcehcm.com/CandidatePortal/en-US/comptia"/>
+    <hyperlink ref="C52" r:id="rId409" display="https://artek.uk/careers" tooltip="https://artek.uk/careers"/>
+    <hyperlink ref="C49" r:id="rId410" display="https://careers.arbor-education.com/#jobs"/>
+    <hyperlink ref="C48" r:id="rId411" display="https://www.appearhere.co.uk/about/careers"/>
+    <hyperlink ref="C38" r:id="rId412" display="https://www.allwyn.co.uk/job-board"/>
+    <hyperlink ref="C37" r:id="rId413" display="https://alchemmy.com/careers/#positions"/>
+    <hyperlink ref="C36" r:id="rId414" display="https://www.airwallex.com/careers#roles" tooltip="https://www.airwallex.com/careers#roles"/>
+    <hyperlink ref="C34" r:id="rId415" display="https://careers.isio.com/en-GB/jobs"/>
+    <hyperlink ref="C33" r:id="rId416" display="https://careers.iqstudentaccommodation.com/jobs/vacancy/find/results/" tooltip="https://careers.iqstudentaccommodation.com/jobs/vacancy/find/results/"/>
+    <hyperlink ref="C31" r:id="rId417" display="https://frasers.group/careers/jobs"/>
+    <hyperlink ref="C30" r:id="rId418" display="https://www.prime-propertygroup.com/contacts/"/>
+    <hyperlink ref="C29" r:id="rId419" display="https://careers.next15.com/jobs" tooltip="https://careers.next15.com/jobs"/>
+    <hyperlink ref="C28" r:id="rId420" display="https://work.life/careers/"/>
+    <hyperlink ref="C27" r:id="rId421" display="https://www.hungerrush.com/careers/?an_fb_exaud=an_fb_hungerrushe46sdg56&amp;an_exaud0=an_fb_hungerrush6rsf5dhrd698" tooltip="https://www.hungerrush.com/careers/?an_fb_exaud=an_fb_hungerrushe46sdg56&amp;an_exaud0=an_fb_hungerrush6rsf5dhrd698"/>
+    <hyperlink ref="C25" r:id="rId422" display="https://myndyou.com/about-us/careers/" tooltip="https://myndyou.com/about-us/careers/"/>
+    <hyperlink ref="C24" r:id="rId423" display="https://careers.allianz.com/UK/search/?searchby=location&amp;createNewAlert=false&amp;q=&amp;locationsearch=GB%2C%20US&amp;optionsFacetsDD_department=&amp;optionsFacetsDD_shifttype=&amp;optionsFacetsDD_customfield3=&amp;optionsFacetsDD_customfield2=&amp;optionsFacetsDD_facility=&amp;optionsFacetsDD_customfield4=&amp;optionsFacetsDD_dept=&amp;inputSearchValue=GB%2C%20US&amp;quatFlag=false" tooltip="https://careers.allianz.com/UK/search/?searchby=location&amp;createNewAlert=false&amp;q=&amp;locationsearch=GB%2C%20US&amp;optionsFacetsDD_department=&amp;optionsFacetsDD_shifttype=&amp;optionsFacetsDD_customfield3=&amp;optionsFacetsDD_customfield2=&amp;optionsFacetsDD_facility=&amp;options"/>
+    <hyperlink ref="C23" r:id="rId424" display="https://careers.adyen.com/vacancies" tooltip="https://careers.adyen.com/vacancies"/>
+    <hyperlink ref="C22" r:id="rId425" display="https://www.admiraljobs.co.uk/Jobs?options=26&amp;page=1"/>
+    <hyperlink ref="C21" r:id="rId426" display="https://addland.com/careers"/>
+    <hyperlink ref="C20" r:id="rId427" display="https://acumen.org/work-with-us/" tooltip="https://acumen.org/work-with-us/"/>
+    <hyperlink ref="C19" r:id="rId428" display="https://careers.achievetogether.co.uk/Search.aspx" tooltip="https://careers.achievetogether.co.uk/Search.aspx"/>
+    <hyperlink ref="C18" r:id="rId429" display="https://careers.acco.com/go/All-ACCO-Brands-Job-Search-Results/9104500/"/>
+    <hyperlink ref="C17" r:id="rId430" display="https://abel-cole.breezy.hr/" tooltip="https://abel-cole.breezy.hr/"/>
+    <hyperlink ref="C16" r:id="rId431" display="https://www.aswatsoncareers.com/search" tooltip="https://www.aswatsoncareers.com/search"/>
+    <hyperlink ref="C15" r:id="rId432" display="https://4cassociates.teamtailor.com/jobs" tooltip="https://4cassociates.teamtailor.com/jobs"/>
+    <hyperlink ref="C14" r:id="rId433" display="https://4global.com/company/#" tooltip="https://4global.com/company/#"/>
+    <hyperlink ref="C13" r:id="rId434" display="https://3s.money/join/careers" tooltip="https://3s.money/join/careers"/>
+    <hyperlink ref="C12" r:id="rId435" display="https://www.kfh.co.uk/careers/vacancies/"/>
+    <hyperlink ref="C11" r:id="rId436" display="https://lendlease.wd3.myworkdayjobs.com/LendleaseCareers"/>
+    <hyperlink ref="C10" r:id="rId437" display="https://landsecurities.wd3.myworkdayjobs.com/Landseccareers" tooltip="https://landsecurities.wd3.myworkdayjobs.com/Landseccareers"/>
+    <hyperlink ref="C9" r:id="rId438" display="https://globalus232.dayforcehcm.com/CandidatePortal/en-US/caventures/SITE/caventurescareers"/>
+    <hyperlink ref="C8" r:id="rId439" display="https://careerssearch.saga.co.uk/"/>
+    <hyperlink ref="C7" r:id="rId440" display="https://jobs.lever.co/cfgi" tooltip="https://jobs.lever.co/cfgi"/>
+    <hyperlink ref="C6" r:id="rId441" display="https://www.biogen.com/careers/careers-search.html?country=United%2520Kingdom%2CUnited%2520States"/>
+    <hyperlink ref="C5" r:id="rId442" display="https://www.ardenthire.com/careers/our-careers/#"/>
+    <hyperlink ref="C4" r:id="rId443" display="https://mycareer.hsbc.com/en_GB/external/SearchJobs/?1017=%5B67222%2C67234%5D&amp;1017_format=812&amp;1023=%5B1248547%5D&amp;1023_format=913&amp;listFilterMode=1&amp;pipelineRecordsPerPage=10&amp;#anchor__search-jobs"/>
+    <hyperlink ref="C2" r:id="rId444" display="https://careers.techwolf.ai/" tooltip="https://careers.techwolf.ai/"/>
+    <hyperlink ref="C543" r:id="rId445" display="https://www.vitabiotics.com/pages/careers" tooltip="https://www.vitabiotics.com/pages/careers"/>
+    <hyperlink ref="C544" r:id="rId446" display="https://acaioutdoorwear.com/pages/careers?srsltid=AfmBOoqnOobmUDr6S8GiBsDp-PDhvxfbWJgkukM8PWSnqPoEmQJihHcF" tooltip="https://acaioutdoorwear.com/pages/careers?srsltid=AfmBOoqnOobmUDr6S8GiBsDp-PDhvxfbWJgkukM8PWSnqPoEmQJihHcF"/>
+    <hyperlink ref="C545" r:id="rId447" display="https://acorn-i.com/join-our-team/" tooltip="https://acorn-i.com/join-our-team/"/>
+    <hyperlink ref="C546" r:id="rId448" display="https://bdrthermea.wd103.myworkdayjobs.com/External?locationCountry=29247e57dbaf46fb855b224e03170bc7" tooltip="https://bdrthermea.wd103.myworkdayjobs.com/External?locationCountry=29247e57dbaf46fb855b224e03170bc7"/>
+    <hyperlink ref="C547" r:id="rId449" display="https://bitrise.io/careers" tooltip="https://bitrise.io/careers"/>
+    <hyperlink ref="C548" r:id="rId450" display="https://boards.greenhouse.io/blacklane" tooltip="https://boards.greenhouse.io/blacklane"/>
+    <hyperlink ref="C549" r:id="rId451" display="https://careers.bgf.co.uk/#jobs" tooltip="https://careers.bgf.co.uk/#jobs"/>
+    <hyperlink ref="C550" r:id="rId452" display="https://careers.carefertility.com/CareFertility/Home" tooltip="https://careers.carefertility.com/CareFertility/Home"/>
+    <hyperlink ref="C551" r:id="rId453" display="https://chambers.com/careers" tooltip="https://chambers.com/careers"/>
+    <hyperlink ref="C552" r:id="rId454" display="https://ciandt.com/us/en-us/careers/open-positions" tooltip="https://ciandt.com/us/en-us/careers/open-positions"/>
+    <hyperlink ref="C553" r:id="rId455" display="https://countingup.com/careers/" tooltip="https://countingup.com/careers/"/>
+    <hyperlink ref="C554" r:id="rId456" display="https://fsr.cvmailuk.com/bevanbrittan/main.cfm?srxksl=1" tooltip="https://fsr.cvmailuk.com/bevanbrittan/main.cfm?srxksl=1"/>
+    <hyperlink ref="C555" r:id="rId457" display="https://jobs.ajg.com/ajg-uk/jobs" tooltip="https://jobs.ajg.com/ajg-uk/jobs"/>
+    <hyperlink ref="C556" r:id="rId458" display="https://klowt.com/join-klowt/#vacancies" tooltip="https://klowt.com/join-klowt/#vacancies"/>
+    <hyperlink ref="C557" r:id="rId459" display="https://www.alpha.pet/en/career/jobs-and-application" tooltip="https://www.alpha.pet/en/career/jobs-and-application"/>
+    <hyperlink ref="C558" r:id="rId460" display="https://www.blueprintpartners.com/job-opportunities" tooltip="https://www.blueprintpartners.com/job-opportunities"/>
+    <hyperlink ref="C559" r:id="rId461" display="https://www.capitaleconomics.com/careers" tooltip="https://www.capitaleconomics.com/careers"/>
+    <hyperlink ref="C560" r:id="rId462" display="https://www.carnallfarrar.com/work-with-us/" tooltip="https://www.carnallfarrar.com/work-with-us/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="C419 C344:C346" listDataValidation="1"/>
+    <ignoredError sqref="C344:C346 C419" listDataValidation="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -14523,10 +14849,10 @@
         <v>231</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1086</v>
+        <v>1118</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1087</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="2" ht="22" customHeight="1" spans="1:3">
@@ -14545,10 +14871,10 @@
         <v>389</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>1088</v>
+        <v>1120</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>1089</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -14567,10 +14893,10 @@
         <v>474</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>1090</v>
+        <v>1122</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>1091</v>
+        <v>1123</v>
       </c>
       <c r="D5" s="11"/>
     </row>
@@ -14579,10 +14905,10 @@
         <v>484</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>1092</v>
+        <v>1124</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>1093</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -14604,10 +14930,10 @@
         <v>562</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>1094</v>
+        <v>1126</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>1095</v>
+        <v>1127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>